<commit_message>
redes sociales y texto typewrite integrado con blogger
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
+++ b/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Bitacioras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\pruebas\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB6DDBC-B6F7-4553-A3D0-1B2F2BFF034D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E63EC1D-D96B-4499-AFC5-60B2106B734B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>BITÁCORA DE SEGUIMIENTO ETAPA PRODUCTIVA</t>
   </si>
@@ -318,6 +318,14 @@
     <t>supongo que fue el texto animado, me tomo demaciado, desde la idea que tenia, implementarlo en una sola palabra, acomodarlo en el blog y luego intentar hacerlo con un numero ilimitado de mensajes
 pero me gusto como quedo el codigo, bien comentado y fasil de entender
 pero si esto es lo que mas me costo hoy</t>
+  </si>
+  <si>
+    <t>Los íconos de las redes sociales no son imágenes; están en formato SVG directamente insertados en el código. De esta forma, aparecen instantáneamente al cargar la página y ayudan a la optimización al no ser imágenes.
+Me costó demasiado encontrar estos íconos, además de modificar su padding para que todos quedaran iguales, pero estoy bastante contento con el resultado.</t>
+  </si>
+  <si>
+    <t>Di compatibilidad para agregar inserciones de YouTube y TikTok, pero este último consume demasiados recursos en los celulares. En una PC funciona muy bien, pero tendré que anotar que, preferiblemente, no inserten videos de TikTok.
+Agregué redes sociales, además de que estas pueden modificarse desde la interfaz de Blogger. Siguiendo esa misma lógica, apliqué lo mismo a los textos animados: se pueden agregar cuantos se quieran, además de tener un orden totalmente reorganizable.</t>
   </si>
 </sst>
 </file>
@@ -758,36 +766,226 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -797,200 +995,88 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1004,84 +1090,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1799,6 +1807,206 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2238416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>67493</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>806823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagen 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F42B8B9-3C41-469F-9A6B-6F578D2B2622}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6006353" y="29479916"/>
+          <a:ext cx="1871640" cy="2322378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>172411</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>26735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>97544</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2252382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagen 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04522C0F-CD90-4BBF-80A6-A6F0D8168FC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5965852" y="27268235"/>
+          <a:ext cx="1942192" cy="2225647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>75883</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>818029</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>416100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1535745</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagen 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7694DEEA-3030-49D5-A779-3D621464A602}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6250324" y="31813500"/>
+          <a:ext cx="1494423" cy="717716"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>212911</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1532281</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>3305734</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagen 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D62A40B7-0AB3-441D-978E-2A6873B70DA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6006352" y="32527752"/>
+          <a:ext cx="2039471" cy="1773453"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2211,8 +2419,8 @@
   </sheetPr>
   <dimension ref="B1:AA53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32:Y33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
@@ -2237,294 +2445,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B1" s="71"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="69" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
     </row>
     <row r="2" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="34" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
     </row>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="77"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
     </row>
     <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
     </row>
     <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="54"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="67"/>
     </row>
     <row r="6" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="54"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66"/>
+      <c r="T6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="66"/>
+      <c r="X6" s="66"/>
+      <c r="Y6" s="67"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1">
-      <c r="B8" s="18"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="78"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="78"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="68"/>
+      <c r="W8" s="68"/>
+      <c r="X8" s="68"/>
+      <c r="Y8" s="68"/>
     </row>
     <row r="9" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="30" t="s">
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="33" t="s">
+      <c r="Q9" s="94"/>
+      <c r="R9" s="94"/>
+      <c r="S9" s="95"/>
+      <c r="T9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="33"/>
-      <c r="V9" s="33"/>
-      <c r="W9" s="33"/>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="33" t="s">
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="30">
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="73">
         <v>5</v>
       </c>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="57" t="s">
+      <c r="Q10" s="94"/>
+      <c r="R10" s="94"/>
+      <c r="S10" s="95"/>
+      <c r="T10" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B11" s="3"/>
@@ -2553,68 +2761,68 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="58" t="s">
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58" t="s">
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="82"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="82"/>
+      <c r="W12" s="82"/>
+      <c r="X12" s="82"/>
+      <c r="Y12" s="82"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1">
-      <c r="B13" s="63">
+      <c r="B13" s="84">
         <v>3177294629</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="41">
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="49">
         <v>3177294629</v>
       </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="59" t="s">
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="81"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="81"/>
+      <c r="Y13" s="81"/>
     </row>
     <row r="14" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B14" s="3"/>
@@ -2643,100 +2851,100 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1">
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="79"/>
-      <c r="X15" s="79"/>
-      <c r="Y15" s="79"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="69"/>
+      <c r="W15" s="69"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1">
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="84" t="s">
+      <c r="I16" s="25"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="85"/>
-      <c r="M16" s="86"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="55" t="s">
+      <c r="L16" s="29"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="55" t="s">
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="55"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="55" t="s">
+      <c r="T16" s="25"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
-      <c r="Y16" s="56"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="27"/>
     </row>
     <row r="17" spans="2:27" ht="45.75" customHeight="1">
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="89"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="55"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="55"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="55"/>
-      <c r="Y17" s="56"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="27"/>
     </row>
     <row r="18" spans="2:27" ht="9.9499999999999993" customHeight="1">
       <c r="B18" s="3"/>
@@ -2765,72 +2973,72 @@
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="2:27" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="21" t="s">
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="21" t="s">
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="25" t="s">
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="27"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="91"/>
     </row>
     <row r="20" spans="2:27" ht="18" customHeight="1">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="92">
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="46">
         <v>1096800316</v>
       </c>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="23">
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="89">
         <v>3219713759</v>
       </c>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="28" t="s">
+      <c r="P20" s="90"/>
+      <c r="Q20" s="90"/>
+      <c r="R20" s="90"/>
+      <c r="S20" s="90"/>
+      <c r="T20" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="27"/>
+      <c r="U20" s="93"/>
+      <c r="V20" s="93"/>
+      <c r="W20" s="93"/>
+      <c r="X20" s="93"/>
+      <c r="Y20" s="91"/>
     </row>
     <row r="21" spans="2:27" ht="9.75" customHeight="1">
       <c r="B21" s="8"/>
@@ -2859,64 +3067,64 @@
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:27" ht="18" customHeight="1">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="33" t="s">
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="82"/>
-      <c r="R22" s="82"/>
-      <c r="S22" s="82"/>
-      <c r="T22" s="82"/>
-      <c r="U22" s="82"/>
-      <c r="V22" s="82"/>
-      <c r="W22" s="82"/>
-      <c r="X22" s="82"/>
-      <c r="Y22" s="82"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
     </row>
     <row r="23" spans="2:27" ht="18" customHeight="1">
-      <c r="B23" s="60">
+      <c r="B23" s="70">
         <v>2557356</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="47" t="s">
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
-      <c r="Y23" s="49"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="79"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="79"/>
+      <c r="S23" s="79"/>
+      <c r="T23" s="79"/>
+      <c r="U23" s="79"/>
+      <c r="V23" s="79"/>
+      <c r="W23" s="79"/>
+      <c r="X23" s="79"/>
+      <c r="Y23" s="80"/>
     </row>
     <row r="24" spans="2:27" ht="9.75" customHeight="1">
       <c r="B24" s="3"/>
@@ -2945,518 +3153,526 @@
       <c r="Y24" s="3"/>
     </row>
     <row r="25" spans="2:27" ht="48" customHeight="1">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="30" t="s">
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="50"/>
-      <c r="M25" s="30" t="s">
+      <c r="L25" s="74"/>
+      <c r="M25" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="50"/>
-      <c r="O25" s="30" t="s">
+      <c r="N25" s="74"/>
+      <c r="O25" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="30" t="s">
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="74"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="51"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="75"/>
     </row>
     <row r="26" spans="2:27" ht="216" customHeight="1">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="43">
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="54">
         <v>45705</v>
       </c>
-      <c r="L26" s="44"/>
-      <c r="M26" s="43">
+      <c r="L26" s="55"/>
+      <c r="M26" s="54">
         <v>45706</v>
       </c>
-      <c r="N26" s="44"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="61"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="42" t="s">
+      <c r="N26" s="55"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="71"/>
+      <c r="Q26" s="71"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="71"/>
+      <c r="T26" s="72"/>
+      <c r="U26" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="V26" s="42"/>
-      <c r="W26" s="42"/>
-      <c r="X26" s="42"/>
-      <c r="Y26" s="42"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
     </row>
     <row r="27" spans="2:27" ht="232.5" customHeight="1">
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="42"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="42"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="57"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="71"/>
+      <c r="Q27" s="71"/>
+      <c r="R27" s="71"/>
+      <c r="S27" s="71"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="50"/>
     </row>
     <row r="28" spans="2:27" ht="126.75" customHeight="1">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="43">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="54">
         <v>45706</v>
       </c>
-      <c r="L28" s="44"/>
-      <c r="M28" s="43">
+      <c r="L28" s="55"/>
+      <c r="M28" s="54">
         <v>45707</v>
       </c>
-      <c r="N28" s="44"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="42" t="s">
+      <c r="N28" s="55"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="V28" s="42"/>
-      <c r="W28" s="42"/>
-      <c r="X28" s="42"/>
-      <c r="Y28" s="42"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
     </row>
     <row r="29" spans="2:27" ht="189" customHeight="1">
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="42"/>
-      <c r="W29" s="42"/>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="42"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
       <c r="AA29" s="16"/>
     </row>
     <row r="30" spans="2:27" ht="105" customHeight="1">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="43">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="54">
         <v>45707</v>
       </c>
-      <c r="L30" s="44"/>
-      <c r="M30" s="43">
+      <c r="L30" s="55"/>
+      <c r="M30" s="54">
         <v>45708</v>
       </c>
-      <c r="N30" s="44"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="42" t="s">
+      <c r="N30" s="55"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="V30" s="42"/>
-      <c r="W30" s="42"/>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="42"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
     </row>
     <row r="31" spans="2:27" ht="180.75" customHeight="1">
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="42"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="42"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="50"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="50"/>
       <c r="AA31" s="16"/>
     </row>
     <row r="32" spans="2:27" ht="280.5" customHeight="1">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="43">
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="54">
         <v>45708</v>
       </c>
-      <c r="L32" s="44"/>
-      <c r="M32" s="43">
+      <c r="L32" s="55"/>
+      <c r="M32" s="54">
         <v>45709</v>
       </c>
-      <c r="N32" s="44"/>
-      <c r="O32" s="41"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="42" t="s">
+      <c r="N32" s="55"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="V32" s="42"/>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
+      <c r="V32" s="50"/>
+      <c r="W32" s="50"/>
+      <c r="X32" s="50"/>
+      <c r="Y32" s="50"/>
     </row>
     <row r="33" spans="2:25" ht="259.5" customHeight="1">
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="41"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="42"/>
-      <c r="V33" s="42"/>
-      <c r="W33" s="42"/>
-      <c r="X33" s="42"/>
-      <c r="Y33" s="42"/>
-    </row>
-    <row r="34" spans="2:25" ht="15" customHeight="1">
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="41"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="41"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="42"/>
-      <c r="V34" s="42"/>
-      <c r="W34" s="42"/>
-      <c r="X34" s="42"/>
-      <c r="Y34" s="42"/>
-    </row>
-    <row r="35" spans="2:25" ht="15" customHeight="1">
-      <c r="B35" s="38"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="41"/>
-      <c r="P35" s="41"/>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="41"/>
-      <c r="S35" s="41"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="42"/>
-      <c r="V35" s="42"/>
-      <c r="W35" s="42"/>
-      <c r="X35" s="42"/>
-      <c r="Y35" s="42"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="57"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="50"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="50"/>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="50"/>
+    </row>
+    <row r="34" spans="2:25" ht="295.5" customHeight="1">
+      <c r="B34" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="54">
+        <v>45709</v>
+      </c>
+      <c r="L34" s="55"/>
+      <c r="M34" s="54">
+        <v>45710</v>
+      </c>
+      <c r="N34" s="55"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="V34" s="50"/>
+      <c r="W34" s="50"/>
+      <c r="X34" s="50"/>
+      <c r="Y34" s="50"/>
+    </row>
+    <row r="35" spans="2:25" ht="265.5" customHeight="1">
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="50"/>
+      <c r="V35" s="50"/>
+      <c r="W35" s="50"/>
+      <c r="X35" s="50"/>
+      <c r="Y35" s="50"/>
     </row>
     <row r="36" spans="2:25" ht="15" customHeight="1">
-      <c r="B36" s="35"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="41"/>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="42"/>
-      <c r="V36" s="42"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="42"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="50"/>
     </row>
     <row r="37" spans="2:25" ht="15" customHeight="1">
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="41"/>
-      <c r="S37" s="41"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="42"/>
-      <c r="V37" s="42"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="42"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="50"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="50"/>
+      <c r="X37" s="50"/>
+      <c r="Y37" s="50"/>
     </row>
     <row r="38" spans="2:25" ht="15" customHeight="1">
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="44"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="42"/>
-      <c r="V38" s="42"/>
-      <c r="W38" s="42"/>
-      <c r="X38" s="42"/>
-      <c r="Y38" s="42"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="49"/>
+      <c r="U38" s="50"/>
+      <c r="V38" s="50"/>
+      <c r="W38" s="50"/>
+      <c r="X38" s="50"/>
+      <c r="Y38" s="50"/>
     </row>
     <row r="39" spans="2:25" ht="15" customHeight="1">
-      <c r="B39" s="38"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="41"/>
-      <c r="P39" s="41"/>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="41"/>
-      <c r="S39" s="41"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="42"/>
-      <c r="V39" s="42"/>
-      <c r="W39" s="42"/>
-      <c r="X39" s="42"/>
-      <c r="Y39" s="42"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="49"/>
+      <c r="U39" s="50"/>
+      <c r="V39" s="50"/>
+      <c r="W39" s="50"/>
+      <c r="X39" s="50"/>
+      <c r="Y39" s="50"/>
     </row>
     <row r="40" spans="2:25" ht="15" customHeight="1">
-      <c r="B40" s="35"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="41"/>
-      <c r="S40" s="41"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="42"/>
-      <c r="X40" s="42"/>
-      <c r="Y40" s="42"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="54"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="55"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="50"/>
+      <c r="V40" s="50"/>
+      <c r="W40" s="50"/>
+      <c r="X40" s="50"/>
+      <c r="Y40" s="50"/>
     </row>
     <row r="41" spans="2:25" ht="15" customHeight="1">
-      <c r="B41" s="38"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="46"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="41"/>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="41"/>
-      <c r="S41" s="41"/>
-      <c r="T41" s="41"/>
-      <c r="U41" s="42"/>
-      <c r="V41" s="42"/>
-      <c r="W41" s="42"/>
-      <c r="X41" s="42"/>
-      <c r="Y41" s="42"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="50"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="50"/>
+      <c r="Y41" s="50"/>
     </row>
     <row r="42" spans="2:25" ht="15" customHeight="1">
-      <c r="B42" s="95" t="s">
+      <c r="B42" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="95"/>
-      <c r="L42" s="95"/>
-      <c r="M42" s="95"/>
-      <c r="N42" s="95"/>
-      <c r="O42" s="95"/>
-      <c r="P42" s="95"/>
-      <c r="Q42" s="95"/>
-      <c r="R42" s="95"/>
-      <c r="S42" s="95"/>
-      <c r="T42" s="95"/>
-      <c r="U42" s="95"/>
-      <c r="V42" s="95"/>
-      <c r="W42" s="95"/>
-      <c r="X42" s="95"/>
-      <c r="Y42" s="95"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="51"/>
+      <c r="U42" s="51"/>
+      <c r="V42" s="51"/>
+      <c r="W42" s="51"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51"/>
     </row>
     <row r="43" spans="2:25" ht="15" customHeight="1">
       <c r="B43" s="10"/>
@@ -3485,16 +3701,16 @@
       <c r="Y43" s="10"/>
     </row>
     <row r="44" spans="2:25" ht="15" customHeight="1">
-      <c r="B44" s="68" t="s">
+      <c r="B44" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="68"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
@@ -3505,11 +3721,11 @@
       <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
-      <c r="T44" s="67"/>
-      <c r="U44" s="68"/>
-      <c r="V44" s="68"/>
-      <c r="W44" s="68"/>
-      <c r="X44" s="68"/>
+      <c r="T44" s="76"/>
+      <c r="U44" s="77"/>
+      <c r="V44" s="77"/>
+      <c r="W44" s="77"/>
+      <c r="X44" s="77"/>
       <c r="Y44" s="10"/>
     </row>
     <row r="45" spans="2:25" ht="15" customHeight="1">
@@ -3539,35 +3755,35 @@
       <c r="Y45" s="8"/>
     </row>
     <row r="46" spans="2:25">
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
       <c r="J46" s="11"/>
-      <c r="K46" s="18" t="s">
+      <c r="K46" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="40"/>
+      <c r="O46" s="40"/>
+      <c r="P46" s="40"/>
+      <c r="Q46" s="40"/>
       <c r="R46" s="13"/>
       <c r="S46" s="11"/>
-      <c r="T46" s="17" t="s">
+      <c r="T46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="U46" s="17"/>
-      <c r="V46" s="17"/>
-      <c r="W46" s="17"/>
-      <c r="X46" s="17"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
       <c r="Y46" s="11"/>
     </row>
     <row r="47" spans="2:25">
@@ -3597,16 +3813,16 @@
       <c r="Y47" s="11"/>
     </row>
     <row r="48" spans="2:25" ht="15" customHeight="1">
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
     </row>
     <row r="49" spans="2:25" ht="15" customHeight="1">
       <c r="B49" s="14"/>
@@ -3635,100 +3851,184 @@
       <c r="Y49" s="12"/>
     </row>
     <row r="50" spans="2:25" ht="15.75" customHeight="1">
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
       <c r="J50" s="11"/>
-      <c r="K50" s="18" t="s">
+      <c r="K50" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="40"/>
+      <c r="N50" s="40"/>
+      <c r="O50" s="40"/>
+      <c r="P50" s="40"/>
+      <c r="Q50" s="40"/>
       <c r="R50" s="13"/>
-      <c r="S50" s="19" t="s">
+      <c r="S50" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="T50" s="20"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+      <c r="V50" s="18"/>
+      <c r="W50" s="18"/>
+      <c r="X50" s="18"/>
+      <c r="Y50" s="18"/>
     </row>
     <row r="51" spans="2:25" ht="23.25" customHeight="1">
-      <c r="Q51" s="94"/>
-      <c r="R51" s="94"/>
-      <c r="S51" s="94"/>
-      <c r="T51" s="94"/>
-      <c r="U51" s="94"/>
+      <c r="Q51" s="48"/>
+      <c r="R51" s="48"/>
+      <c r="S51" s="48"/>
+      <c r="T51" s="48"/>
+      <c r="U51" s="48"/>
     </row>
     <row r="52" spans="2:25" ht="18" customHeight="1">
-      <c r="B52" s="73" t="s">
+      <c r="B52" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="20"/>
-      <c r="R52" s="20"/>
-      <c r="S52" s="20"/>
-      <c r="T52" s="20"/>
-      <c r="U52" s="20"/>
-      <c r="V52" s="20"/>
-      <c r="W52" s="20"/>
-      <c r="X52" s="20"/>
-      <c r="Y52" s="20"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="18"/>
+      <c r="U52" s="18"/>
+      <c r="V52" s="18"/>
+      <c r="W52" s="18"/>
+      <c r="X52" s="18"/>
+      <c r="Y52" s="18"/>
     </row>
     <row r="53" spans="2:25">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="20"/>
-      <c r="O53" s="20"/>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="20"/>
-      <c r="T53" s="20"/>
-      <c r="U53" s="20"/>
-      <c r="V53" s="20"/>
-      <c r="W53" s="20"/>
-      <c r="X53" s="20"/>
-      <c r="Y53" s="20"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+      <c r="V53" s="18"/>
+      <c r="W53" s="18"/>
+      <c r="X53" s="18"/>
+      <c r="Y53" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="S50:Y50"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="T20:Y20"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="B40:J41"/>
+    <mergeCell ref="O40:T41"/>
+    <mergeCell ref="U40:Y41"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="O34:T35"/>
+    <mergeCell ref="U34:Y35"/>
+    <mergeCell ref="B38:J39"/>
+    <mergeCell ref="M36:N37"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="M38:N39"/>
+    <mergeCell ref="U36:Y37"/>
+    <mergeCell ref="B36:J37"/>
+    <mergeCell ref="B34:J35"/>
+    <mergeCell ref="K23:Y23"/>
+    <mergeCell ref="U25:Y25"/>
+    <mergeCell ref="B26:J27"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="B30:J31"/>
+    <mergeCell ref="U26:Y27"/>
+    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="O25:T25"/>
+    <mergeCell ref="T44:X44"/>
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O26:T26"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="O36:T37"/>
+    <mergeCell ref="K30:L31"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="K34:L35"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="B8:Y8"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O28:T29"/>
+    <mergeCell ref="U28:Y29"/>
+    <mergeCell ref="O30:T31"/>
+    <mergeCell ref="U30:Y31"/>
+    <mergeCell ref="B23:J23"/>
     <mergeCell ref="B52:Y53"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B22:J22"/>
@@ -3753,90 +4053,6 @@
     <mergeCell ref="T46:X46"/>
     <mergeCell ref="U32:Y33"/>
     <mergeCell ref="B42:Y42"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="O36:T37"/>
-    <mergeCell ref="K30:L31"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="M26:N27"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="K34:L35"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O28:T29"/>
-    <mergeCell ref="U28:Y29"/>
-    <mergeCell ref="O30:T31"/>
-    <mergeCell ref="U30:Y31"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="B30:J31"/>
-    <mergeCell ref="U26:Y27"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="O25:T25"/>
-    <mergeCell ref="T44:X44"/>
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O26:T26"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="K23:Y23"/>
-    <mergeCell ref="U25:Y25"/>
-    <mergeCell ref="B26:J27"/>
-    <mergeCell ref="B6:Y6"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="K50:Q50"/>
-    <mergeCell ref="S50:Y50"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="T19:Y19"/>
-    <mergeCell ref="T20:Y20"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="B40:J41"/>
-    <mergeCell ref="O40:T41"/>
-    <mergeCell ref="U40:Y41"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="O34:T35"/>
-    <mergeCell ref="U34:Y35"/>
-    <mergeCell ref="B38:J39"/>
-    <mergeCell ref="M36:N37"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="M38:N39"/>
-    <mergeCell ref="U36:Y37"/>
-    <mergeCell ref="B36:J37"/>
-    <mergeCell ref="B34:J35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T20" r:id="rId1" xr:uid="{BE351EEA-9877-430E-96A9-ADC6513FEEA9}"/>
@@ -3864,124 +4080,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="118"/>
-      <c r="P1" s="118"/>
-      <c r="Q1" s="118"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="118"/>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="118"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="102" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="102"/>
-      <c r="W2" s="102"/>
-      <c r="X2" s="102"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1">
-      <c r="U3" s="125"/>
-      <c r="V3" s="125"/>
-      <c r="W3" s="125"/>
-      <c r="X3" s="125"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="105"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="122" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123"/>
-      <c r="Q4" s="123"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123"/>
-      <c r="V4" s="123"/>
-      <c r="W4" s="123"/>
-      <c r="X4" s="124"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="102"/>
+      <c r="X4" s="103"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="119"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="121"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="120"/>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="120"/>
-      <c r="S5" s="120"/>
-      <c r="T5" s="120"/>
-      <c r="U5" s="120"/>
-      <c r="V5" s="120"/>
-      <c r="W5" s="120"/>
-      <c r="X5" s="121"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="99"/>
+      <c r="U5" s="99"/>
+      <c r="V5" s="99"/>
+      <c r="W5" s="99"/>
+      <c r="X5" s="100"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A6" s="3"/>
@@ -4010,66 +4226,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100" t="s">
+      <c r="B7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100" t="s">
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="100"/>
-      <c r="W7" s="100"/>
-      <c r="X7" s="100"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="97"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="97"/>
+      <c r="V7" s="97"/>
+      <c r="W7" s="97"/>
+      <c r="X7" s="97"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1">
-      <c r="A8" s="93"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="107" t="s">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
-      <c r="O8" s="109"/>
-      <c r="P8" s="107" t="s">
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="108"/>
+      <c r="P8" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="108"/>
-      <c r="R8" s="108"/>
-      <c r="S8" s="108"/>
-      <c r="T8" s="108"/>
-      <c r="U8" s="108"/>
-      <c r="V8" s="108"/>
-      <c r="W8" s="108"/>
-      <c r="X8" s="109"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107"/>
+      <c r="U8" s="107"/>
+      <c r="V8" s="107"/>
+      <c r="W8" s="107"/>
+      <c r="X8" s="108"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A9" s="3"/>
@@ -4098,66 +4314,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="79"/>
-      <c r="U10" s="79"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="79"/>
-      <c r="X10" s="79"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="69"/>
+      <c r="W10" s="69"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57" t="s">
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57" t="s">
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
+      <c r="T11" s="81"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="81"/>
+      <c r="W11" s="81"/>
+      <c r="X11" s="81"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="3"/>
@@ -4186,66 +4402,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100" t="s">
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="100" t="s">
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="97"/>
+      <c r="P13" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="100"/>
-      <c r="S13" s="100"/>
-      <c r="T13" s="100"/>
-      <c r="U13" s="100"/>
-      <c r="V13" s="100"/>
-      <c r="W13" s="100"/>
-      <c r="X13" s="100"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
+      <c r="S13" s="97"/>
+      <c r="T13" s="97"/>
+      <c r="U13" s="97"/>
+      <c r="V13" s="97"/>
+      <c r="W13" s="97"/>
+      <c r="X13" s="97"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1">
-      <c r="A14" s="93"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="107" t="s">
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="108"/>
-      <c r="L14" s="108"/>
-      <c r="M14" s="108"/>
-      <c r="N14" s="108"/>
-      <c r="O14" s="109"/>
-      <c r="P14" s="107" t="s">
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="108"/>
-      <c r="R14" s="108"/>
-      <c r="S14" s="108"/>
-      <c r="T14" s="108"/>
-      <c r="U14" s="108"/>
-      <c r="V14" s="108"/>
-      <c r="W14" s="108"/>
-      <c r="X14" s="109"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
+      <c r="U14" s="107"/>
+      <c r="V14" s="107"/>
+      <c r="W14" s="107"/>
+      <c r="X14" s="108"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A15" s="3"/>
@@ -4274,184 +4490,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="110" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="110"/>
-      <c r="L16" s="110"/>
-      <c r="M16" s="110"/>
-      <c r="N16" s="17" t="s">
+      <c r="K16" s="114"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
+      <c r="N16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="111" t="s">
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="111"/>
-      <c r="V16" s="111"/>
-      <c r="W16" s="111"/>
-      <c r="X16" s="111"/>
+      <c r="U16" s="115"/>
+      <c r="V16" s="115"/>
+      <c r="W16" s="115"/>
+      <c r="X16" s="115"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="102"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="112" t="s">
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="114"/>
-      <c r="N17" s="101" t="s">
+      <c r="K17" s="117"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="102"/>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="103"/>
-      <c r="T17" s="101" t="s">
+      <c r="O17" s="104"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="110"/>
+      <c r="T17" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="102"/>
-      <c r="V17" s="102"/>
-      <c r="W17" s="102"/>
-      <c r="X17" s="103"/>
+      <c r="U17" s="104"/>
+      <c r="V17" s="104"/>
+      <c r="W17" s="104"/>
+      <c r="X17" s="110"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A18" s="104"/>
-      <c r="B18" s="105"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="115"/>
-      <c r="K18" s="116"/>
-      <c r="L18" s="116"/>
-      <c r="M18" s="117"/>
-      <c r="N18" s="104"/>
-      <c r="O18" s="105"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="106"/>
-      <c r="T18" s="104"/>
-      <c r="U18" s="105"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="105"/>
-      <c r="X18" s="106"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="113"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="111"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="113"/>
+      <c r="T18" s="111"/>
+      <c r="U18" s="112"/>
+      <c r="V18" s="112"/>
+      <c r="W18" s="112"/>
+      <c r="X18" s="113"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1"/>
     <row r="20" spans="1:24" ht="39" customHeight="1"/>
     <row r="21" spans="1:24">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
+      <c r="B21" s="125"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="125"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="99" t="s">
+      <c r="J21" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="99"/>
-      <c r="L21" s="99"/>
-      <c r="M21" s="99"/>
-      <c r="N21" s="99"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="99"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="125"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="99" t="s">
+      <c r="R21" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="99"/>
-      <c r="T21" s="99"/>
-      <c r="U21" s="99"/>
-      <c r="V21" s="99"/>
-      <c r="W21" s="99"/>
-      <c r="X21" s="99"/>
+      <c r="S21" s="125"/>
+      <c r="T21" s="125"/>
+      <c r="U21" s="125"/>
+      <c r="V21" s="125"/>
+      <c r="W21" s="125"/>
+      <c r="X21" s="125"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P23" s="96" t="s">
+      <c r="P23" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-      <c r="S23" s="96"/>
-      <c r="T23" s="96"/>
-      <c r="U23" s="97" t="s">
+      <c r="Q23" s="122"/>
+      <c r="R23" s="122"/>
+      <c r="S23" s="122"/>
+      <c r="T23" s="122"/>
+      <c r="U23" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="97"/>
-      <c r="W23" s="97"/>
-      <c r="X23" s="97"/>
+      <c r="V23" s="123"/>
+      <c r="W23" s="123"/>
+      <c r="X23" s="123"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P24" s="96" t="s">
+      <c r="P24" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="96"/>
-      <c r="S24" s="96"/>
-      <c r="T24" s="96"/>
-      <c r="U24" s="98" t="s">
+      <c r="Q24" s="122"/>
+      <c r="R24" s="122"/>
+      <c r="S24" s="122"/>
+      <c r="T24" s="122"/>
+      <c r="U24" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="98"/>
-      <c r="W24" s="98"/>
-      <c r="X24" s="98"/>
+      <c r="V24" s="124"/>
+      <c r="W24" s="124"/>
+      <c r="X24" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -4466,13 +4670,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
forma de cargar la pagina + redes sociales +
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
+++ b/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\pruebas\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E63EC1D-D96B-4499-AFC5-60B2106B734B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E08F763-F13A-4FBA-BB4A-7C431152AB39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>BITÁCORA DE SEGUIMIENTO ETAPA PRODUCTIVA</t>
   </si>
@@ -326,6 +326,15 @@
   <si>
     <t>Di compatibilidad para agregar inserciones de YouTube y TikTok, pero este último consume demasiados recursos en los celulares. En una PC funciona muy bien, pero tendré que anotar que, preferiblemente, no inserten videos de TikTok.
 Agregué redes sociales, además de que estas pueden modificarse desde la interfaz de Blogger. Siguiendo esa misma lógica, apliqué lo mismo a los textos animados: se pueden agregar cuantos se quieran, además de tener un orden totalmente reorganizable.</t>
+  </si>
+  <si>
+    <t>tuve cambiar la forma como se ocultaba el texto animado para hacer que se viera el puntero aun que la animacion no haya empezado, TODO lo que tuve que ver con acomodar los post según el tamaño llevo un arduo trabajo para intentar encontrar las forma menos exigente para el sistema de hacerlo</t>
+  </si>
+  <si>
+    <t>le agrege animaciones a las redes sociales cuando pasas el cursor por encima, tambien un efecto de ola que hacen para ser mas llamativas
+la animacion del texto superior no comienza hasta que el documento carga por completo, asi esta no seve lageada ya que al principio de tantas cosas las animacion se trababa
+volve a crear el sistema que determina si  un post debe ocupar toda la fila, si la pantallamide menos de 900px  no se ejecutara por ende los dispositivos moviles no tendran que prosesarlo, ahora  no solo eso si no que detecta si la pantalla de vuelve mas grande, y si llega ah un punto se ejecuta y la funcion se borra ya que no es nesesaria mas
+acomodo en otra parte el codigo del post ya que vi que se ejecutava una vez por cada post que se pintaba ( 15 veces)</t>
   </si>
 </sst>
 </file>
@@ -766,17 +775,192 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -784,20 +968,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -817,42 +992,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -862,151 +1007,78 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1025,71 +1097,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1617,8 +1626,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>2296579</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2296</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1999,6 +2008,256 @@
         <a:xfrm>
           <a:off x="6006352" y="32527752"/>
           <a:ext cx="2039471" cy="1773453"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1232831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>115367</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5FB48A1-213E-4480-8D73-DD34E85D1D2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6196853" y="35601272"/>
+          <a:ext cx="1367118" cy="2056725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>93970</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>86735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>10997</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1123551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Imagen 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE472C74-1D5C-4124-8CC9-EBA155B64FCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5887411" y="34455176"/>
+          <a:ext cx="1071233" cy="1036816"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>185993</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>600489</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>128655</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>2062392</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagen 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D4BBDA3-90B1-4E8D-AC83-DFF97F0AB883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5975536" y="38178685"/>
+          <a:ext cx="1093945" cy="1461903"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>46589</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>280540</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1199030</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagen 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A98D36-1FEE-4320-9144-C21398896930}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6994236" y="34469294"/>
+          <a:ext cx="1096804" cy="1098177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>265044</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>587120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>300325</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1924049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagen 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{399C8924-B0B3-4146-AA62-8B6E30D7D86F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7205870" y="38165316"/>
+          <a:ext cx="896672" cy="1336929"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2419,8 +2678,8 @@
   </sheetPr>
   <dimension ref="B1:AA53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:J35"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
@@ -2445,294 +2704,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B1" s="59"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="52" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
     </row>
     <row r="2" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="58" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
     </row>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="77"/>
     </row>
     <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
     </row>
     <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="67"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="53"/>
+      <c r="Y5" s="54"/>
     </row>
     <row r="6" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="66"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="67"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="54"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1">
-      <c r="B8" s="40"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="68"/>
-      <c r="V8" s="68"/>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="68"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="78"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="78"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="78"/>
     </row>
     <row r="9" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="73" t="s">
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="95"/>
-      <c r="T9" s="23" t="s">
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="23" t="s">
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="73">
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="30">
         <v>5</v>
       </c>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="95"/>
-      <c r="T10" s="81" t="s">
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B11" s="3"/>
@@ -2761,68 +3020,68 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="82" t="s">
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82" t="s">
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="82"/>
-      <c r="S12" s="82"/>
-      <c r="T12" s="82"/>
-      <c r="U12" s="82"/>
-      <c r="V12" s="82"/>
-      <c r="W12" s="82"/>
-      <c r="X12" s="82"/>
-      <c r="Y12" s="82"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1">
-      <c r="B13" s="84">
+      <c r="B13" s="63">
         <v>3177294629</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="49">
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="41">
         <v>3177294629</v>
       </c>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="83" t="s">
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="81"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
-      <c r="Y13" s="81"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
+      <c r="Y13" s="57"/>
     </row>
     <row r="14" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B14" s="3"/>
@@ -2851,100 +3110,100 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1">
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
-      <c r="T15" s="69"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="69"/>
-      <c r="W15" s="69"/>
-      <c r="X15" s="69"/>
-      <c r="Y15" s="69"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="79"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="79"/>
+      <c r="X15" s="79"/>
+      <c r="Y15" s="79"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="25" t="s">
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28" t="s">
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="25" t="s">
+      <c r="L16" s="85"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="25" t="s">
+      <c r="P16" s="83"/>
+      <c r="Q16" s="83"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="25"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="25" t="s">
+      <c r="T16" s="55"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="27"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="56"/>
     </row>
     <row r="17" spans="2:27" ht="45.75" customHeight="1">
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="27"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
+      <c r="Y17" s="56"/>
     </row>
     <row r="18" spans="2:27" ht="9.9499999999999993" customHeight="1">
       <c r="B18" s="3"/>
@@ -2973,72 +3232,72 @@
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="2:27" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="44" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="44" t="s">
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="20" t="s">
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="91"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="27"/>
     </row>
     <row r="20" spans="2:27" ht="18" customHeight="1">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="46">
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="92">
         <v>1096800316</v>
       </c>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="89">
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="93"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="23">
         <v>3219713759</v>
       </c>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="92" t="s">
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="U20" s="93"/>
-      <c r="V20" s="93"/>
-      <c r="W20" s="93"/>
-      <c r="X20" s="93"/>
-      <c r="Y20" s="91"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="27"/>
     </row>
     <row r="21" spans="2:27" ht="9.75" customHeight="1">
       <c r="B21" s="8"/>
@@ -3067,64 +3326,64 @@
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:27" ht="18" customHeight="1">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="23" t="s">
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="82"/>
+      <c r="W22" s="82"/>
+      <c r="X22" s="82"/>
+      <c r="Y22" s="82"/>
     </row>
     <row r="23" spans="2:27" ht="18" customHeight="1">
-      <c r="B23" s="70">
+      <c r="B23" s="60">
         <v>2557356</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="78" t="s">
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="S23" s="79"/>
-      <c r="T23" s="79"/>
-      <c r="U23" s="79"/>
-      <c r="V23" s="79"/>
-      <c r="W23" s="79"/>
-      <c r="X23" s="79"/>
-      <c r="Y23" s="80"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="49"/>
     </row>
     <row r="24" spans="2:27" ht="9.75" customHeight="1">
       <c r="B24" s="3"/>
@@ -3153,526 +3412,534 @@
       <c r="Y24" s="3"/>
     </row>
     <row r="25" spans="2:27" ht="48" customHeight="1">
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="73" t="s">
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="74"/>
-      <c r="M25" s="73" t="s">
+      <c r="L25" s="50"/>
+      <c r="M25" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="74"/>
-      <c r="O25" s="73" t="s">
+      <c r="N25" s="50"/>
+      <c r="O25" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="73" t="s">
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="74"/>
-      <c r="W25" s="74"/>
-      <c r="X25" s="74"/>
-      <c r="Y25" s="75"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="51"/>
     </row>
     <row r="26" spans="2:27" ht="216" customHeight="1">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="54">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="43">
         <v>45705</v>
       </c>
-      <c r="L26" s="55"/>
-      <c r="M26" s="54">
+      <c r="L26" s="44"/>
+      <c r="M26" s="43">
         <v>45706</v>
       </c>
-      <c r="N26" s="55"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="71"/>
-      <c r="Q26" s="71"/>
-      <c r="R26" s="71"/>
-      <c r="S26" s="71"/>
-      <c r="T26" s="72"/>
-      <c r="U26" s="50" t="s">
+      <c r="N26" s="44"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="61"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="61"/>
+      <c r="T26" s="62"/>
+      <c r="U26" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="50"/>
+      <c r="V26" s="42"/>
+      <c r="W26" s="42"/>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="42"/>
     </row>
     <row r="27" spans="2:27" ht="232.5" customHeight="1">
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="71"/>
-      <c r="S27" s="71"/>
-      <c r="T27" s="72"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="50"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="42"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="42"/>
     </row>
     <row r="28" spans="2:27" ht="126.75" customHeight="1">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="54">
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="43">
         <v>45706</v>
       </c>
-      <c r="L28" s="55"/>
-      <c r="M28" s="54">
+      <c r="L28" s="44"/>
+      <c r="M28" s="43">
         <v>45707</v>
       </c>
-      <c r="N28" s="55"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="49"/>
-      <c r="U28" s="50" t="s">
+      <c r="N28" s="44"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="V28" s="50"/>
-      <c r="W28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="50"/>
+      <c r="V28" s="42"/>
+      <c r="W28" s="42"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
     </row>
     <row r="29" spans="2:27" ht="189" customHeight="1">
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="49"/>
-      <c r="U29" s="50"/>
-      <c r="V29" s="50"/>
-      <c r="W29" s="50"/>
-      <c r="X29" s="50"/>
-      <c r="Y29" s="50"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="42"/>
+      <c r="V29" s="42"/>
+      <c r="W29" s="42"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="42"/>
       <c r="AA29" s="16"/>
     </row>
     <row r="30" spans="2:27" ht="105" customHeight="1">
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="54">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="43">
         <v>45707</v>
       </c>
-      <c r="L30" s="55"/>
-      <c r="M30" s="54">
+      <c r="L30" s="44"/>
+      <c r="M30" s="43">
         <v>45708</v>
       </c>
-      <c r="N30" s="55"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="50" t="s">
+      <c r="N30" s="44"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="V30" s="50"/>
-      <c r="W30" s="50"/>
-      <c r="X30" s="50"/>
-      <c r="Y30" s="50"/>
+      <c r="V30" s="42"/>
+      <c r="W30" s="42"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="42"/>
     </row>
     <row r="31" spans="2:27" ht="180.75" customHeight="1">
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="50"/>
-      <c r="V31" s="50"/>
-      <c r="W31" s="50"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="50"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
       <c r="AA31" s="16"/>
     </row>
     <row r="32" spans="2:27" ht="280.5" customHeight="1">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="54">
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="43">
         <v>45708</v>
       </c>
-      <c r="L32" s="55"/>
-      <c r="M32" s="54">
+      <c r="L32" s="44"/>
+      <c r="M32" s="43">
         <v>45709</v>
       </c>
-      <c r="N32" s="55"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="49"/>
-      <c r="U32" s="50" t="s">
+      <c r="N32" s="44"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="V32" s="50"/>
-      <c r="W32" s="50"/>
-      <c r="X32" s="50"/>
-      <c r="Y32" s="50"/>
+      <c r="V32" s="42"/>
+      <c r="W32" s="42"/>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="42"/>
     </row>
     <row r="33" spans="2:25" ht="259.5" customHeight="1">
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="50"/>
-      <c r="V33" s="50"/>
-      <c r="W33" s="50"/>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="50"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="42"/>
+      <c r="V33" s="42"/>
+      <c r="W33" s="42"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
     </row>
     <row r="34" spans="2:25" ht="295.5" customHeight="1">
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="54">
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="43">
         <v>45709</v>
       </c>
-      <c r="L34" s="55"/>
-      <c r="M34" s="54">
+      <c r="L34" s="44"/>
+      <c r="M34" s="43">
         <v>45710</v>
       </c>
-      <c r="N34" s="55"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="49"/>
-      <c r="U34" s="50" t="s">
+      <c r="N34" s="44"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="V34" s="50"/>
-      <c r="W34" s="50"/>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="50"/>
+      <c r="V34" s="42"/>
+      <c r="W34" s="42"/>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="42"/>
     </row>
     <row r="35" spans="2:25" ht="265.5" customHeight="1">
-      <c r="B35" s="37"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="49"/>
-      <c r="U35" s="50"/>
-      <c r="V35" s="50"/>
-      <c r="W35" s="50"/>
-      <c r="X35" s="50"/>
-      <c r="Y35" s="50"/>
-    </row>
-    <row r="36" spans="2:25" ht="15" customHeight="1">
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="49"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="49"/>
-      <c r="T36" s="49"/>
-      <c r="U36" s="50"/>
-      <c r="V36" s="50"/>
-      <c r="W36" s="50"/>
-      <c r="X36" s="50"/>
-      <c r="Y36" s="50"/>
-    </row>
-    <row r="37" spans="2:25" ht="15" customHeight="1">
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="50"/>
-      <c r="V37" s="50"/>
-      <c r="W37" s="50"/>
-      <c r="X37" s="50"/>
-      <c r="Y37" s="50"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="42"/>
+      <c r="V35" s="42"/>
+      <c r="W35" s="42"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="42"/>
+    </row>
+    <row r="36" spans="2:25" ht="249.75" customHeight="1">
+      <c r="B36" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="43">
+        <v>45712</v>
+      </c>
+      <c r="L36" s="44"/>
+      <c r="M36" s="43">
+        <v>45712</v>
+      </c>
+      <c r="N36" s="44"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="V36" s="42"/>
+      <c r="W36" s="42"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
+    </row>
+    <row r="37" spans="2:25" ht="211.5" customHeight="1">
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="41"/>
+      <c r="U37" s="42"/>
+      <c r="V37" s="42"/>
+      <c r="W37" s="42"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
     </row>
     <row r="38" spans="2:25" ht="15" customHeight="1">
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="54"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="49"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="49"/>
-      <c r="U38" s="50"/>
-      <c r="V38" s="50"/>
-      <c r="W38" s="50"/>
-      <c r="X38" s="50"/>
-      <c r="Y38" s="50"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="42"/>
+      <c r="V38" s="42"/>
+      <c r="W38" s="42"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
     </row>
     <row r="39" spans="2:25" ht="15" customHeight="1">
-      <c r="B39" s="37"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="50"/>
-      <c r="V39" s="50"/>
-      <c r="W39" s="50"/>
-      <c r="X39" s="50"/>
-      <c r="Y39" s="50"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="41"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="42"/>
+      <c r="V39" s="42"/>
+      <c r="W39" s="42"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
     </row>
     <row r="40" spans="2:25" ht="15" customHeight="1">
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="55"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="50"/>
-      <c r="V40" s="50"/>
-      <c r="W40" s="50"/>
-      <c r="X40" s="50"/>
-      <c r="Y40" s="50"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="41"/>
+      <c r="U40" s="42"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="42"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
     </row>
     <row r="41" spans="2:25" ht="15" customHeight="1">
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="57"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="57"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-      <c r="T41" s="49"/>
-      <c r="U41" s="50"/>
-      <c r="V41" s="50"/>
-      <c r="W41" s="50"/>
-      <c r="X41" s="50"/>
-      <c r="Y41" s="50"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="41"/>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="41"/>
+      <c r="R41" s="41"/>
+      <c r="S41" s="41"/>
+      <c r="T41" s="41"/>
+      <c r="U41" s="42"/>
+      <c r="V41" s="42"/>
+      <c r="W41" s="42"/>
+      <c r="X41" s="42"/>
+      <c r="Y41" s="42"/>
     </row>
     <row r="42" spans="2:25" ht="15" customHeight="1">
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="51"/>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="51"/>
-      <c r="R42" s="51"/>
-      <c r="S42" s="51"/>
-      <c r="T42" s="51"/>
-      <c r="U42" s="51"/>
-      <c r="V42" s="51"/>
-      <c r="W42" s="51"/>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="51"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="95"/>
+      <c r="G42" s="95"/>
+      <c r="H42" s="95"/>
+      <c r="I42" s="95"/>
+      <c r="J42" s="95"/>
+      <c r="K42" s="95"/>
+      <c r="L42" s="95"/>
+      <c r="M42" s="95"/>
+      <c r="N42" s="95"/>
+      <c r="O42" s="95"/>
+      <c r="P42" s="95"/>
+      <c r="Q42" s="95"/>
+      <c r="R42" s="95"/>
+      <c r="S42" s="95"/>
+      <c r="T42" s="95"/>
+      <c r="U42" s="95"/>
+      <c r="V42" s="95"/>
+      <c r="W42" s="95"/>
+      <c r="X42" s="95"/>
+      <c r="Y42" s="95"/>
     </row>
     <row r="43" spans="2:25" ht="15" customHeight="1">
       <c r="B43" s="10"/>
@@ -3701,16 +3968,16 @@
       <c r="Y43" s="10"/>
     </row>
     <row r="44" spans="2:25" ht="15" customHeight="1">
-      <c r="B44" s="77" t="s">
+      <c r="B44" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="77"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="68"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
@@ -3721,11 +3988,11 @@
       <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
-      <c r="T44" s="76"/>
-      <c r="U44" s="77"/>
-      <c r="V44" s="77"/>
-      <c r="W44" s="77"/>
-      <c r="X44" s="77"/>
+      <c r="T44" s="67"/>
+      <c r="U44" s="68"/>
+      <c r="V44" s="68"/>
+      <c r="W44" s="68"/>
+      <c r="X44" s="68"/>
       <c r="Y44" s="10"/>
     </row>
     <row r="45" spans="2:25" ht="15" customHeight="1">
@@ -3755,35 +4022,35 @@
       <c r="Y45" s="8"/>
     </row>
     <row r="46" spans="2:25">
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
       <c r="J46" s="11"/>
-      <c r="K46" s="40" t="s">
+      <c r="K46" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L46" s="40"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="40"/>
-      <c r="O46" s="40"/>
-      <c r="P46" s="40"/>
-      <c r="Q46" s="40"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
       <c r="R46" s="13"/>
       <c r="S46" s="11"/>
-      <c r="T46" s="19" t="s">
+      <c r="T46" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
       <c r="Y46" s="11"/>
     </row>
     <row r="47" spans="2:25">
@@ -3813,16 +4080,16 @@
       <c r="Y47" s="11"/>
     </row>
     <row r="48" spans="2:25" ht="15" customHeight="1">
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
     </row>
     <row r="49" spans="2:25" ht="15" customHeight="1">
       <c r="B49" s="14"/>
@@ -3851,100 +4118,184 @@
       <c r="Y49" s="12"/>
     </row>
     <row r="50" spans="2:25" ht="15.75" customHeight="1">
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
       <c r="J50" s="11"/>
-      <c r="K50" s="40" t="s">
+      <c r="K50" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40"/>
-      <c r="N50" s="40"/>
-      <c r="O50" s="40"/>
-      <c r="P50" s="40"/>
-      <c r="Q50" s="40"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
       <c r="R50" s="13"/>
-      <c r="S50" s="88" t="s">
+      <c r="S50" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
-      <c r="W50" s="18"/>
-      <c r="X50" s="18"/>
-      <c r="Y50" s="18"/>
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="20"/>
+      <c r="Y50" s="20"/>
     </row>
     <row r="51" spans="2:25" ht="23.25" customHeight="1">
-      <c r="Q51" s="48"/>
-      <c r="R51" s="48"/>
-      <c r="S51" s="48"/>
-      <c r="T51" s="48"/>
-      <c r="U51" s="48"/>
+      <c r="Q51" s="94"/>
+      <c r="R51" s="94"/>
+      <c r="S51" s="94"/>
+      <c r="T51" s="94"/>
+      <c r="U51" s="94"/>
     </row>
     <row r="52" spans="2:25" ht="18" customHeight="1">
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="18"/>
-      <c r="U52" s="18"/>
-      <c r="V52" s="18"/>
-      <c r="W52" s="18"/>
-      <c r="X52" s="18"/>
-      <c r="Y52" s="18"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="20"/>
+      <c r="S52" s="20"/>
+      <c r="T52" s="20"/>
+      <c r="U52" s="20"/>
+      <c r="V52" s="20"/>
+      <c r="W52" s="20"/>
+      <c r="X52" s="20"/>
+      <c r="Y52" s="20"/>
     </row>
     <row r="53" spans="2:25">
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-      <c r="U53" s="18"/>
-      <c r="V53" s="18"/>
-      <c r="W53" s="18"/>
-      <c r="X53" s="18"/>
-      <c r="Y53" s="18"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="20"/>
+      <c r="R53" s="20"/>
+      <c r="S53" s="20"/>
+      <c r="T53" s="20"/>
+      <c r="U53" s="20"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="20"/>
+      <c r="X53" s="20"/>
+      <c r="Y53" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="B52:Y53"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="K22:Y22"/>
+    <mergeCell ref="O16:Q17"/>
+    <mergeCell ref="S16:T17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="K16:M17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="B32:J33"/>
+    <mergeCell ref="B28:J29"/>
+    <mergeCell ref="K46:Q46"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="O38:T39"/>
+    <mergeCell ref="U38:Y39"/>
+    <mergeCell ref="T46:X46"/>
+    <mergeCell ref="U32:Y33"/>
+    <mergeCell ref="B42:Y42"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="O36:T37"/>
+    <mergeCell ref="K30:L31"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="K34:L35"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="B8:Y8"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O28:T29"/>
+    <mergeCell ref="U28:Y29"/>
+    <mergeCell ref="O30:T31"/>
+    <mergeCell ref="U30:Y31"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="B30:J31"/>
+    <mergeCell ref="U26:Y27"/>
+    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="O25:T25"/>
+    <mergeCell ref="T44:X44"/>
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O26:T26"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="K23:Y23"/>
+    <mergeCell ref="U25:Y25"/>
+    <mergeCell ref="B26:J27"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="B50:I50"/>
     <mergeCell ref="K50:Q50"/>
     <mergeCell ref="S50:Y50"/>
@@ -3969,90 +4320,6 @@
     <mergeCell ref="U36:Y37"/>
     <mergeCell ref="B36:J37"/>
     <mergeCell ref="B34:J35"/>
-    <mergeCell ref="K23:Y23"/>
-    <mergeCell ref="U25:Y25"/>
-    <mergeCell ref="B26:J27"/>
-    <mergeCell ref="B6:Y6"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="B30:J31"/>
-    <mergeCell ref="U26:Y27"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="O25:T25"/>
-    <mergeCell ref="T44:X44"/>
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O26:T26"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="O36:T37"/>
-    <mergeCell ref="K30:L31"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="M26:N27"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="K34:L35"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O28:T29"/>
-    <mergeCell ref="U28:Y29"/>
-    <mergeCell ref="O30:T31"/>
-    <mergeCell ref="U30:Y31"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B52:Y53"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="K22:Y22"/>
-    <mergeCell ref="O16:Q17"/>
-    <mergeCell ref="S16:T17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="K16:M17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="B32:J33"/>
-    <mergeCell ref="B28:J29"/>
-    <mergeCell ref="K46:Q46"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="O38:T39"/>
-    <mergeCell ref="U38:Y39"/>
-    <mergeCell ref="T46:X46"/>
-    <mergeCell ref="U32:Y33"/>
-    <mergeCell ref="B42:Y42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T20" r:id="rId1" xr:uid="{BE351EEA-9877-430E-96A9-ADC6513FEEA9}"/>
@@ -4080,124 +4347,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1">
-      <c r="A2" s="96"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="104" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1">
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
+      <c r="U3" s="125"/>
+      <c r="V3" s="125"/>
+      <c r="W3" s="125"/>
+      <c r="X3" s="125"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="101" t="s">
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="103"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123"/>
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123"/>
+      <c r="X4" s="124"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="99"/>
-      <c r="U5" s="99"/>
-      <c r="V5" s="99"/>
-      <c r="W5" s="99"/>
-      <c r="X5" s="100"/>
+      <c r="A5" s="119"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="120"/>
+      <c r="T5" s="120"/>
+      <c r="U5" s="120"/>
+      <c r="V5" s="120"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="121"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A6" s="3"/>
@@ -4226,66 +4493,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="97"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97" t="s">
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97" t="s">
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="97"/>
-      <c r="T7" s="97"/>
-      <c r="U7" s="97"/>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
+      <c r="Q7" s="100"/>
+      <c r="R7" s="100"/>
+      <c r="S7" s="100"/>
+      <c r="T7" s="100"/>
+      <c r="U7" s="100"/>
+      <c r="V7" s="100"/>
+      <c r="W7" s="100"/>
+      <c r="X7" s="100"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="106" t="s">
+      <c r="A8" s="93"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="93"/>
+      <c r="J8" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="107"/>
-      <c r="O8" s="108"/>
-      <c r="P8" s="106" t="s">
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="107"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="107"/>
-      <c r="T8" s="107"/>
-      <c r="U8" s="107"/>
-      <c r="V8" s="107"/>
-      <c r="W8" s="107"/>
-      <c r="X8" s="108"/>
+      <c r="Q8" s="108"/>
+      <c r="R8" s="108"/>
+      <c r="S8" s="108"/>
+      <c r="T8" s="108"/>
+      <c r="U8" s="108"/>
+      <c r="V8" s="108"/>
+      <c r="W8" s="108"/>
+      <c r="X8" s="109"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A9" s="3"/>
@@ -4314,66 +4581,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
+      <c r="X10" s="79"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81" t="s">
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81" t="s">
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81" t="s">
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="T11" s="81"/>
-      <c r="U11" s="81"/>
-      <c r="V11" s="81"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="3"/>
@@ -4402,66 +4669,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97" t="s">
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="97"/>
-      <c r="P13" s="97" t="s">
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="97"/>
-      <c r="R13" s="97"/>
-      <c r="S13" s="97"/>
-      <c r="T13" s="97"/>
-      <c r="U13" s="97"/>
-      <c r="V13" s="97"/>
-      <c r="W13" s="97"/>
-      <c r="X13" s="97"/>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="100"/>
+      <c r="S13" s="100"/>
+      <c r="T13" s="100"/>
+      <c r="U13" s="100"/>
+      <c r="V13" s="100"/>
+      <c r="W13" s="100"/>
+      <c r="X13" s="100"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="106" t="s">
+      <c r="A14" s="93"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="107"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="107"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="108"/>
-      <c r="P14" s="106" t="s">
+      <c r="K14" s="108"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
-      <c r="U14" s="107"/>
-      <c r="V14" s="107"/>
-      <c r="W14" s="107"/>
-      <c r="X14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="108"/>
+      <c r="X14" s="109"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A15" s="3"/>
@@ -4490,172 +4757,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="114" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="114"/>
-      <c r="L16" s="114"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="19" t="s">
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
+      <c r="N16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="115" t="s">
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="115"/>
-      <c r="V16" s="115"/>
-      <c r="W16" s="115"/>
-      <c r="X16" s="115"/>
+      <c r="U16" s="111"/>
+      <c r="V16" s="111"/>
+      <c r="W16" s="111"/>
+      <c r="X16" s="111"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="116" t="s">
+      <c r="B17" s="102"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="109" t="s">
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="114"/>
+      <c r="N17" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="104"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="110"/>
-      <c r="T17" s="109" t="s">
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="103"/>
+      <c r="T17" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="104"/>
-      <c r="V17" s="104"/>
-      <c r="W17" s="104"/>
-      <c r="X17" s="110"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="102"/>
+      <c r="W17" s="102"/>
+      <c r="X17" s="103"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A18" s="111"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="113"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="121"/>
-      <c r="N18" s="111"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
-      <c r="S18" s="113"/>
-      <c r="T18" s="111"/>
-      <c r="U18" s="112"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="112"/>
-      <c r="X18" s="113"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="115"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="116"/>
+      <c r="M18" s="117"/>
+      <c r="N18" s="104"/>
+      <c r="O18" s="105"/>
+      <c r="P18" s="105"/>
+      <c r="Q18" s="105"/>
+      <c r="R18" s="105"/>
+      <c r="S18" s="106"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="105"/>
+      <c r="X18" s="106"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1"/>
     <row r="20" spans="1:24" ht="39" customHeight="1"/>
     <row r="21" spans="1:24">
-      <c r="A21" s="125" t="s">
+      <c r="A21" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="125"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="125"/>
-      <c r="F21" s="125"/>
-      <c r="G21" s="125"/>
-      <c r="H21" s="125"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="125" t="s">
+      <c r="J21" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="125"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
-      <c r="O21" s="125"/>
-      <c r="P21" s="125"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="99"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="125" t="s">
+      <c r="R21" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="125"/>
-      <c r="T21" s="125"/>
-      <c r="U21" s="125"/>
-      <c r="V21" s="125"/>
-      <c r="W21" s="125"/>
-      <c r="X21" s="125"/>
+      <c r="S21" s="99"/>
+      <c r="T21" s="99"/>
+      <c r="U21" s="99"/>
+      <c r="V21" s="99"/>
+      <c r="W21" s="99"/>
+      <c r="X21" s="99"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P23" s="122" t="s">
+      <c r="P23" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="122"/>
-      <c r="R23" s="122"/>
-      <c r="S23" s="122"/>
-      <c r="T23" s="122"/>
-      <c r="U23" s="123" t="s">
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
+      <c r="T23" s="96"/>
+      <c r="U23" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="123"/>
-      <c r="W23" s="123"/>
-      <c r="X23" s="123"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="97"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P24" s="122" t="s">
+      <c r="P24" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="124" t="s">
+      <c r="Q24" s="96"/>
+      <c r="R24" s="96"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="96"/>
+      <c r="U24" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="124"/>
-      <c r="W24" s="124"/>
-      <c r="X24" s="124"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -4670,25 +4949,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
acomodar btn download y notificaciones
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
+++ b/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\pruebas\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADDA751-5DC4-4D82-81F0-F745CA367C05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2FE8A8-76BB-4BE9-A326-0761E257E197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
   <si>
     <t>BITÁCORA DE SEGUIMIENTO ETAPA PRODUCTIVA</t>
   </si>
@@ -345,6 +345,15 @@
   <si>
     <t>las imágenes al provenir de un servidor diferente al que reside la pagina  hacia que el naveganor me prohiviera hacerlo directamente (esto me complico mucho) 
 pero lo peor fue intentar hayar la forma de agregar el boton por cada imagen del post. Queria hacerlos atravez del html para que sea mas optimizdo pero desafortunadamente seme hiso imposible por como funciona blogger asi que me rendi y tuve que agregar los botones artificialmente atravez de js</t>
+  </si>
+  <si>
+    <t>acomode los botones de descarga para que tuviera una mejor presentacion 
+estuve revisando un buen rato el codigo de descarga de los botones pero no fui capas de encontrar una forma para que fueran mas rapidos, aun que tienen un velocidad aceptable
+cree un sistema de notificaciones globales y asi poderlas usar en cualquier parate del proyecto, ademas para probarlas las integre al sistema de descarga de imagenes
+como extra organise los marcadores de una mejor forma, ahora se llaman marker, y son mas pequeños</t>
+  </si>
+  <si>
+    <t>sin mayores complicaciones, como dije antes lo unico fue lo de la forma de descargar imágenes que no lo pude mejorar</t>
   </si>
 </sst>
 </file>
@@ -735,7 +744,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -785,17 +794,192 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -803,20 +987,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -836,42 +1011,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -881,151 +1026,78 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1044,70 +1116,58 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1132,6 +1192,56 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>41912</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>756038</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9831</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1391478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Imagen 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3EA13F1-F24E-4CDF-A6AB-138735A3A97A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5831455" y="45432429"/>
+          <a:ext cx="1980593" cy="635440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1160,7 +1270,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
@@ -1203,7 +1313,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1253,7 +1363,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1303,7 +1413,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1353,7 +1463,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1403,7 +1513,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1453,7 +1563,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1503,7 +1613,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1553,7 +1663,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1603,7 +1713,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1653,7 +1763,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1703,7 +1813,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1753,7 +1863,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1803,7 +1913,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1853,7 +1963,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1903,7 +2013,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1953,7 +2063,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2003,7 +2113,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2053,7 +2163,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2103,7 +2213,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2153,7 +2263,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2203,7 +2313,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2253,7 +2363,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2303,7 +2413,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2353,7 +2463,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2368,6 +2478,156 @@
         <a:xfrm>
           <a:off x="6245998" y="43492890"/>
           <a:ext cx="1333686" cy="990738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>298707</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>115527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>364435</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1568958</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Imagen 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA77F260-8B73-47E3-8A8B-49D6FC01CEF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239533" y="44791918"/>
+          <a:ext cx="927119" cy="1453431"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>174323</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>100357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>256947</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>704022</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Imagen 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9A63A1-F459-4C3C-8E47-876CD6728748}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5963866" y="44776748"/>
+          <a:ext cx="1233907" cy="603665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>49696</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1707290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>273327</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>715760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Imagen 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1170F93-363E-4E9A-9FAD-06CD13BA4446}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5839239" y="46383681"/>
+          <a:ext cx="2236305" cy="1799709"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2786,10 +3046,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AA53"/>
+  <dimension ref="B1:AA59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A38" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38:Y39"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A39" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40:Y41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
@@ -2814,294 +3074,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B1" s="59"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="52" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
     </row>
     <row r="2" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="58" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
     </row>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="77"/>
     </row>
     <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
     </row>
     <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="67"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="53"/>
+      <c r="Y5" s="54"/>
     </row>
     <row r="6" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="66"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="67"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="54"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1">
-      <c r="B8" s="40"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="68"/>
-      <c r="V8" s="68"/>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="68"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="78"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="78"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="78"/>
     </row>
     <row r="9" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="73" t="s">
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="95"/>
-      <c r="T9" s="23" t="s">
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="23" t="s">
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="73">
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="30">
         <v>5</v>
       </c>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="95"/>
-      <c r="T10" s="81" t="s">
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B11" s="3"/>
@@ -3130,68 +3390,68 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="82" t="s">
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82" t="s">
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="82"/>
-      <c r="S12" s="82"/>
-      <c r="T12" s="82"/>
-      <c r="U12" s="82"/>
-      <c r="V12" s="82"/>
-      <c r="W12" s="82"/>
-      <c r="X12" s="82"/>
-      <c r="Y12" s="82"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1">
-      <c r="B13" s="84">
+      <c r="B13" s="63">
         <v>3177294629</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="49">
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="41">
         <v>3177294629</v>
       </c>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="83" t="s">
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="81"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
-      <c r="Y13" s="81"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
+      <c r="Y13" s="57"/>
     </row>
     <row r="14" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B14" s="3"/>
@@ -3220,100 +3480,100 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1">
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
-      <c r="T15" s="69"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="69"/>
-      <c r="W15" s="69"/>
-      <c r="X15" s="69"/>
-      <c r="Y15" s="69"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="79"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="79"/>
+      <c r="X15" s="79"/>
+      <c r="Y15" s="79"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="25" t="s">
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28" t="s">
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="25" t="s">
+      <c r="L16" s="85"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="25" t="s">
+      <c r="P16" s="83"/>
+      <c r="Q16" s="83"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="25"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="25" t="s">
+      <c r="T16" s="55"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="27"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="56"/>
     </row>
     <row r="17" spans="2:27" ht="45.75" customHeight="1">
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="27"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
+      <c r="Y17" s="56"/>
     </row>
     <row r="18" spans="2:27" ht="9.9499999999999993" customHeight="1">
       <c r="B18" s="3"/>
@@ -3342,72 +3602,72 @@
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="2:27" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="44" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="44" t="s">
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="20" t="s">
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="91"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="27"/>
     </row>
     <row r="20" spans="2:27" ht="18" customHeight="1">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="46">
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="92">
         <v>1096800316</v>
       </c>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="89">
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="93"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="23">
         <v>3219713759</v>
       </c>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="92" t="s">
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="U20" s="93"/>
-      <c r="V20" s="93"/>
-      <c r="W20" s="93"/>
-      <c r="X20" s="93"/>
-      <c r="Y20" s="91"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="27"/>
     </row>
     <row r="21" spans="2:27" ht="9.75" customHeight="1">
       <c r="B21" s="8"/>
@@ -3436,64 +3696,64 @@
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:27" ht="18" customHeight="1">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="23" t="s">
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="82"/>
+      <c r="W22" s="82"/>
+      <c r="X22" s="82"/>
+      <c r="Y22" s="82"/>
     </row>
     <row r="23" spans="2:27" ht="18" customHeight="1">
-      <c r="B23" s="70">
+      <c r="B23" s="60">
         <v>2557356</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="78" t="s">
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="S23" s="79"/>
-      <c r="T23" s="79"/>
-      <c r="U23" s="79"/>
-      <c r="V23" s="79"/>
-      <c r="W23" s="79"/>
-      <c r="X23" s="79"/>
-      <c r="Y23" s="80"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="49"/>
     </row>
     <row r="24" spans="2:27" ht="9.75" customHeight="1">
       <c r="B24" s="3"/>
@@ -3522,874 +3782,999 @@
       <c r="Y24" s="3"/>
     </row>
     <row r="25" spans="2:27" ht="48" customHeight="1">
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="73" t="s">
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="74"/>
-      <c r="M25" s="73" t="s">
+      <c r="L25" s="50"/>
+      <c r="M25" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="74"/>
-      <c r="O25" s="73" t="s">
+      <c r="N25" s="50"/>
+      <c r="O25" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="73" t="s">
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="74"/>
-      <c r="W25" s="74"/>
-      <c r="X25" s="74"/>
-      <c r="Y25" s="75"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="51"/>
     </row>
     <row r="26" spans="2:27" ht="216" customHeight="1">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="54">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="43">
         <v>45705</v>
       </c>
-      <c r="L26" s="55"/>
-      <c r="M26" s="54">
+      <c r="L26" s="44"/>
+      <c r="M26" s="43">
         <v>45706</v>
       </c>
-      <c r="N26" s="55"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="71"/>
-      <c r="Q26" s="71"/>
-      <c r="R26" s="71"/>
-      <c r="S26" s="71"/>
-      <c r="T26" s="72"/>
-      <c r="U26" s="50" t="s">
+      <c r="N26" s="44"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="61"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="61"/>
+      <c r="T26" s="62"/>
+      <c r="U26" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="50"/>
+      <c r="V26" s="42"/>
+      <c r="W26" s="42"/>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="42"/>
     </row>
     <row r="27" spans="2:27" ht="232.5" customHeight="1">
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="71"/>
-      <c r="S27" s="71"/>
-      <c r="T27" s="72"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="50"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="42"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="42"/>
     </row>
     <row r="28" spans="2:27" ht="126.75" customHeight="1">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="54">
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="43">
         <v>45706</v>
       </c>
-      <c r="L28" s="55"/>
-      <c r="M28" s="54">
+      <c r="L28" s="44"/>
+      <c r="M28" s="43">
         <v>45707</v>
       </c>
-      <c r="N28" s="55"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="49"/>
-      <c r="U28" s="50" t="s">
+      <c r="N28" s="44"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="V28" s="50"/>
-      <c r="W28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="50"/>
+      <c r="V28" s="42"/>
+      <c r="W28" s="42"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
     </row>
     <row r="29" spans="2:27" ht="189" customHeight="1">
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="49"/>
-      <c r="U29" s="50"/>
-      <c r="V29" s="50"/>
-      <c r="W29" s="50"/>
-      <c r="X29" s="50"/>
-      <c r="Y29" s="50"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="42"/>
+      <c r="V29" s="42"/>
+      <c r="W29" s="42"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="42"/>
       <c r="AA29" s="16"/>
     </row>
     <row r="30" spans="2:27" ht="105" customHeight="1">
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="54">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="43">
         <v>45707</v>
       </c>
-      <c r="L30" s="55"/>
-      <c r="M30" s="54">
+      <c r="L30" s="44"/>
+      <c r="M30" s="43">
         <v>45708</v>
       </c>
-      <c r="N30" s="55"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="50" t="s">
+      <c r="N30" s="44"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="V30" s="50"/>
-      <c r="W30" s="50"/>
-      <c r="X30" s="50"/>
-      <c r="Y30" s="50"/>
+      <c r="V30" s="42"/>
+      <c r="W30" s="42"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="42"/>
     </row>
     <row r="31" spans="2:27" ht="180.75" customHeight="1">
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="50"/>
-      <c r="V31" s="50"/>
-      <c r="W31" s="50"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="50"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
       <c r="AA31" s="16"/>
     </row>
     <row r="32" spans="2:27" ht="280.5" customHeight="1">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="54">
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="43">
         <v>45708</v>
       </c>
-      <c r="L32" s="55"/>
-      <c r="M32" s="54">
+      <c r="L32" s="44"/>
+      <c r="M32" s="43">
         <v>45709</v>
       </c>
-      <c r="N32" s="55"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="49"/>
-      <c r="U32" s="50" t="s">
+      <c r="N32" s="44"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="V32" s="50"/>
-      <c r="W32" s="50"/>
-      <c r="X32" s="50"/>
-      <c r="Y32" s="50"/>
+      <c r="V32" s="42"/>
+      <c r="W32" s="42"/>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="42"/>
     </row>
     <row r="33" spans="2:25" ht="259.5" customHeight="1">
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="50"/>
-      <c r="V33" s="50"/>
-      <c r="W33" s="50"/>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="50"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="42"/>
+      <c r="V33" s="42"/>
+      <c r="W33" s="42"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
     </row>
     <row r="34" spans="2:25" ht="295.5" customHeight="1">
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="54">
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="43">
         <v>45709</v>
       </c>
-      <c r="L34" s="55"/>
-      <c r="M34" s="54">
+      <c r="L34" s="44"/>
+      <c r="M34" s="43">
         <v>45710</v>
       </c>
-      <c r="N34" s="55"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="49"/>
-      <c r="U34" s="50" t="s">
+      <c r="N34" s="44"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="V34" s="50"/>
-      <c r="W34" s="50"/>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="50"/>
+      <c r="V34" s="42"/>
+      <c r="W34" s="42"/>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="42"/>
     </row>
     <row r="35" spans="2:25" ht="265.5" customHeight="1">
-      <c r="B35" s="37"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="49"/>
-      <c r="U35" s="50"/>
-      <c r="V35" s="50"/>
-      <c r="W35" s="50"/>
-      <c r="X35" s="50"/>
-      <c r="Y35" s="50"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="42"/>
+      <c r="V35" s="42"/>
+      <c r="W35" s="42"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="42"/>
     </row>
     <row r="36" spans="2:25" ht="249.75" customHeight="1">
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="54">
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="43">
         <v>45712</v>
       </c>
-      <c r="L36" s="55"/>
-      <c r="M36" s="54">
+      <c r="L36" s="44"/>
+      <c r="M36" s="43">
         <v>45713</v>
       </c>
-      <c r="N36" s="55"/>
-      <c r="O36" s="49"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="49"/>
-      <c r="T36" s="49"/>
-      <c r="U36" s="50" t="s">
+      <c r="N36" s="44"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="V36" s="50"/>
-      <c r="W36" s="50"/>
-      <c r="X36" s="50"/>
-      <c r="Y36" s="50"/>
+      <c r="V36" s="42"/>
+      <c r="W36" s="42"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
     </row>
     <row r="37" spans="2:25" ht="211.5" customHeight="1">
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="50"/>
-      <c r="V37" s="50"/>
-      <c r="W37" s="50"/>
-      <c r="X37" s="50"/>
-      <c r="Y37" s="50"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="41"/>
+      <c r="U37" s="42"/>
+      <c r="V37" s="42"/>
+      <c r="W37" s="42"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
     </row>
     <row r="38" spans="2:25" ht="182.25" customHeight="1">
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="54">
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="43">
         <v>45713</v>
       </c>
-      <c r="L38" s="55"/>
-      <c r="M38" s="54">
+      <c r="L38" s="44"/>
+      <c r="M38" s="43">
         <v>45714</v>
       </c>
-      <c r="N38" s="55"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="49"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="49"/>
-      <c r="U38" s="50" t="s">
+      <c r="N38" s="44"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="V38" s="50"/>
-      <c r="W38" s="50"/>
-      <c r="X38" s="50"/>
-      <c r="Y38" s="50"/>
+      <c r="V38" s="42"/>
+      <c r="W38" s="42"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
     </row>
     <row r="39" spans="2:25" ht="165.75" customHeight="1">
-      <c r="B39" s="37"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="50"/>
-      <c r="V39" s="50"/>
-      <c r="W39" s="50"/>
-      <c r="X39" s="50"/>
-      <c r="Y39" s="50"/>
-    </row>
-    <row r="40" spans="2:25" ht="15" customHeight="1">
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="55"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="50"/>
-      <c r="V40" s="50"/>
-      <c r="W40" s="50"/>
-      <c r="X40" s="50"/>
-      <c r="Y40" s="50"/>
-    </row>
-    <row r="41" spans="2:25" ht="15" customHeight="1">
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="57"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="57"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-      <c r="T41" s="49"/>
-      <c r="U41" s="50"/>
-      <c r="V41" s="50"/>
-      <c r="W41" s="50"/>
-      <c r="X41" s="50"/>
-      <c r="Y41" s="50"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="41"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="42"/>
+      <c r="V39" s="42"/>
+      <c r="W39" s="42"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+    </row>
+    <row r="40" spans="2:25" ht="219.75" customHeight="1">
+      <c r="B40" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="129"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="129"/>
+      <c r="O40" s="132"/>
+      <c r="P40" s="133"/>
+      <c r="Q40" s="133"/>
+      <c r="R40" s="133"/>
+      <c r="S40" s="133"/>
+      <c r="T40" s="134"/>
+      <c r="U40" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="V40" s="36"/>
+      <c r="W40" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="Y40" s="37"/>
+    </row>
+    <row r="41" spans="2:25" ht="153" customHeight="1">
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="130"/>
+      <c r="L41" s="131"/>
+      <c r="M41" s="130"/>
+      <c r="N41" s="131"/>
+      <c r="O41" s="135"/>
+      <c r="P41" s="136"/>
+      <c r="Q41" s="136"/>
+      <c r="R41" s="136"/>
+      <c r="S41" s="136"/>
+      <c r="T41" s="137"/>
+      <c r="U41" s="38"/>
+      <c r="V41" s="39"/>
+      <c r="W41" s="39"/>
+      <c r="X41" s="39"/>
+      <c r="Y41" s="40"/>
     </row>
     <row r="42" spans="2:25" ht="15" customHeight="1">
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="35"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="129"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="132"/>
+      <c r="P42" s="133"/>
+      <c r="Q42" s="133"/>
+      <c r="R42" s="133"/>
+      <c r="S42" s="133"/>
+      <c r="T42" s="134"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="36"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="Y42" s="37"/>
+    </row>
+    <row r="43" spans="2:25" ht="15" customHeight="1">
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="131"/>
+      <c r="M43" s="130"/>
+      <c r="N43" s="131"/>
+      <c r="O43" s="135"/>
+      <c r="P43" s="136"/>
+      <c r="Q43" s="136"/>
+      <c r="R43" s="136"/>
+      <c r="S43" s="136"/>
+      <c r="T43" s="137"/>
+      <c r="U43" s="38"/>
+      <c r="V43" s="39"/>
+      <c r="W43" s="39"/>
+      <c r="X43" s="39"/>
+      <c r="Y43" s="40"/>
+    </row>
+    <row r="44" spans="2:25" ht="15" customHeight="1">
+      <c r="B44" s="126"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="127"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="127"/>
+      <c r="H44" s="127"/>
+      <c r="I44" s="127"/>
+      <c r="J44" s="128"/>
+      <c r="K44" s="138"/>
+      <c r="L44" s="139"/>
+      <c r="M44" s="138"/>
+      <c r="N44" s="139"/>
+      <c r="O44" s="140"/>
+      <c r="P44" s="141"/>
+      <c r="Q44" s="141"/>
+      <c r="R44" s="141"/>
+      <c r="S44" s="141"/>
+      <c r="T44" s="142"/>
+      <c r="U44" s="126"/>
+      <c r="V44" s="127"/>
+      <c r="W44" s="127"/>
+      <c r="X44" s="127"/>
+      <c r="Y44" s="128"/>
+    </row>
+    <row r="45" spans="2:25" ht="15" customHeight="1">
+      <c r="B45" s="126"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="127"/>
+      <c r="E45" s="127"/>
+      <c r="F45" s="127"/>
+      <c r="G45" s="127"/>
+      <c r="H45" s="127"/>
+      <c r="I45" s="127"/>
+      <c r="J45" s="128"/>
+      <c r="K45" s="138"/>
+      <c r="L45" s="139"/>
+      <c r="M45" s="138"/>
+      <c r="N45" s="139"/>
+      <c r="O45" s="140"/>
+      <c r="P45" s="141"/>
+      <c r="Q45" s="141"/>
+      <c r="R45" s="141"/>
+      <c r="S45" s="141"/>
+      <c r="T45" s="142"/>
+      <c r="U45" s="126"/>
+      <c r="V45" s="127"/>
+      <c r="W45" s="127"/>
+      <c r="X45" s="127"/>
+      <c r="Y45" s="128"/>
+    </row>
+    <row r="46" spans="2:25">
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="129"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="129"/>
+      <c r="O46" s="132"/>
+      <c r="P46" s="133"/>
+      <c r="Q46" s="133"/>
+      <c r="R46" s="133"/>
+      <c r="S46" s="133"/>
+      <c r="T46" s="134"/>
+      <c r="U46" s="35"/>
+      <c r="V46" s="36"/>
+      <c r="W46" s="36"/>
+      <c r="X46" s="36"/>
+      <c r="Y46" s="37"/>
+    </row>
+    <row r="47" spans="2:25">
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="130"/>
+      <c r="L47" s="131"/>
+      <c r="M47" s="130"/>
+      <c r="N47" s="131"/>
+      <c r="O47" s="135"/>
+      <c r="P47" s="136"/>
+      <c r="Q47" s="136"/>
+      <c r="R47" s="136"/>
+      <c r="S47" s="136"/>
+      <c r="T47" s="137"/>
+      <c r="U47" s="38"/>
+      <c r="V47" s="39"/>
+      <c r="W47" s="39"/>
+      <c r="X47" s="39"/>
+      <c r="Y47" s="40"/>
+    </row>
+    <row r="48" spans="2:25" ht="15" customHeight="1">
+      <c r="B48" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="51"/>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="51"/>
-      <c r="R42" s="51"/>
-      <c r="S42" s="51"/>
-      <c r="T42" s="51"/>
-      <c r="U42" s="51"/>
-      <c r="V42" s="51"/>
-      <c r="W42" s="51"/>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="51"/>
-    </row>
-    <row r="43" spans="2:25" ht="15" customHeight="1">
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
-      <c r="V43" s="10"/>
-      <c r="W43" s="10"/>
-      <c r="X43" s="10"/>
-      <c r="Y43" s="10"/>
-    </row>
-    <row r="44" spans="2:25" ht="15" customHeight="1">
-      <c r="B44" s="77" t="s">
+      <c r="C48" s="95"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="95"/>
+      <c r="I48" s="95"/>
+      <c r="J48" s="95"/>
+      <c r="K48" s="95"/>
+      <c r="L48" s="95"/>
+      <c r="M48" s="95"/>
+      <c r="N48" s="95"/>
+      <c r="O48" s="95"/>
+      <c r="P48" s="95"/>
+      <c r="Q48" s="95"/>
+      <c r="R48" s="95"/>
+      <c r="S48" s="95"/>
+      <c r="T48" s="95"/>
+      <c r="U48" s="95"/>
+      <c r="V48" s="95"/>
+      <c r="W48" s="95"/>
+      <c r="X48" s="95"/>
+      <c r="Y48" s="95"/>
+    </row>
+    <row r="49" spans="2:25" ht="15" customHeight="1">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="10"/>
+      <c r="V49" s="10"/>
+      <c r="W49" s="10"/>
+      <c r="X49" s="10"/>
+      <c r="Y49" s="10"/>
+    </row>
+    <row r="50" spans="2:25" ht="15.75" customHeight="1">
+      <c r="B50" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="76"/>
-      <c r="U44" s="77"/>
-      <c r="V44" s="77"/>
-      <c r="W44" s="77"/>
-      <c r="X44" s="77"/>
-      <c r="Y44" s="10"/>
-    </row>
-    <row r="45" spans="2:25" ht="15" customHeight="1">
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="12"/>
-      <c r="U45" s="12"/>
-      <c r="V45" s="12"/>
-      <c r="W45" s="12"/>
-      <c r="X45" s="12"/>
-      <c r="Y45" s="8"/>
-    </row>
-    <row r="46" spans="2:25">
-      <c r="B46" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="L46" s="40"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="40"/>
-      <c r="O46" s="40"/>
-      <c r="P46" s="40"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="11"/>
-      <c r="T46" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="11"/>
-    </row>
-    <row r="47" spans="2:25">
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="13"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-      <c r="V47" s="15"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="11"/>
-    </row>
-    <row r="48" spans="2:25" ht="15" customHeight="1">
-      <c r="B48" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-    </row>
-    <row r="49" spans="2:25" ht="15" customHeight="1">
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="12"/>
-      <c r="T49" s="12"/>
-      <c r="U49" s="12"/>
-      <c r="V49" s="12"/>
-      <c r="W49" s="12"/>
-      <c r="X49" s="12"/>
-      <c r="Y49" s="12"/>
-    </row>
-    <row r="50" spans="2:25" ht="15.75" customHeight="1">
-      <c r="B50" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40"/>
-      <c r="N50" s="40"/>
-      <c r="O50" s="40"/>
-      <c r="P50" s="40"/>
-      <c r="Q50" s="40"/>
-      <c r="R50" s="13"/>
-      <c r="S50" s="88" t="s">
-        <v>56</v>
-      </c>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
-      <c r="W50" s="18"/>
-      <c r="X50" s="18"/>
-      <c r="Y50" s="18"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="68"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="67"/>
+      <c r="U50" s="68"/>
+      <c r="V50" s="68"/>
+      <c r="W50" s="68"/>
+      <c r="X50" s="68"/>
+      <c r="Y50" s="10"/>
     </row>
     <row r="51" spans="2:25" ht="23.25" customHeight="1">
-      <c r="Q51" s="48"/>
-      <c r="R51" s="48"/>
-      <c r="S51" s="48"/>
-      <c r="T51" s="48"/>
-      <c r="U51" s="48"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="X51" s="12"/>
+      <c r="Y51" s="8"/>
     </row>
     <row r="52" spans="2:25" ht="18" customHeight="1">
       <c r="B52" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="L52" s="18"/>
       <c r="M52" s="18"/>
       <c r="N52" s="18"/>
       <c r="O52" s="18"/>
       <c r="P52" s="18"/>
       <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="18"/>
-      <c r="U52" s="18"/>
-      <c r="V52" s="18"/>
-      <c r="W52" s="18"/>
-      <c r="X52" s="18"/>
-      <c r="Y52" s="18"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="U52" s="17"/>
+      <c r="V52" s="17"/>
+      <c r="W52" s="17"/>
+      <c r="X52" s="17"/>
+      <c r="Y52" s="11"/>
     </row>
     <row r="53" spans="2:25">
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-      <c r="U53" s="18"/>
-      <c r="V53" s="18"/>
-      <c r="W53" s="18"/>
-      <c r="X53" s="18"/>
-      <c r="Y53" s="18"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="15"/>
+      <c r="X53" s="15"/>
+      <c r="Y53" s="11"/>
+    </row>
+    <row r="54" spans="2:25">
+      <c r="B54" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="2:25">
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="12"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="12"/>
+      <c r="V55" s="12"/>
+      <c r="W55" s="12"/>
+      <c r="X55" s="12"/>
+      <c r="Y55" s="12"/>
+    </row>
+    <row r="56" spans="2:25">
+      <c r="B56" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="13"/>
+      <c r="S56" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="20"/>
+      <c r="X56" s="20"/>
+      <c r="Y56" s="20"/>
+    </row>
+    <row r="57" spans="2:25">
+      <c r="Q57" s="94"/>
+      <c r="R57" s="94"/>
+      <c r="S57" s="94"/>
+      <c r="T57" s="94"/>
+      <c r="U57" s="94"/>
+    </row>
+    <row r="58" spans="2:25">
+      <c r="B58" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="73"/>
+      <c r="K58" s="73"/>
+      <c r="L58" s="73"/>
+      <c r="M58" s="73"/>
+      <c r="N58" s="73"/>
+      <c r="O58" s="73"/>
+      <c r="P58" s="73"/>
+      <c r="Q58" s="73"/>
+      <c r="R58" s="73"/>
+      <c r="S58" s="73"/>
+      <c r="T58" s="73"/>
+      <c r="U58" s="73"/>
+      <c r="V58" s="73"/>
+      <c r="W58" s="73"/>
+      <c r="X58" s="73"/>
+      <c r="Y58" s="73"/>
+    </row>
+    <row r="59" spans="2:25">
+      <c r="B59" s="73"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
+      <c r="J59" s="73"/>
+      <c r="K59" s="73"/>
+      <c r="L59" s="73"/>
+      <c r="M59" s="73"/>
+      <c r="N59" s="73"/>
+      <c r="O59" s="73"/>
+      <c r="P59" s="73"/>
+      <c r="Q59" s="73"/>
+      <c r="R59" s="73"/>
+      <c r="S59" s="73"/>
+      <c r="T59" s="73"/>
+      <c r="U59" s="73"/>
+      <c r="V59" s="73"/>
+      <c r="W59" s="73"/>
+      <c r="X59" s="73"/>
+      <c r="Y59" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="K50:Q50"/>
-    <mergeCell ref="S50:Y50"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="T19:Y19"/>
-    <mergeCell ref="T20:Y20"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="B40:J41"/>
-    <mergeCell ref="O40:T41"/>
-    <mergeCell ref="U40:Y41"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="O34:T35"/>
-    <mergeCell ref="U34:Y35"/>
-    <mergeCell ref="B38:J39"/>
-    <mergeCell ref="M36:N37"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="M38:N39"/>
-    <mergeCell ref="U36:Y37"/>
-    <mergeCell ref="B36:J37"/>
-    <mergeCell ref="B34:J35"/>
-    <mergeCell ref="K23:Y23"/>
-    <mergeCell ref="U25:Y25"/>
-    <mergeCell ref="B26:J27"/>
-    <mergeCell ref="B6:Y6"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="B30:J31"/>
-    <mergeCell ref="U26:Y27"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="O25:T25"/>
-    <mergeCell ref="T44:X44"/>
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O26:T26"/>
-    <mergeCell ref="B44:I44"/>
+  <mergeCells count="118">
+    <mergeCell ref="U42:Y43"/>
+    <mergeCell ref="B58:Y59"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="K22:Y22"/>
+    <mergeCell ref="O16:Q17"/>
+    <mergeCell ref="S16:T17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="K16:M17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="B32:J33"/>
+    <mergeCell ref="B28:J29"/>
+    <mergeCell ref="K52:Q52"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="Q57:U57"/>
+    <mergeCell ref="O38:T39"/>
+    <mergeCell ref="U38:Y39"/>
+    <mergeCell ref="T52:X52"/>
+    <mergeCell ref="U32:Y33"/>
+    <mergeCell ref="B48:Y48"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="O36:T37"/>
     <mergeCell ref="K30:L31"/>
@@ -4414,30 +4799,75 @@
     <mergeCell ref="O30:T31"/>
     <mergeCell ref="U30:Y31"/>
     <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B52:Y53"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="K22:Y22"/>
-    <mergeCell ref="O16:Q17"/>
-    <mergeCell ref="S16:T17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="K16:M17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="B32:J33"/>
-    <mergeCell ref="B28:J29"/>
-    <mergeCell ref="K46:Q46"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="O38:T39"/>
-    <mergeCell ref="U38:Y39"/>
-    <mergeCell ref="T46:X46"/>
-    <mergeCell ref="U32:Y33"/>
-    <mergeCell ref="B42:Y42"/>
+    <mergeCell ref="M46:N47"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B30:J31"/>
+    <mergeCell ref="U26:Y27"/>
+    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="O25:T25"/>
+    <mergeCell ref="T50:X50"/>
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O26:T26"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B40:J41"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="O40:T41"/>
+    <mergeCell ref="U40:Y41"/>
+    <mergeCell ref="B42:J43"/>
+    <mergeCell ref="K42:L43"/>
+    <mergeCell ref="M42:N43"/>
+    <mergeCell ref="O42:T43"/>
+    <mergeCell ref="K23:Y23"/>
+    <mergeCell ref="U25:Y25"/>
+    <mergeCell ref="B26:J27"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="K56:Q56"/>
+    <mergeCell ref="S56:Y56"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="T20:Y20"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="B46:J47"/>
+    <mergeCell ref="O46:T47"/>
+    <mergeCell ref="U46:Y47"/>
+    <mergeCell ref="K46:L47"/>
+    <mergeCell ref="O34:T35"/>
+    <mergeCell ref="U34:Y35"/>
+    <mergeCell ref="B38:J39"/>
+    <mergeCell ref="M36:N37"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="M38:N39"/>
+    <mergeCell ref="U36:Y37"/>
+    <mergeCell ref="B36:J37"/>
+    <mergeCell ref="B34:J35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T20" r:id="rId1" xr:uid="{BE351EEA-9877-430E-96A9-ADC6513FEEA9}"/>
@@ -4465,124 +4895,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1">
-      <c r="A2" s="96"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="104" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1">
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
+      <c r="U3" s="125"/>
+      <c r="V3" s="125"/>
+      <c r="W3" s="125"/>
+      <c r="X3" s="125"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="101" t="s">
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="103"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123"/>
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123"/>
+      <c r="X4" s="124"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="99"/>
-      <c r="U5" s="99"/>
-      <c r="V5" s="99"/>
-      <c r="W5" s="99"/>
-      <c r="X5" s="100"/>
+      <c r="A5" s="119"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="120"/>
+      <c r="T5" s="120"/>
+      <c r="U5" s="120"/>
+      <c r="V5" s="120"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="121"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A6" s="3"/>
@@ -4611,66 +5041,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="97"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97" t="s">
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97" t="s">
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="97"/>
-      <c r="T7" s="97"/>
-      <c r="U7" s="97"/>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
+      <c r="Q7" s="100"/>
+      <c r="R7" s="100"/>
+      <c r="S7" s="100"/>
+      <c r="T7" s="100"/>
+      <c r="U7" s="100"/>
+      <c r="V7" s="100"/>
+      <c r="W7" s="100"/>
+      <c r="X7" s="100"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="106" t="s">
+      <c r="A8" s="93"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="93"/>
+      <c r="J8" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="107"/>
-      <c r="O8" s="108"/>
-      <c r="P8" s="106" t="s">
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="107"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="107"/>
-      <c r="T8" s="107"/>
-      <c r="U8" s="107"/>
-      <c r="V8" s="107"/>
-      <c r="W8" s="107"/>
-      <c r="X8" s="108"/>
+      <c r="Q8" s="108"/>
+      <c r="R8" s="108"/>
+      <c r="S8" s="108"/>
+      <c r="T8" s="108"/>
+      <c r="U8" s="108"/>
+      <c r="V8" s="108"/>
+      <c r="W8" s="108"/>
+      <c r="X8" s="109"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A9" s="3"/>
@@ -4699,66 +5129,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
+      <c r="X10" s="79"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81" t="s">
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81" t="s">
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81" t="s">
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="T11" s="81"/>
-      <c r="U11" s="81"/>
-      <c r="V11" s="81"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="3"/>
@@ -4787,66 +5217,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97" t="s">
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="97"/>
-      <c r="P13" s="97" t="s">
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="97"/>
-      <c r="R13" s="97"/>
-      <c r="S13" s="97"/>
-      <c r="T13" s="97"/>
-      <c r="U13" s="97"/>
-      <c r="V13" s="97"/>
-      <c r="W13" s="97"/>
-      <c r="X13" s="97"/>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="100"/>
+      <c r="S13" s="100"/>
+      <c r="T13" s="100"/>
+      <c r="U13" s="100"/>
+      <c r="V13" s="100"/>
+      <c r="W13" s="100"/>
+      <c r="X13" s="100"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="106" t="s">
+      <c r="A14" s="93"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="107"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="107"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="108"/>
-      <c r="P14" s="106" t="s">
+      <c r="K14" s="108"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
-      <c r="U14" s="107"/>
-      <c r="V14" s="107"/>
-      <c r="W14" s="107"/>
-      <c r="X14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="108"/>
+      <c r="X14" s="109"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A15" s="3"/>
@@ -4875,172 +5305,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="114" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="114"/>
-      <c r="L16" s="114"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="19" t="s">
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
+      <c r="N16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="115" t="s">
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="115"/>
-      <c r="V16" s="115"/>
-      <c r="W16" s="115"/>
-      <c r="X16" s="115"/>
+      <c r="U16" s="111"/>
+      <c r="V16" s="111"/>
+      <c r="W16" s="111"/>
+      <c r="X16" s="111"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="116" t="s">
+      <c r="B17" s="102"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="109" t="s">
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="114"/>
+      <c r="N17" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="104"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="110"/>
-      <c r="T17" s="109" t="s">
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="103"/>
+      <c r="T17" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="104"/>
-      <c r="V17" s="104"/>
-      <c r="W17" s="104"/>
-      <c r="X17" s="110"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="102"/>
+      <c r="W17" s="102"/>
+      <c r="X17" s="103"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A18" s="111"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="113"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="121"/>
-      <c r="N18" s="111"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
-      <c r="S18" s="113"/>
-      <c r="T18" s="111"/>
-      <c r="U18" s="112"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="112"/>
-      <c r="X18" s="113"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="115"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="116"/>
+      <c r="M18" s="117"/>
+      <c r="N18" s="104"/>
+      <c r="O18" s="105"/>
+      <c r="P18" s="105"/>
+      <c r="Q18" s="105"/>
+      <c r="R18" s="105"/>
+      <c r="S18" s="106"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="105"/>
+      <c r="X18" s="106"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1"/>
     <row r="20" spans="1:24" ht="39" customHeight="1"/>
     <row r="21" spans="1:24">
-      <c r="A21" s="125" t="s">
+      <c r="A21" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="125"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="125"/>
-      <c r="F21" s="125"/>
-      <c r="G21" s="125"/>
-      <c r="H21" s="125"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="125" t="s">
+      <c r="J21" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="125"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
-      <c r="O21" s="125"/>
-      <c r="P21" s="125"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="99"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="125" t="s">
+      <c r="R21" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="125"/>
-      <c r="T21" s="125"/>
-      <c r="U21" s="125"/>
-      <c r="V21" s="125"/>
-      <c r="W21" s="125"/>
-      <c r="X21" s="125"/>
+      <c r="S21" s="99"/>
+      <c r="T21" s="99"/>
+      <c r="U21" s="99"/>
+      <c r="V21" s="99"/>
+      <c r="W21" s="99"/>
+      <c r="X21" s="99"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P23" s="122" t="s">
+      <c r="P23" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="122"/>
-      <c r="R23" s="122"/>
-      <c r="S23" s="122"/>
-      <c r="T23" s="122"/>
-      <c r="U23" s="123" t="s">
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
+      <c r="T23" s="96"/>
+      <c r="U23" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="123"/>
-      <c r="W23" s="123"/>
-      <c r="X23" s="123"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="97"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P24" s="122" t="s">
+      <c r="P24" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="124" t="s">
+      <c r="Q24" s="96"/>
+      <c r="R24" s="96"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="96"/>
+      <c r="U24" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="124"/>
-      <c r="W24" s="124"/>
-      <c r="X24" s="124"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -5055,25 +5497,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
notis, tamaños, inserciones en el menu
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
+++ b/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\pruebas\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2FE8A8-76BB-4BE9-A326-0761E257E197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A83269-7906-48EA-9082-55AADF3C2E4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
   <si>
     <t>BITÁCORA DE SEGUIMIENTO ETAPA PRODUCTIVA</t>
   </si>
@@ -354,6 +354,16 @@
   </si>
   <si>
     <t>sin mayores complicaciones, como dije antes lo unico fue lo de la forma de descargar imágenes que no lo pude mejorar</t>
+  </si>
+  <si>
+    <t>mejore las funciones para notificaciones, ahora el titulo el personalizable ademas de tener 3 tipos distintos info, positibe y negative cada una con su respectivo color
+me puse un buen rato a buscar denuevo alguna forma para descargar las imágenes mas rapido pero no puede
+agrege las vistas que ah tenido el blog
+agrege una visualizacion de las ultimas publicaciones de x del cena 
+cambie los tamaños de el menu lateral y contenedor principal, son un poco mas grandes y con mejores margenes</t>
+  </si>
+  <si>
+    <t>falle al intentar optimizar la imagenn</t>
   </si>
 </sst>
 </file>
@@ -794,36 +804,277 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -833,200 +1084,88 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1039,135 +1178,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2628,6 +2638,256 @@
         <a:xfrm>
           <a:off x="5839239" y="46383681"/>
           <a:ext cx="2236305" cy="1799709"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>130332</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>812538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>348230</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1383196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Imagen 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D2ED7A-A6C4-4565-8807-5C70E3F3B815}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7071158" y="50226581"/>
+          <a:ext cx="1079289" cy="570658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>17701</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>2569604</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>314740</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>631163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagen 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40CDA0B5-369E-487A-AFAA-514FA047ECA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5807244" y="51983647"/>
+          <a:ext cx="2309713" cy="1382886"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>157370</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>320662</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>3529</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>806852</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Imagen 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA38D481-FC97-45A6-9DF4-C2F906291B7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7098196" y="49734705"/>
+          <a:ext cx="1088550" cy="486190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>99392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>376220</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>2446682</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Imagen 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{082AAA19-4BFF-4AD9-9221-D1E91158FF6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5880652" y="49513435"/>
+          <a:ext cx="1047111" cy="2347290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>124240</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1529298</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>265045</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1973908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Imagen 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E50E0F7-895E-4E3B-A0BA-50F5695D5AB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7065066" y="50943341"/>
+          <a:ext cx="1002196" cy="444610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3048,8 +3308,8 @@
   </sheetPr>
   <dimension ref="B1:AA59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A39" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40:Y41"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="U42" sqref="U42:Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
@@ -3074,294 +3334,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B1" s="71"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="69" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
     </row>
     <row r="2" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="34" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="68"/>
+      <c r="W2" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
     </row>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="77"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
     </row>
     <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="71"/>
+      <c r="Y4" s="71"/>
     </row>
     <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="54"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="73"/>
+      <c r="W5" s="73"/>
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74"/>
     </row>
     <row r="6" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="54"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="73"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
+      <c r="X6" s="73"/>
+      <c r="Y6" s="74"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="52"/>
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1">
-      <c r="B8" s="18"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="78"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="78"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="75"/>
+      <c r="V8" s="75"/>
+      <c r="W8" s="75"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="75"/>
     </row>
     <row r="9" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="30" t="s">
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="33" t="s">
+      <c r="Q9" s="111"/>
+      <c r="R9" s="111"/>
+      <c r="S9" s="112"/>
+      <c r="T9" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="33"/>
-      <c r="V9" s="33"/>
-      <c r="W9" s="33"/>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="36"/>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="33" t="s">
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="30">
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="83">
         <v>5</v>
       </c>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="57" t="s">
+      <c r="Q10" s="111"/>
+      <c r="R10" s="111"/>
+      <c r="S10" s="112"/>
+      <c r="T10" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
+      <c r="U10" s="97"/>
+      <c r="V10" s="97"/>
+      <c r="W10" s="97"/>
+      <c r="X10" s="97"/>
+      <c r="Y10" s="97"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B11" s="3"/>
@@ -3390,68 +3650,68 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="58" t="s">
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58" t="s">
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
+      <c r="R12" s="98"/>
+      <c r="S12" s="98"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="98"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="98"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1">
-      <c r="B13" s="63">
+      <c r="B13" s="100">
         <v>3177294629</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="41">
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="56">
         <v>3177294629</v>
       </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="59" t="s">
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
+      <c r="R13" s="97"/>
+      <c r="S13" s="97"/>
+      <c r="T13" s="97"/>
+      <c r="U13" s="97"/>
+      <c r="V13" s="97"/>
+      <c r="W13" s="97"/>
+      <c r="X13" s="97"/>
+      <c r="Y13" s="97"/>
     </row>
     <row r="14" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B14" s="3"/>
@@ -3480,100 +3740,100 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1">
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="79"/>
-      <c r="X15" s="79"/>
-      <c r="Y15" s="79"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="76"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="76"/>
+      <c r="R15" s="76"/>
+      <c r="S15" s="76"/>
+      <c r="T15" s="76"/>
+      <c r="U15" s="76"/>
+      <c r="V15" s="76"/>
+      <c r="W15" s="76"/>
+      <c r="X15" s="76"/>
+      <c r="Y15" s="76"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1">
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="F16" s="38"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="84" t="s">
+      <c r="I16" s="38"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="85"/>
-      <c r="M16" s="86"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="55" t="s">
+      <c r="L16" s="42"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="55" t="s">
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="55"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="55" t="s">
+      <c r="T16" s="38"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
-      <c r="Y16" s="56"/>
+      <c r="W16" s="38"/>
+      <c r="X16" s="38"/>
+      <c r="Y16" s="40"/>
     </row>
     <row r="17" spans="2:27" ht="45.75" customHeight="1">
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="89"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="55"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="55"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="55"/>
-      <c r="Y17" s="56"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="40"/>
     </row>
     <row r="18" spans="2:27" ht="9.9499999999999993" customHeight="1">
       <c r="B18" s="3"/>
@@ -3602,72 +3862,72 @@
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="2:27" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="21" t="s">
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="21" t="s">
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="25" t="s">
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="27"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="48"/>
+      <c r="W19" s="48"/>
+      <c r="X19" s="48"/>
+      <c r="Y19" s="108"/>
     </row>
     <row r="20" spans="2:27" ht="18" customHeight="1">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="92">
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="53">
         <v>1096800316</v>
       </c>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="23">
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="106">
         <v>3219713759</v>
       </c>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="28" t="s">
+      <c r="P20" s="107"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="107"/>
+      <c r="S20" s="107"/>
+      <c r="T20" s="109" t="s">
         <v>71</v>
       </c>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="27"/>
+      <c r="U20" s="110"/>
+      <c r="V20" s="110"/>
+      <c r="W20" s="110"/>
+      <c r="X20" s="110"/>
+      <c r="Y20" s="108"/>
     </row>
     <row r="21" spans="2:27" ht="9.75" customHeight="1">
       <c r="B21" s="8"/>
@@ -3696,64 +3956,64 @@
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:27" ht="18" customHeight="1">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="33" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="82"/>
-      <c r="R22" s="82"/>
-      <c r="S22" s="82"/>
-      <c r="T22" s="82"/>
-      <c r="U22" s="82"/>
-      <c r="V22" s="82"/>
-      <c r="W22" s="82"/>
-      <c r="X22" s="82"/>
-      <c r="Y22" s="82"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
     </row>
     <row r="23" spans="2:27" ht="18" customHeight="1">
-      <c r="B23" s="60">
+      <c r="B23" s="77">
         <v>2557356</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="47" t="s">
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
-      <c r="Y23" s="49"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="95"/>
+      <c r="Q23" s="95"/>
+      <c r="R23" s="95"/>
+      <c r="S23" s="95"/>
+      <c r="T23" s="95"/>
+      <c r="U23" s="95"/>
+      <c r="V23" s="95"/>
+      <c r="W23" s="95"/>
+      <c r="X23" s="95"/>
+      <c r="Y23" s="96"/>
     </row>
     <row r="24" spans="2:27" ht="9.75" customHeight="1">
       <c r="B24" s="3"/>
@@ -3782,702 +4042,706 @@
       <c r="Y24" s="3"/>
     </row>
     <row r="25" spans="2:27" ht="48" customHeight="1">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="30" t="s">
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="50"/>
-      <c r="M25" s="30" t="s">
+      <c r="L25" s="84"/>
+      <c r="M25" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="50"/>
-      <c r="O25" s="30" t="s">
+      <c r="N25" s="84"/>
+      <c r="O25" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="30" t="s">
+      <c r="P25" s="84"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="84"/>
+      <c r="S25" s="84"/>
+      <c r="T25" s="85"/>
+      <c r="U25" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="51"/>
+      <c r="V25" s="84"/>
+      <c r="W25" s="84"/>
+      <c r="X25" s="84"/>
+      <c r="Y25" s="85"/>
     </row>
     <row r="26" spans="2:27" ht="216" customHeight="1">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="43">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="61">
         <v>45705</v>
       </c>
-      <c r="L26" s="44"/>
-      <c r="M26" s="43">
+      <c r="L26" s="62"/>
+      <c r="M26" s="61">
         <v>45706</v>
       </c>
-      <c r="N26" s="44"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="61"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="42" t="s">
+      <c r="N26" s="62"/>
+      <c r="O26" s="77"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="79"/>
+      <c r="U26" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="V26" s="42"/>
-      <c r="W26" s="42"/>
-      <c r="X26" s="42"/>
-      <c r="Y26" s="42"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="57"/>
     </row>
     <row r="27" spans="2:27" ht="232.5" customHeight="1">
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="42"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="42"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="77"/>
+      <c r="P27" s="78"/>
+      <c r="Q27" s="78"/>
+      <c r="R27" s="78"/>
+      <c r="S27" s="78"/>
+      <c r="T27" s="79"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="57"/>
     </row>
     <row r="28" spans="2:27" ht="126.75" customHeight="1">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="43">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="61">
         <v>45706</v>
       </c>
-      <c r="L28" s="44"/>
-      <c r="M28" s="43">
+      <c r="L28" s="62"/>
+      <c r="M28" s="61">
         <v>45707</v>
       </c>
-      <c r="N28" s="44"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="42" t="s">
+      <c r="N28" s="62"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="V28" s="42"/>
-      <c r="W28" s="42"/>
-      <c r="X28" s="42"/>
-      <c r="Y28" s="42"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="57"/>
+      <c r="X28" s="57"/>
+      <c r="Y28" s="57"/>
     </row>
     <row r="29" spans="2:27" ht="189" customHeight="1">
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="42"/>
-      <c r="W29" s="42"/>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="42"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="57"/>
+      <c r="Y29" s="57"/>
       <c r="AA29" s="16"/>
     </row>
     <row r="30" spans="2:27" ht="105" customHeight="1">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="43">
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="61">
         <v>45707</v>
       </c>
-      <c r="L30" s="44"/>
-      <c r="M30" s="43">
+      <c r="L30" s="62"/>
+      <c r="M30" s="61">
         <v>45708</v>
       </c>
-      <c r="N30" s="44"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="42" t="s">
+      <c r="N30" s="62"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="S30" s="56"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="V30" s="42"/>
-      <c r="W30" s="42"/>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="42"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="57"/>
     </row>
     <row r="31" spans="2:27" ht="180.75" customHeight="1">
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="42"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="42"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="56"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
       <c r="AA31" s="16"/>
     </row>
     <row r="32" spans="2:27" ht="280.5" customHeight="1">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="43">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="61">
         <v>45708</v>
       </c>
-      <c r="L32" s="44"/>
-      <c r="M32" s="43">
+      <c r="L32" s="62"/>
+      <c r="M32" s="61">
         <v>45709</v>
       </c>
-      <c r="N32" s="44"/>
-      <c r="O32" s="41"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="42" t="s">
+      <c r="N32" s="62"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="56"/>
+      <c r="U32" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="V32" s="42"/>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="57"/>
     </row>
     <row r="33" spans="2:25" ht="259.5" customHeight="1">
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="41"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="42"/>
-      <c r="V33" s="42"/>
-      <c r="W33" s="42"/>
-      <c r="X33" s="42"/>
-      <c r="Y33" s="42"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="56"/>
+      <c r="U33" s="57"/>
+      <c r="V33" s="57"/>
+      <c r="W33" s="57"/>
+      <c r="X33" s="57"/>
+      <c r="Y33" s="57"/>
     </row>
     <row r="34" spans="2:25" ht="295.5" customHeight="1">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="43">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="61">
         <v>45709</v>
       </c>
-      <c r="L34" s="44"/>
-      <c r="M34" s="43">
+      <c r="L34" s="62"/>
+      <c r="M34" s="61">
         <v>45710</v>
       </c>
-      <c r="N34" s="44"/>
-      <c r="O34" s="41"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="41"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="42" t="s">
+      <c r="N34" s="62"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="56"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+      <c r="U34" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="V34" s="42"/>
-      <c r="W34" s="42"/>
-      <c r="X34" s="42"/>
-      <c r="Y34" s="42"/>
+      <c r="V34" s="57"/>
+      <c r="W34" s="57"/>
+      <c r="X34" s="57"/>
+      <c r="Y34" s="57"/>
     </row>
     <row r="35" spans="2:25" ht="265.5" customHeight="1">
-      <c r="B35" s="38"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="41"/>
-      <c r="P35" s="41"/>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="41"/>
-      <c r="S35" s="41"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="42"/>
-      <c r="V35" s="42"/>
-      <c r="W35" s="42"/>
-      <c r="X35" s="42"/>
-      <c r="Y35" s="42"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+      <c r="S35" s="56"/>
+      <c r="T35" s="56"/>
+      <c r="U35" s="57"/>
+      <c r="V35" s="57"/>
+      <c r="W35" s="57"/>
+      <c r="X35" s="57"/>
+      <c r="Y35" s="57"/>
     </row>
     <row r="36" spans="2:25" ht="249.75" customHeight="1">
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="43">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="61">
         <v>45712</v>
       </c>
-      <c r="L36" s="44"/>
-      <c r="M36" s="43">
+      <c r="L36" s="62"/>
+      <c r="M36" s="61">
         <v>45713</v>
       </c>
-      <c r="N36" s="44"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="41"/>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="42" t="s">
+      <c r="N36" s="62"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="56"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="56"/>
+      <c r="U36" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="V36" s="42"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="42"/>
+      <c r="V36" s="57"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57"/>
     </row>
     <row r="37" spans="2:25" ht="211.5" customHeight="1">
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="41"/>
-      <c r="S37" s="41"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="42"/>
-      <c r="V37" s="42"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="42"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="64"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="64"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="56"/>
+      <c r="S37" s="56"/>
+      <c r="T37" s="56"/>
+      <c r="U37" s="57"/>
+      <c r="V37" s="57"/>
+      <c r="W37" s="57"/>
+      <c r="X37" s="57"/>
+      <c r="Y37" s="57"/>
     </row>
     <row r="38" spans="2:25" ht="182.25" customHeight="1">
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="43">
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="61">
         <v>45713</v>
       </c>
-      <c r="L38" s="44"/>
-      <c r="M38" s="43">
+      <c r="L38" s="62"/>
+      <c r="M38" s="61">
         <v>45714</v>
       </c>
-      <c r="N38" s="44"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="42" t="s">
+      <c r="N38" s="62"/>
+      <c r="O38" s="56"/>
+      <c r="P38" s="56"/>
+      <c r="Q38" s="56"/>
+      <c r="R38" s="56"/>
+      <c r="S38" s="56"/>
+      <c r="T38" s="56"/>
+      <c r="U38" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="V38" s="42"/>
-      <c r="W38" s="42"/>
-      <c r="X38" s="42"/>
-      <c r="Y38" s="42"/>
+      <c r="V38" s="57"/>
+      <c r="W38" s="57"/>
+      <c r="X38" s="57"/>
+      <c r="Y38" s="57"/>
     </row>
     <row r="39" spans="2:25" ht="165.75" customHeight="1">
-      <c r="B39" s="38"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="41"/>
-      <c r="P39" s="41"/>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="41"/>
-      <c r="S39" s="41"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="42"/>
-      <c r="V39" s="42"/>
-      <c r="W39" s="42"/>
-      <c r="X39" s="42"/>
-      <c r="Y39" s="42"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="64"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="56"/>
+      <c r="T39" s="56"/>
+      <c r="U39" s="57"/>
+      <c r="V39" s="57"/>
+      <c r="W39" s="57"/>
+      <c r="X39" s="57"/>
+      <c r="Y39" s="57"/>
     </row>
     <row r="40" spans="2:25" ht="219.75" customHeight="1">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="129"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="129"/>
-      <c r="O40" s="132"/>
-      <c r="P40" s="133"/>
-      <c r="Q40" s="133"/>
-      <c r="R40" s="133"/>
-      <c r="S40" s="133"/>
-      <c r="T40" s="134"/>
-      <c r="U40" s="35" t="s">
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="80"/>
+      <c r="O40" s="88"/>
+      <c r="P40" s="89"/>
+      <c r="Q40" s="89"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="89"/>
+      <c r="T40" s="90"/>
+      <c r="U40" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="V40" s="36"/>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="37"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="27"/>
     </row>
     <row r="41" spans="2:25" ht="153" customHeight="1">
-      <c r="B41" s="38"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="130"/>
-      <c r="L41" s="131"/>
-      <c r="M41" s="130"/>
-      <c r="N41" s="131"/>
-      <c r="O41" s="135"/>
-      <c r="P41" s="136"/>
-      <c r="Q41" s="136"/>
-      <c r="R41" s="136"/>
-      <c r="S41" s="136"/>
-      <c r="T41" s="137"/>
-      <c r="U41" s="38"/>
-      <c r="V41" s="39"/>
-      <c r="W41" s="39"/>
-      <c r="X41" s="39"/>
-      <c r="Y41" s="40"/>
-    </row>
-    <row r="42" spans="2:25" ht="15" customHeight="1">
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="129"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="129"/>
-      <c r="O42" s="132"/>
-      <c r="P42" s="133"/>
-      <c r="Q42" s="133"/>
-      <c r="R42" s="133"/>
-      <c r="S42" s="133"/>
-      <c r="T42" s="134"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="36"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="37"/>
-    </row>
-    <row r="43" spans="2:25" ht="15" customHeight="1">
-      <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="131"/>
-      <c r="M43" s="130"/>
-      <c r="N43" s="131"/>
-      <c r="O43" s="135"/>
-      <c r="P43" s="136"/>
-      <c r="Q43" s="136"/>
-      <c r="R43" s="136"/>
-      <c r="S43" s="136"/>
-      <c r="T43" s="137"/>
-      <c r="U43" s="38"/>
-      <c r="V43" s="39"/>
-      <c r="W43" s="39"/>
-      <c r="X43" s="39"/>
-      <c r="Y43" s="40"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="81"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="81"/>
+      <c r="N41" s="82"/>
+      <c r="O41" s="91"/>
+      <c r="P41" s="92"/>
+      <c r="Q41" s="92"/>
+      <c r="R41" s="92"/>
+      <c r="S41" s="92"/>
+      <c r="T41" s="93"/>
+      <c r="U41" s="28"/>
+      <c r="V41" s="29"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="30"/>
+    </row>
+    <row r="42" spans="2:25" ht="261.75" customHeight="1">
+      <c r="B42" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="61"/>
+      <c r="L42" s="80"/>
+      <c r="M42" s="61"/>
+      <c r="N42" s="80"/>
+      <c r="O42" s="88"/>
+      <c r="P42" s="89"/>
+      <c r="Q42" s="89"/>
+      <c r="R42" s="89"/>
+      <c r="S42" s="89"/>
+      <c r="T42" s="90"/>
+      <c r="U42" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="27"/>
+    </row>
+    <row r="43" spans="2:25" ht="204" customHeight="1">
+      <c r="B43" s="28"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="81"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="81"/>
+      <c r="N43" s="82"/>
+      <c r="O43" s="91"/>
+      <c r="P43" s="92"/>
+      <c r="Q43" s="92"/>
+      <c r="R43" s="92"/>
+      <c r="S43" s="92"/>
+      <c r="T43" s="93"/>
+      <c r="U43" s="28"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="30"/>
     </row>
     <row r="44" spans="2:25" ht="15" customHeight="1">
-      <c r="B44" s="126"/>
-      <c r="C44" s="127"/>
-      <c r="D44" s="127"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="127"/>
-      <c r="I44" s="127"/>
-      <c r="J44" s="128"/>
-      <c r="K44" s="138"/>
-      <c r="L44" s="139"/>
-      <c r="M44" s="138"/>
-      <c r="N44" s="139"/>
-      <c r="O44" s="140"/>
-      <c r="P44" s="141"/>
-      <c r="Q44" s="141"/>
-      <c r="R44" s="141"/>
-      <c r="S44" s="141"/>
-      <c r="T44" s="142"/>
-      <c r="U44" s="126"/>
-      <c r="V44" s="127"/>
-      <c r="W44" s="127"/>
-      <c r="X44" s="127"/>
-      <c r="Y44" s="128"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="18"/>
+      <c r="W44" s="18"/>
+      <c r="X44" s="18"/>
+      <c r="Y44" s="19"/>
     </row>
     <row r="45" spans="2:25" ht="15" customHeight="1">
-      <c r="B45" s="126"/>
-      <c r="C45" s="127"/>
-      <c r="D45" s="127"/>
-      <c r="E45" s="127"/>
-      <c r="F45" s="127"/>
-      <c r="G45" s="127"/>
-      <c r="H45" s="127"/>
-      <c r="I45" s="127"/>
-      <c r="J45" s="128"/>
-      <c r="K45" s="138"/>
-      <c r="L45" s="139"/>
-      <c r="M45" s="138"/>
-      <c r="N45" s="139"/>
-      <c r="O45" s="140"/>
-      <c r="P45" s="141"/>
-      <c r="Q45" s="141"/>
-      <c r="R45" s="141"/>
-      <c r="S45" s="141"/>
-      <c r="T45" s="142"/>
-      <c r="U45" s="126"/>
-      <c r="V45" s="127"/>
-      <c r="W45" s="127"/>
-      <c r="X45" s="127"/>
-      <c r="Y45" s="128"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="23"/>
+      <c r="S45" s="23"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="18"/>
+      <c r="W45" s="18"/>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="19"/>
     </row>
     <row r="46" spans="2:25">
-      <c r="B46" s="35"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="129"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="129"/>
-      <c r="O46" s="132"/>
-      <c r="P46" s="133"/>
-      <c r="Q46" s="133"/>
-      <c r="R46" s="133"/>
-      <c r="S46" s="133"/>
-      <c r="T46" s="134"/>
-      <c r="U46" s="35"/>
-      <c r="V46" s="36"/>
-      <c r="W46" s="36"/>
-      <c r="X46" s="36"/>
-      <c r="Y46" s="37"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="80"/>
+      <c r="M46" s="61"/>
+      <c r="N46" s="80"/>
+      <c r="O46" s="88"/>
+      <c r="P46" s="89"/>
+      <c r="Q46" s="89"/>
+      <c r="R46" s="89"/>
+      <c r="S46" s="89"/>
+      <c r="T46" s="90"/>
+      <c r="U46" s="25"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
+      <c r="Y46" s="27"/>
     </row>
     <row r="47" spans="2:25">
-      <c r="B47" s="38"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="130"/>
-      <c r="L47" s="131"/>
-      <c r="M47" s="130"/>
-      <c r="N47" s="131"/>
-      <c r="O47" s="135"/>
-      <c r="P47" s="136"/>
-      <c r="Q47" s="136"/>
-      <c r="R47" s="136"/>
-      <c r="S47" s="136"/>
-      <c r="T47" s="137"/>
-      <c r="U47" s="38"/>
-      <c r="V47" s="39"/>
-      <c r="W47" s="39"/>
-      <c r="X47" s="39"/>
-      <c r="Y47" s="40"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="81"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="81"/>
+      <c r="N47" s="82"/>
+      <c r="O47" s="91"/>
+      <c r="P47" s="92"/>
+      <c r="Q47" s="92"/>
+      <c r="R47" s="92"/>
+      <c r="S47" s="92"/>
+      <c r="T47" s="93"/>
+      <c r="U47" s="28"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="30"/>
     </row>
     <row r="48" spans="2:25" ht="15" customHeight="1">
-      <c r="B48" s="95" t="s">
+      <c r="B48" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="95"/>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="95"/>
-      <c r="I48" s="95"/>
-      <c r="J48" s="95"/>
-      <c r="K48" s="95"/>
-      <c r="L48" s="95"/>
-      <c r="M48" s="95"/>
-      <c r="N48" s="95"/>
-      <c r="O48" s="95"/>
-      <c r="P48" s="95"/>
-      <c r="Q48" s="95"/>
-      <c r="R48" s="95"/>
-      <c r="S48" s="95"/>
-      <c r="T48" s="95"/>
-      <c r="U48" s="95"/>
-      <c r="V48" s="95"/>
-      <c r="W48" s="95"/>
-      <c r="X48" s="95"/>
-      <c r="Y48" s="95"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="58"/>
+      <c r="R48" s="58"/>
+      <c r="S48" s="58"/>
+      <c r="T48" s="58"/>
+      <c r="U48" s="58"/>
+      <c r="V48" s="58"/>
+      <c r="W48" s="58"/>
+      <c r="X48" s="58"/>
+      <c r="Y48" s="58"/>
     </row>
     <row r="49" spans="2:25" ht="15" customHeight="1">
       <c r="B49" s="10"/>
@@ -4506,16 +4770,16 @@
       <c r="Y49" s="10"/>
     </row>
     <row r="50" spans="2:25" ht="15.75" customHeight="1">
-      <c r="B50" s="68" t="s">
+      <c r="B50" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="68"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="68"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
+      <c r="I50" s="87"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -4526,11 +4790,11 @@
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
-      <c r="T50" s="67"/>
-      <c r="U50" s="68"/>
-      <c r="V50" s="68"/>
-      <c r="W50" s="68"/>
-      <c r="X50" s="68"/>
+      <c r="T50" s="86"/>
+      <c r="U50" s="87"/>
+      <c r="V50" s="87"/>
+      <c r="W50" s="87"/>
+      <c r="X50" s="87"/>
       <c r="Y50" s="10"/>
     </row>
     <row r="51" spans="2:25" ht="23.25" customHeight="1">
@@ -4560,35 +4824,35 @@
       <c r="Y51" s="8"/>
     </row>
     <row r="52" spans="2:25" ht="18" customHeight="1">
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
       <c r="J52" s="11"/>
-      <c r="K52" s="18" t="s">
+      <c r="K52" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
+      <c r="L52" s="47"/>
+      <c r="M52" s="47"/>
+      <c r="N52" s="47"/>
+      <c r="O52" s="47"/>
+      <c r="P52" s="47"/>
+      <c r="Q52" s="47"/>
       <c r="R52" s="13"/>
       <c r="S52" s="11"/>
-      <c r="T52" s="17" t="s">
+      <c r="T52" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="U52" s="17"/>
-      <c r="V52" s="17"/>
-      <c r="W52" s="17"/>
-      <c r="X52" s="17"/>
+      <c r="U52" s="32"/>
+      <c r="V52" s="32"/>
+      <c r="W52" s="32"/>
+      <c r="X52" s="32"/>
       <c r="Y52" s="11"/>
     </row>
     <row r="53" spans="2:25">
@@ -4618,16 +4882,16 @@
       <c r="Y53" s="11"/>
     </row>
     <row r="54" spans="2:25">
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
     </row>
     <row r="55" spans="2:25">
       <c r="B55" s="14"/>
@@ -4656,100 +4920,194 @@
       <c r="Y55" s="12"/>
     </row>
     <row r="56" spans="2:25">
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
       <c r="J56" s="11"/>
-      <c r="K56" s="18" t="s">
+      <c r="K56" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="47"/>
+      <c r="O56" s="47"/>
+      <c r="P56" s="47"/>
+      <c r="Q56" s="47"/>
       <c r="R56" s="13"/>
-      <c r="S56" s="19" t="s">
+      <c r="S56" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="T56" s="20"/>
-      <c r="U56" s="20"/>
-      <c r="V56" s="20"/>
-      <c r="W56" s="20"/>
-      <c r="X56" s="20"/>
-      <c r="Y56" s="20"/>
+      <c r="T56" s="105"/>
+      <c r="U56" s="105"/>
+      <c r="V56" s="105"/>
+      <c r="W56" s="105"/>
+      <c r="X56" s="105"/>
+      <c r="Y56" s="105"/>
     </row>
     <row r="57" spans="2:25">
-      <c r="Q57" s="94"/>
-      <c r="R57" s="94"/>
-      <c r="S57" s="94"/>
-      <c r="T57" s="94"/>
-      <c r="U57" s="94"/>
+      <c r="Q57" s="55"/>
+      <c r="R57" s="55"/>
+      <c r="S57" s="55"/>
+      <c r="T57" s="55"/>
+      <c r="U57" s="55"/>
     </row>
     <row r="58" spans="2:25">
-      <c r="B58" s="73" t="s">
+      <c r="B58" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="73"/>
-      <c r="M58" s="73"/>
-      <c r="N58" s="73"/>
-      <c r="O58" s="73"/>
-      <c r="P58" s="73"/>
-      <c r="Q58" s="73"/>
-      <c r="R58" s="73"/>
-      <c r="S58" s="73"/>
-      <c r="T58" s="73"/>
-      <c r="U58" s="73"/>
-      <c r="V58" s="73"/>
-      <c r="W58" s="73"/>
-      <c r="X58" s="73"/>
-      <c r="Y58" s="73"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31"/>
+      <c r="Q58" s="31"/>
+      <c r="R58" s="31"/>
+      <c r="S58" s="31"/>
+      <c r="T58" s="31"/>
+      <c r="U58" s="31"/>
+      <c r="V58" s="31"/>
+      <c r="W58" s="31"/>
+      <c r="X58" s="31"/>
+      <c r="Y58" s="31"/>
     </row>
     <row r="59" spans="2:25">
-      <c r="B59" s="73"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="73"/>
-      <c r="G59" s="73"/>
-      <c r="H59" s="73"/>
-      <c r="I59" s="73"/>
-      <c r="J59" s="73"/>
-      <c r="K59" s="73"/>
-      <c r="L59" s="73"/>
-      <c r="M59" s="73"/>
-      <c r="N59" s="73"/>
-      <c r="O59" s="73"/>
-      <c r="P59" s="73"/>
-      <c r="Q59" s="73"/>
-      <c r="R59" s="73"/>
-      <c r="S59" s="73"/>
-      <c r="T59" s="73"/>
-      <c r="U59" s="73"/>
-      <c r="V59" s="73"/>
-      <c r="W59" s="73"/>
-      <c r="X59" s="73"/>
-      <c r="Y59" s="73"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
+      <c r="Q59" s="31"/>
+      <c r="R59" s="31"/>
+      <c r="S59" s="31"/>
+      <c r="T59" s="31"/>
+      <c r="U59" s="31"/>
+      <c r="V59" s="31"/>
+      <c r="W59" s="31"/>
+      <c r="X59" s="31"/>
+      <c r="Y59" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="118">
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="K56:Q56"/>
+    <mergeCell ref="S56:Y56"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="T20:Y20"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="B46:J47"/>
+    <mergeCell ref="O46:T47"/>
+    <mergeCell ref="U46:Y47"/>
+    <mergeCell ref="K46:L47"/>
+    <mergeCell ref="O34:T35"/>
+    <mergeCell ref="U34:Y35"/>
+    <mergeCell ref="B38:J39"/>
+    <mergeCell ref="M36:N37"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="M38:N39"/>
+    <mergeCell ref="U36:Y37"/>
+    <mergeCell ref="B36:J37"/>
+    <mergeCell ref="B34:J35"/>
+    <mergeCell ref="O42:T43"/>
+    <mergeCell ref="K23:Y23"/>
+    <mergeCell ref="U25:Y25"/>
+    <mergeCell ref="B26:J27"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="M46:N47"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B30:J31"/>
+    <mergeCell ref="U26:Y27"/>
+    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="O25:T25"/>
+    <mergeCell ref="T50:X50"/>
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O26:T26"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B40:J41"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="O40:T41"/>
+    <mergeCell ref="U40:Y41"/>
+    <mergeCell ref="B42:J43"/>
+    <mergeCell ref="K42:L43"/>
+    <mergeCell ref="M42:N43"/>
+    <mergeCell ref="B48:Y48"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="O36:T37"/>
+    <mergeCell ref="K30:L31"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="K34:L35"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="B8:Y8"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O28:T29"/>
+    <mergeCell ref="U28:Y29"/>
+    <mergeCell ref="O30:T31"/>
+    <mergeCell ref="U30:Y31"/>
     <mergeCell ref="U42:Y43"/>
     <mergeCell ref="B58:Y59"/>
     <mergeCell ref="B54:I54"/>
@@ -4774,100 +5132,6 @@
     <mergeCell ref="U38:Y39"/>
     <mergeCell ref="T52:X52"/>
     <mergeCell ref="U32:Y33"/>
-    <mergeCell ref="B48:Y48"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="O36:T37"/>
-    <mergeCell ref="K30:L31"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="M26:N27"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="K34:L35"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O28:T29"/>
-    <mergeCell ref="U28:Y29"/>
-    <mergeCell ref="O30:T31"/>
-    <mergeCell ref="U30:Y31"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="M46:N47"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B30:J31"/>
-    <mergeCell ref="U26:Y27"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="O25:T25"/>
-    <mergeCell ref="T50:X50"/>
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O26:T26"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B40:J41"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="O40:T41"/>
-    <mergeCell ref="U40:Y41"/>
-    <mergeCell ref="B42:J43"/>
-    <mergeCell ref="K42:L43"/>
-    <mergeCell ref="M42:N43"/>
-    <mergeCell ref="O42:T43"/>
-    <mergeCell ref="K23:Y23"/>
-    <mergeCell ref="U25:Y25"/>
-    <mergeCell ref="B26:J27"/>
-    <mergeCell ref="B6:Y6"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="K56:Q56"/>
-    <mergeCell ref="S56:Y56"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="T19:Y19"/>
-    <mergeCell ref="T20:Y20"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="B46:J47"/>
-    <mergeCell ref="O46:T47"/>
-    <mergeCell ref="U46:Y47"/>
-    <mergeCell ref="K46:L47"/>
-    <mergeCell ref="O34:T35"/>
-    <mergeCell ref="U34:Y35"/>
-    <mergeCell ref="B38:J39"/>
-    <mergeCell ref="M36:N37"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="M38:N39"/>
-    <mergeCell ref="U36:Y37"/>
-    <mergeCell ref="B36:J37"/>
-    <mergeCell ref="B34:J35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T20" r:id="rId1" xr:uid="{BE351EEA-9877-430E-96A9-ADC6513FEEA9}"/>
@@ -4895,124 +5159,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="118"/>
-      <c r="P1" s="118"/>
-      <c r="Q1" s="118"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="118"/>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="118"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="102" t="s">
+      <c r="A2" s="113"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="102"/>
-      <c r="W2" s="102"/>
-      <c r="X2" s="102"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1">
-      <c r="U3" s="125"/>
-      <c r="V3" s="125"/>
-      <c r="W3" s="125"/>
-      <c r="X3" s="125"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="122"/>
+      <c r="X3" s="122"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="122" t="s">
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123"/>
-      <c r="Q4" s="123"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123"/>
-      <c r="V4" s="123"/>
-      <c r="W4" s="123"/>
-      <c r="X4" s="124"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+      <c r="T4" s="119"/>
+      <c r="U4" s="119"/>
+      <c r="V4" s="119"/>
+      <c r="W4" s="119"/>
+      <c r="X4" s="120"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="119"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="121"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="120"/>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="120"/>
-      <c r="S5" s="120"/>
-      <c r="T5" s="120"/>
-      <c r="U5" s="120"/>
-      <c r="V5" s="120"/>
-      <c r="W5" s="120"/>
-      <c r="X5" s="121"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="116"/>
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="117"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A6" s="3"/>
@@ -5041,66 +5305,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100" t="s">
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100" t="s">
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="114"/>
+      <c r="N7" s="114"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="100"/>
-      <c r="W7" s="100"/>
-      <c r="X7" s="100"/>
+      <c r="Q7" s="114"/>
+      <c r="R7" s="114"/>
+      <c r="S7" s="114"/>
+      <c r="T7" s="114"/>
+      <c r="U7" s="114"/>
+      <c r="V7" s="114"/>
+      <c r="W7" s="114"/>
+      <c r="X7" s="114"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1">
-      <c r="A8" s="93"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="107" t="s">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
-      <c r="O8" s="109"/>
-      <c r="P8" s="107" t="s">
+      <c r="K8" s="124"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="124"/>
+      <c r="N8" s="124"/>
+      <c r="O8" s="125"/>
+      <c r="P8" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="108"/>
-      <c r="R8" s="108"/>
-      <c r="S8" s="108"/>
-      <c r="T8" s="108"/>
-      <c r="U8" s="108"/>
-      <c r="V8" s="108"/>
-      <c r="W8" s="108"/>
-      <c r="X8" s="109"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="124"/>
+      <c r="S8" s="124"/>
+      <c r="T8" s="124"/>
+      <c r="U8" s="124"/>
+      <c r="V8" s="124"/>
+      <c r="W8" s="124"/>
+      <c r="X8" s="125"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A9" s="3"/>
@@ -5129,66 +5393,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="79"/>
-      <c r="U10" s="79"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="79"/>
-      <c r="X10" s="79"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="76"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="76"/>
+      <c r="V10" s="76"/>
+      <c r="W10" s="76"/>
+      <c r="X10" s="76"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57" t="s">
+      <c r="B11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57" t="s">
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57" t="s">
+      <c r="N11" s="97"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="97"/>
+      <c r="Q11" s="97"/>
+      <c r="R11" s="97"/>
+      <c r="S11" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
+      <c r="T11" s="97"/>
+      <c r="U11" s="97"/>
+      <c r="V11" s="97"/>
+      <c r="W11" s="97"/>
+      <c r="X11" s="97"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="3"/>
@@ -5217,66 +5481,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100" t="s">
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="100" t="s">
+      <c r="K13" s="114"/>
+      <c r="L13" s="114"/>
+      <c r="M13" s="114"/>
+      <c r="N13" s="114"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="100"/>
-      <c r="S13" s="100"/>
-      <c r="T13" s="100"/>
-      <c r="U13" s="100"/>
-      <c r="V13" s="100"/>
-      <c r="W13" s="100"/>
-      <c r="X13" s="100"/>
+      <c r="Q13" s="114"/>
+      <c r="R13" s="114"/>
+      <c r="S13" s="114"/>
+      <c r="T13" s="114"/>
+      <c r="U13" s="114"/>
+      <c r="V13" s="114"/>
+      <c r="W13" s="114"/>
+      <c r="X13" s="114"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1">
-      <c r="A14" s="93"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="107" t="s">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="108"/>
-      <c r="L14" s="108"/>
-      <c r="M14" s="108"/>
-      <c r="N14" s="108"/>
-      <c r="O14" s="109"/>
-      <c r="P14" s="107" t="s">
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="125"/>
+      <c r="P14" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="108"/>
-      <c r="R14" s="108"/>
-      <c r="S14" s="108"/>
-      <c r="T14" s="108"/>
-      <c r="U14" s="108"/>
-      <c r="V14" s="108"/>
-      <c r="W14" s="108"/>
-      <c r="X14" s="109"/>
+      <c r="Q14" s="124"/>
+      <c r="R14" s="124"/>
+      <c r="S14" s="124"/>
+      <c r="T14" s="124"/>
+      <c r="U14" s="124"/>
+      <c r="V14" s="124"/>
+      <c r="W14" s="124"/>
+      <c r="X14" s="125"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A15" s="3"/>
@@ -5305,184 +5569,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="110" t="s">
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="110"/>
-      <c r="L16" s="110"/>
-      <c r="M16" s="110"/>
-      <c r="N16" s="17" t="s">
+      <c r="K16" s="131"/>
+      <c r="L16" s="131"/>
+      <c r="M16" s="131"/>
+      <c r="N16" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="111" t="s">
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="111"/>
-      <c r="V16" s="111"/>
-      <c r="W16" s="111"/>
-      <c r="X16" s="111"/>
+      <c r="U16" s="132"/>
+      <c r="V16" s="132"/>
+      <c r="W16" s="132"/>
+      <c r="X16" s="132"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="102"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="112" t="s">
+      <c r="B17" s="121"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="114"/>
-      <c r="N17" s="101" t="s">
+      <c r="K17" s="134"/>
+      <c r="L17" s="134"/>
+      <c r="M17" s="135"/>
+      <c r="N17" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="102"/>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="103"/>
-      <c r="T17" s="101" t="s">
+      <c r="O17" s="121"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="121"/>
+      <c r="R17" s="121"/>
+      <c r="S17" s="127"/>
+      <c r="T17" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="102"/>
-      <c r="V17" s="102"/>
-      <c r="W17" s="102"/>
-      <c r="X17" s="103"/>
+      <c r="U17" s="121"/>
+      <c r="V17" s="121"/>
+      <c r="W17" s="121"/>
+      <c r="X17" s="127"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A18" s="104"/>
-      <c r="B18" s="105"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="115"/>
-      <c r="K18" s="116"/>
-      <c r="L18" s="116"/>
-      <c r="M18" s="117"/>
-      <c r="N18" s="104"/>
-      <c r="O18" s="105"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="106"/>
-      <c r="T18" s="104"/>
-      <c r="U18" s="105"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="105"/>
-      <c r="X18" s="106"/>
+      <c r="A18" s="128"/>
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
+      <c r="D18" s="129"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="129"/>
+      <c r="G18" s="129"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="130"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="128"/>
+      <c r="O18" s="129"/>
+      <c r="P18" s="129"/>
+      <c r="Q18" s="129"/>
+      <c r="R18" s="129"/>
+      <c r="S18" s="130"/>
+      <c r="T18" s="128"/>
+      <c r="U18" s="129"/>
+      <c r="V18" s="129"/>
+      <c r="W18" s="129"/>
+      <c r="X18" s="130"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1"/>
     <row r="20" spans="1:24" ht="39" customHeight="1"/>
     <row r="21" spans="1:24">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="142" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
+      <c r="B21" s="142"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="142"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="142"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="99" t="s">
+      <c r="J21" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="99"/>
-      <c r="L21" s="99"/>
-      <c r="M21" s="99"/>
-      <c r="N21" s="99"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="99"/>
+      <c r="K21" s="142"/>
+      <c r="L21" s="142"/>
+      <c r="M21" s="142"/>
+      <c r="N21" s="142"/>
+      <c r="O21" s="142"/>
+      <c r="P21" s="142"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="99" t="s">
+      <c r="R21" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="99"/>
-      <c r="T21" s="99"/>
-      <c r="U21" s="99"/>
-      <c r="V21" s="99"/>
-      <c r="W21" s="99"/>
-      <c r="X21" s="99"/>
+      <c r="S21" s="142"/>
+      <c r="T21" s="142"/>
+      <c r="U21" s="142"/>
+      <c r="V21" s="142"/>
+      <c r="W21" s="142"/>
+      <c r="X21" s="142"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P23" s="96" t="s">
+      <c r="P23" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-      <c r="S23" s="96"/>
-      <c r="T23" s="96"/>
-      <c r="U23" s="97" t="s">
+      <c r="Q23" s="139"/>
+      <c r="R23" s="139"/>
+      <c r="S23" s="139"/>
+      <c r="T23" s="139"/>
+      <c r="U23" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="97"/>
-      <c r="W23" s="97"/>
-      <c r="X23" s="97"/>
+      <c r="V23" s="140"/>
+      <c r="W23" s="140"/>
+      <c r="X23" s="140"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P24" s="96" t="s">
+      <c r="P24" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="96"/>
-      <c r="S24" s="96"/>
-      <c r="T24" s="96"/>
-      <c r="U24" s="98" t="s">
+      <c r="Q24" s="139"/>
+      <c r="R24" s="139"/>
+      <c r="S24" s="139"/>
+      <c r="T24" s="139"/>
+      <c r="U24" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="98"/>
-      <c r="W24" s="98"/>
-      <c r="X24" s="98"/>
+      <c r="V24" s="141"/>
+      <c r="W24" s="141"/>
+      <c r="X24" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -5497,13 +5749,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
carusel de imagenes pt 1
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
+++ b/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\pruebas\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A83269-7906-48EA-9082-55AADF3C2E4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82399CFC-707D-4D43-91DF-C9C8E5502F19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="98">
   <si>
     <t>BITÁCORA DE SEGUIMIENTO ETAPA PRODUCTIVA</t>
   </si>
@@ -364,6 +364,15 @@
   </si>
   <si>
     <t>falle al intentar optimizar la imagenn</t>
+  </si>
+  <si>
+    <t>29/02/2025</t>
+  </si>
+  <si>
+    <t>cree un carusel de imágenes, es compatible para deslizrlo en moviles, ademas de que lo incorpore a la pagina ala vercion de movil, pero no tuve tiempo para agregar lo botodes de adelantar y retroceder</t>
+  </si>
+  <si>
+    <t>fue un infierno, tenia 2 caminos el caruse con desbanecimiento pero sin se scroleable o este, y la verdad mordi mas de lo que podia masticar pero quedo mas oh menos sinseramente no me comvense las dimenciones de las imágenes de muestra</t>
   </si>
 </sst>
 </file>
@@ -754,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -804,29 +813,59 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -846,14 +885,150 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -861,20 +1036,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -894,24 +1060,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -921,181 +1075,75 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1114,71 +1162,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2888,6 +2909,106 @@
         <a:xfrm>
           <a:off x="7065066" y="50943341"/>
           <a:ext cx="1002196" cy="444610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>41415</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>216050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>339588</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1053616</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Imagen 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59B8E034-E92B-4AB3-8C4D-61A2337E4431}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5830958" y="55543876"/>
+          <a:ext cx="2310847" cy="837566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>107673</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1138979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>339585</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>2281944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Imagen 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607E6143-346D-4A76-927A-1AC73418DE36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6278216" y="56466805"/>
+          <a:ext cx="1383195" cy="3097661"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3308,8 +3429,8 @@
   </sheetPr>
   <dimension ref="B1:AA59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="U42" sqref="U42:Y43"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="U44" sqref="U44:Y45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
@@ -3334,294 +3455,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B1" s="66"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="59" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
     </row>
     <row r="2" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B2" s="66"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="65" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
     </row>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="71"/>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="71"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
     </row>
     <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="71"/>
-      <c r="V4" s="71"/>
-      <c r="W4" s="71"/>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
     </row>
     <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="74"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="62"/>
+      <c r="Y5" s="63"/>
     </row>
     <row r="6" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
-      <c r="T6" s="73"/>
-      <c r="U6" s="73"/>
-      <c r="V6" s="73"/>
-      <c r="W6" s="73"/>
-      <c r="X6" s="73"/>
-      <c r="Y6" s="74"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="63"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1">
-      <c r="B8" s="47"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="75"/>
-      <c r="V8" s="75"/>
-      <c r="W8" s="75"/>
-      <c r="X8" s="75"/>
-      <c r="Y8" s="75"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
+      <c r="X8" s="88"/>
+      <c r="Y8" s="88"/>
     </row>
     <row r="9" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="83" t="s">
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="111"/>
-      <c r="R9" s="111"/>
-      <c r="S9" s="112"/>
-      <c r="T9" s="36" t="s">
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="36" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="83">
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="30">
         <v>5</v>
       </c>
-      <c r="Q10" s="111"/>
-      <c r="R10" s="111"/>
-      <c r="S10" s="112"/>
-      <c r="T10" s="97" t="s">
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="97"/>
-      <c r="V10" s="97"/>
-      <c r="W10" s="97"/>
-      <c r="X10" s="97"/>
-      <c r="Y10" s="97"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B11" s="3"/>
@@ -3650,68 +3771,68 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="98" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="98"/>
-      <c r="P12" s="98"/>
-      <c r="Q12" s="98" t="s">
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="98"/>
-      <c r="S12" s="98"/>
-      <c r="T12" s="98"/>
-      <c r="U12" s="98"/>
-      <c r="V12" s="98"/>
-      <c r="W12" s="98"/>
-      <c r="X12" s="98"/>
-      <c r="Y12" s="98"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="67"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="67"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1">
-      <c r="B13" s="100">
+      <c r="B13" s="72">
         <v>3177294629</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="56">
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="51">
         <v>3177294629</v>
       </c>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="99" t="s">
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="97"/>
-      <c r="S13" s="97"/>
-      <c r="T13" s="97"/>
-      <c r="U13" s="97"/>
-      <c r="V13" s="97"/>
-      <c r="W13" s="97"/>
-      <c r="X13" s="97"/>
-      <c r="Y13" s="97"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="66"/>
+      <c r="V13" s="66"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="66"/>
+      <c r="Y13" s="66"/>
     </row>
     <row r="14" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B14" s="3"/>
@@ -3740,100 +3861,100 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="76"/>
-      <c r="U15" s="76"/>
-      <c r="V15" s="76"/>
-      <c r="W15" s="76"/>
-      <c r="X15" s="76"/>
-      <c r="Y15" s="76"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="89"/>
+      <c r="P15" s="89"/>
+      <c r="Q15" s="89"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="89"/>
+      <c r="T15" s="89"/>
+      <c r="U15" s="89"/>
+      <c r="V15" s="89"/>
+      <c r="W15" s="89"/>
+      <c r="X15" s="89"/>
+      <c r="Y15" s="89"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="40" t="s">
+      <c r="C16" s="64"/>
+      <c r="D16" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="38" t="s">
+      <c r="F16" s="64"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41" t="s">
+      <c r="I16" s="64"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="42"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="38" t="s">
+      <c r="L16" s="95"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="65"/>
+      <c r="O16" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="40"/>
-      <c r="S16" s="38" t="s">
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="38"/>
-      <c r="U16" s="40"/>
-      <c r="V16" s="38" t="s">
+      <c r="T16" s="64"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="40"/>
+      <c r="W16" s="64"/>
+      <c r="X16" s="64"/>
+      <c r="Y16" s="65"/>
     </row>
     <row r="17" spans="2:27" ht="45.75" customHeight="1">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="40"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="99"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="64"/>
+      <c r="T17" s="64"/>
+      <c r="U17" s="65"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="64"/>
+      <c r="X17" s="64"/>
+      <c r="Y17" s="65"/>
     </row>
     <row r="18" spans="2:27" ht="9.9499999999999993" customHeight="1">
       <c r="B18" s="3"/>
@@ -3862,72 +3983,72 @@
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="2:27" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="51" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="51" t="s">
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="52"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="33" t="s">
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="48"/>
-      <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
-      <c r="X19" s="48"/>
-      <c r="Y19" s="108"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="27"/>
     </row>
     <row r="20" spans="2:27" ht="18" customHeight="1">
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="53">
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="101"/>
+      <c r="J20" s="102">
         <v>1096800316</v>
       </c>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="106">
+      <c r="K20" s="103"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="23">
         <v>3219713759</v>
       </c>
-      <c r="P20" s="107"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="107"/>
-      <c r="S20" s="107"/>
-      <c r="T20" s="109" t="s">
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="U20" s="110"/>
-      <c r="V20" s="110"/>
-      <c r="W20" s="110"/>
-      <c r="X20" s="110"/>
-      <c r="Y20" s="108"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="27"/>
     </row>
     <row r="21" spans="2:27" ht="9.75" customHeight="1">
       <c r="B21" s="8"/>
@@ -3956,64 +4077,64 @@
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="2:27" ht="18" customHeight="1">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="36" t="s">
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="92"/>
+      <c r="R22" s="92"/>
+      <c r="S22" s="92"/>
+      <c r="T22" s="92"/>
+      <c r="U22" s="92"/>
+      <c r="V22" s="92"/>
+      <c r="W22" s="92"/>
+      <c r="X22" s="92"/>
+      <c r="Y22" s="92"/>
     </row>
     <row r="23" spans="2:27" ht="18" customHeight="1">
-      <c r="B23" s="77">
+      <c r="B23" s="69">
         <v>2557356</v>
       </c>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="94" t="s">
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
-      <c r="P23" s="95"/>
-      <c r="Q23" s="95"/>
-      <c r="R23" s="95"/>
-      <c r="S23" s="95"/>
-      <c r="T23" s="95"/>
-      <c r="U23" s="95"/>
-      <c r="V23" s="95"/>
-      <c r="W23" s="95"/>
-      <c r="X23" s="95"/>
-      <c r="Y23" s="96"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="58"/>
     </row>
     <row r="24" spans="2:27" ht="9.75" customHeight="1">
       <c r="B24" s="3"/>
@@ -4042,706 +4163,722 @@
       <c r="Y24" s="3"/>
     </row>
     <row r="25" spans="2:27" ht="48" customHeight="1">
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="83" t="s">
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="84"/>
-      <c r="M25" s="83" t="s">
+      <c r="L25" s="59"/>
+      <c r="M25" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="84"/>
-      <c r="O25" s="83" t="s">
+      <c r="N25" s="59"/>
+      <c r="O25" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="84"/>
-      <c r="Q25" s="84"/>
-      <c r="R25" s="84"/>
-      <c r="S25" s="84"/>
-      <c r="T25" s="85"/>
-      <c r="U25" s="83" t="s">
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="84"/>
-      <c r="W25" s="84"/>
-      <c r="X25" s="84"/>
-      <c r="Y25" s="85"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="60"/>
     </row>
     <row r="26" spans="2:27" ht="216" customHeight="1">
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="61">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="47">
         <v>45705</v>
       </c>
-      <c r="L26" s="62"/>
-      <c r="M26" s="61">
+      <c r="L26" s="53"/>
+      <c r="M26" s="47">
         <v>45706</v>
       </c>
-      <c r="N26" s="62"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="78"/>
-      <c r="Q26" s="78"/>
-      <c r="R26" s="78"/>
-      <c r="S26" s="78"/>
-      <c r="T26" s="79"/>
-      <c r="U26" s="57" t="s">
+      <c r="N26" s="53"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="70"/>
+      <c r="Q26" s="70"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="V26" s="57"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="57"/>
+      <c r="V26" s="52"/>
+      <c r="W26" s="52"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="52"/>
     </row>
     <row r="27" spans="2:27" ht="232.5" customHeight="1">
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="77"/>
-      <c r="P27" s="78"/>
-      <c r="Q27" s="78"/>
-      <c r="R27" s="78"/>
-      <c r="S27" s="78"/>
-      <c r="T27" s="79"/>
-      <c r="U27" s="57"/>
-      <c r="V27" s="57"/>
-      <c r="W27" s="57"/>
-      <c r="X27" s="57"/>
-      <c r="Y27" s="57"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="70"/>
+      <c r="R27" s="70"/>
+      <c r="S27" s="70"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="52"/>
     </row>
     <row r="28" spans="2:27" ht="126.75" customHeight="1">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="61">
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="47">
         <v>45706</v>
       </c>
-      <c r="L28" s="62"/>
-      <c r="M28" s="61">
+      <c r="L28" s="53"/>
+      <c r="M28" s="47">
         <v>45707</v>
       </c>
-      <c r="N28" s="62"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="57" t="s">
+      <c r="N28" s="53"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="V28" s="57"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="57"/>
-      <c r="Y28" s="57"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
     </row>
     <row r="29" spans="2:27" ht="189" customHeight="1">
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="57"/>
-      <c r="V29" s="57"/>
-      <c r="W29" s="57"/>
-      <c r="X29" s="57"/>
-      <c r="Y29" s="57"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="52"/>
+      <c r="V29" s="52"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="52"/>
       <c r="AA29" s="16"/>
     </row>
     <row r="30" spans="2:27" ht="105" customHeight="1">
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="61">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="47">
         <v>45707</v>
       </c>
-      <c r="L30" s="62"/>
-      <c r="M30" s="61">
+      <c r="L30" s="53"/>
+      <c r="M30" s="47">
         <v>45708</v>
       </c>
-      <c r="N30" s="62"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="56"/>
-      <c r="U30" s="57" t="s">
+      <c r="N30" s="53"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="V30" s="57"/>
-      <c r="W30" s="57"/>
-      <c r="X30" s="57"/>
-      <c r="Y30" s="57"/>
+      <c r="V30" s="52"/>
+      <c r="W30" s="52"/>
+      <c r="X30" s="52"/>
+      <c r="Y30" s="52"/>
     </row>
     <row r="31" spans="2:27" ht="180.75" customHeight="1">
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="57"/>
-      <c r="V31" s="57"/>
-      <c r="W31" s="57"/>
-      <c r="X31" s="57"/>
-      <c r="Y31" s="57"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="52"/>
+      <c r="V31" s="52"/>
+      <c r="W31" s="52"/>
+      <c r="X31" s="52"/>
+      <c r="Y31" s="52"/>
       <c r="AA31" s="16"/>
     </row>
     <row r="32" spans="2:27" ht="280.5" customHeight="1">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="61">
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="47">
         <v>45708</v>
       </c>
-      <c r="L32" s="62"/>
-      <c r="M32" s="61">
+      <c r="L32" s="53"/>
+      <c r="M32" s="47">
         <v>45709</v>
       </c>
-      <c r="N32" s="62"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="56"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="56"/>
-      <c r="U32" s="57" t="s">
+      <c r="N32" s="53"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="51"/>
+      <c r="S32" s="51"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="V32" s="57"/>
-      <c r="W32" s="57"/>
-      <c r="X32" s="57"/>
-      <c r="Y32" s="57"/>
+      <c r="V32" s="52"/>
+      <c r="W32" s="52"/>
+      <c r="X32" s="52"/>
+      <c r="Y32" s="52"/>
     </row>
     <row r="33" spans="2:25" ht="259.5" customHeight="1">
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="56"/>
-      <c r="S33" s="56"/>
-      <c r="T33" s="56"/>
-      <c r="U33" s="57"/>
-      <c r="V33" s="57"/>
-      <c r="W33" s="57"/>
-      <c r="X33" s="57"/>
-      <c r="Y33" s="57"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="52"/>
+      <c r="V33" s="52"/>
+      <c r="W33" s="52"/>
+      <c r="X33" s="52"/>
+      <c r="Y33" s="52"/>
     </row>
     <row r="34" spans="2:25" ht="295.5" customHeight="1">
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="61">
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="47">
         <v>45709</v>
       </c>
-      <c r="L34" s="62"/>
-      <c r="M34" s="61">
+      <c r="L34" s="53"/>
+      <c r="M34" s="47">
         <v>45710</v>
       </c>
-      <c r="N34" s="62"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="56"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="56"/>
-      <c r="U34" s="57" t="s">
+      <c r="N34" s="53"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="51"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="V34" s="57"/>
-      <c r="W34" s="57"/>
-      <c r="X34" s="57"/>
-      <c r="Y34" s="57"/>
+      <c r="V34" s="52"/>
+      <c r="W34" s="52"/>
+      <c r="X34" s="52"/>
+      <c r="Y34" s="52"/>
     </row>
     <row r="35" spans="2:25" ht="265.5" customHeight="1">
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="63"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="64"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="56"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
-      <c r="U35" s="57"/>
-      <c r="V35" s="57"/>
-      <c r="W35" s="57"/>
-      <c r="X35" s="57"/>
-      <c r="Y35" s="57"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="54"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="54"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
+      <c r="W35" s="52"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="52"/>
     </row>
     <row r="36" spans="2:25" ht="249.75" customHeight="1">
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="61">
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="47">
         <v>45712</v>
       </c>
-      <c r="L36" s="62"/>
-      <c r="M36" s="61">
+      <c r="L36" s="53"/>
+      <c r="M36" s="47">
         <v>45713</v>
       </c>
-      <c r="N36" s="62"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="57" t="s">
+      <c r="N36" s="53"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="V36" s="57"/>
-      <c r="W36" s="57"/>
-      <c r="X36" s="57"/>
-      <c r="Y36" s="57"/>
+      <c r="V36" s="52"/>
+      <c r="W36" s="52"/>
+      <c r="X36" s="52"/>
+      <c r="Y36" s="52"/>
     </row>
     <row r="37" spans="2:25" ht="211.5" customHeight="1">
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="64"/>
-      <c r="M37" s="63"/>
-      <c r="N37" s="64"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="56"/>
-      <c r="T37" s="56"/>
-      <c r="U37" s="57"/>
-      <c r="V37" s="57"/>
-      <c r="W37" s="57"/>
-      <c r="X37" s="57"/>
-      <c r="Y37" s="57"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="52"/>
+      <c r="V37" s="52"/>
+      <c r="W37" s="52"/>
+      <c r="X37" s="52"/>
+      <c r="Y37" s="52"/>
     </row>
     <row r="38" spans="2:25" ht="182.25" customHeight="1">
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="61">
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="47">
         <v>45713</v>
       </c>
-      <c r="L38" s="62"/>
-      <c r="M38" s="61">
+      <c r="L38" s="53"/>
+      <c r="M38" s="47">
         <v>45714</v>
       </c>
-      <c r="N38" s="62"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
-      <c r="S38" s="56"/>
-      <c r="T38" s="56"/>
-      <c r="U38" s="57" t="s">
+      <c r="N38" s="53"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="V38" s="57"/>
-      <c r="W38" s="57"/>
-      <c r="X38" s="57"/>
-      <c r="Y38" s="57"/>
+      <c r="V38" s="52"/>
+      <c r="W38" s="52"/>
+      <c r="X38" s="52"/>
+      <c r="Y38" s="52"/>
     </row>
     <row r="39" spans="2:25" ht="165.75" customHeight="1">
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="63"/>
-      <c r="N39" s="64"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
-      <c r="T39" s="56"/>
-      <c r="U39" s="57"/>
-      <c r="V39" s="57"/>
-      <c r="W39" s="57"/>
-      <c r="X39" s="57"/>
-      <c r="Y39" s="57"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="54"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="52"/>
+      <c r="V39" s="52"/>
+      <c r="W39" s="52"/>
+      <c r="X39" s="52"/>
+      <c r="Y39" s="52"/>
     </row>
     <row r="40" spans="2:25" ht="219.75" customHeight="1">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="80"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="88"/>
-      <c r="P40" s="89"/>
-      <c r="Q40" s="89"/>
-      <c r="R40" s="89"/>
-      <c r="S40" s="89"/>
-      <c r="T40" s="90"/>
-      <c r="U40" s="25" t="s">
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="47">
+        <v>45714</v>
+      </c>
+      <c r="L40" s="53"/>
+      <c r="M40" s="47">
+        <v>45715</v>
+      </c>
+      <c r="N40" s="53"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="43"/>
+      <c r="U40" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="V40" s="26"/>
-      <c r="W40" s="26"/>
-      <c r="X40" s="26"/>
-      <c r="Y40" s="27"/>
+      <c r="V40" s="36"/>
+      <c r="W40" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="Y40" s="37"/>
     </row>
     <row r="41" spans="2:25" ht="153" customHeight="1">
-      <c r="B41" s="28"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="81"/>
-      <c r="L41" s="82"/>
-      <c r="M41" s="81"/>
-      <c r="N41" s="82"/>
-      <c r="O41" s="91"/>
-      <c r="P41" s="92"/>
-      <c r="Q41" s="92"/>
-      <c r="R41" s="92"/>
-      <c r="S41" s="92"/>
-      <c r="T41" s="93"/>
-      <c r="U41" s="28"/>
-      <c r="V41" s="29"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="30"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="54"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="45"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
+      <c r="S41" s="45"/>
+      <c r="T41" s="46"/>
+      <c r="U41" s="38"/>
+      <c r="V41" s="39"/>
+      <c r="W41" s="39"/>
+      <c r="X41" s="39"/>
+      <c r="Y41" s="40"/>
     </row>
     <row r="42" spans="2:25" ht="261.75" customHeight="1">
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="80"/>
-      <c r="M42" s="61"/>
-      <c r="N42" s="80"/>
-      <c r="O42" s="88"/>
-      <c r="P42" s="89"/>
-      <c r="Q42" s="89"/>
-      <c r="R42" s="89"/>
-      <c r="S42" s="89"/>
-      <c r="T42" s="90"/>
-      <c r="U42" s="25" t="s">
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="47">
+        <v>45715</v>
+      </c>
+      <c r="L42" s="53"/>
+      <c r="M42" s="47">
+        <v>45716</v>
+      </c>
+      <c r="N42" s="53"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="V42" s="26"/>
-      <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
-      <c r="Y42" s="27"/>
+      <c r="V42" s="36"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="Y42" s="37"/>
     </row>
     <row r="43" spans="2:25" ht="204" customHeight="1">
-      <c r="B43" s="28"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="81"/>
-      <c r="L43" s="82"/>
-      <c r="M43" s="81"/>
-      <c r="N43" s="82"/>
-      <c r="O43" s="91"/>
-      <c r="P43" s="92"/>
-      <c r="Q43" s="92"/>
-      <c r="R43" s="92"/>
-      <c r="S43" s="92"/>
-      <c r="T43" s="93"/>
-      <c r="U43" s="28"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="30"/>
-    </row>
-    <row r="44" spans="2:25" ht="15" customHeight="1">
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="24"/>
-      <c r="U44" s="17"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="19"/>
-    </row>
-    <row r="45" spans="2:25" ht="15" customHeight="1">
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="21"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="21"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="24"/>
-      <c r="U45" s="17"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="19"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="54"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="55"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="45"/>
+      <c r="T43" s="46"/>
+      <c r="U43" s="38"/>
+      <c r="V43" s="39"/>
+      <c r="W43" s="39"/>
+      <c r="X43" s="39"/>
+      <c r="Y43" s="40"/>
+    </row>
+    <row r="44" spans="2:25" ht="153.75" customHeight="1">
+      <c r="B44" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="136"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="136"/>
+      <c r="G44" s="136"/>
+      <c r="H44" s="136"/>
+      <c r="I44" s="136"/>
+      <c r="J44" s="137"/>
+      <c r="K44" s="47">
+        <v>45716</v>
+      </c>
+      <c r="L44" s="53"/>
+      <c r="M44" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="N44" s="53"/>
+      <c r="O44" s="141"/>
+      <c r="P44" s="142"/>
+      <c r="Q44" s="142"/>
+      <c r="R44" s="142"/>
+      <c r="S44" s="142"/>
+      <c r="T44" s="143"/>
+      <c r="U44" s="135" t="s">
+        <v>97</v>
+      </c>
+      <c r="V44" s="136"/>
+      <c r="W44" s="136"/>
+      <c r="X44" s="136"/>
+      <c r="Y44" s="137"/>
+    </row>
+    <row r="45" spans="2:25" ht="195.75" customHeight="1">
+      <c r="B45" s="138"/>
+      <c r="C45" s="139"/>
+      <c r="D45" s="139"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="139"/>
+      <c r="G45" s="139"/>
+      <c r="H45" s="139"/>
+      <c r="I45" s="139"/>
+      <c r="J45" s="140"/>
+      <c r="K45" s="54"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="54"/>
+      <c r="N45" s="55"/>
+      <c r="O45" s="144"/>
+      <c r="P45" s="145"/>
+      <c r="Q45" s="145"/>
+      <c r="R45" s="145"/>
+      <c r="S45" s="145"/>
+      <c r="T45" s="146"/>
+      <c r="U45" s="138"/>
+      <c r="V45" s="139"/>
+      <c r="W45" s="139"/>
+      <c r="X45" s="139"/>
+      <c r="Y45" s="140"/>
     </row>
     <row r="46" spans="2:25">
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="80"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="88"/>
-      <c r="P46" s="89"/>
-      <c r="Q46" s="89"/>
-      <c r="R46" s="89"/>
-      <c r="S46" s="89"/>
-      <c r="T46" s="90"/>
-      <c r="U46" s="25"/>
-      <c r="V46" s="26"/>
-      <c r="W46" s="26"/>
-      <c r="X46" s="26"/>
-      <c r="Y46" s="27"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="41"/>
+      <c r="P46" s="42"/>
+      <c r="Q46" s="42"/>
+      <c r="R46" s="42"/>
+      <c r="S46" s="42"/>
+      <c r="T46" s="43"/>
+      <c r="U46" s="35"/>
+      <c r="V46" s="36"/>
+      <c r="W46" s="36"/>
+      <c r="X46" s="36"/>
+      <c r="Y46" s="37"/>
     </row>
     <row r="47" spans="2:25">
-      <c r="B47" s="28"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="81"/>
-      <c r="L47" s="82"/>
-      <c r="M47" s="81"/>
-      <c r="N47" s="82"/>
-      <c r="O47" s="91"/>
-      <c r="P47" s="92"/>
-      <c r="Q47" s="92"/>
-      <c r="R47" s="92"/>
-      <c r="S47" s="92"/>
-      <c r="T47" s="93"/>
-      <c r="U47" s="28"/>
-      <c r="V47" s="29"/>
-      <c r="W47" s="29"/>
-      <c r="X47" s="29"/>
-      <c r="Y47" s="30"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="44"/>
+      <c r="P47" s="45"/>
+      <c r="Q47" s="45"/>
+      <c r="R47" s="45"/>
+      <c r="S47" s="45"/>
+      <c r="T47" s="46"/>
+      <c r="U47" s="38"/>
+      <c r="V47" s="39"/>
+      <c r="W47" s="39"/>
+      <c r="X47" s="39"/>
+      <c r="Y47" s="40"/>
     </row>
     <row r="48" spans="2:25" ht="15" customHeight="1">
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="58"/>
-      <c r="P48" s="58"/>
-      <c r="Q48" s="58"/>
-      <c r="R48" s="58"/>
-      <c r="S48" s="58"/>
-      <c r="T48" s="58"/>
-      <c r="U48" s="58"/>
-      <c r="V48" s="58"/>
-      <c r="W48" s="58"/>
-      <c r="X48" s="58"/>
-      <c r="Y48" s="58"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="78"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="78"/>
+      <c r="O48" s="78"/>
+      <c r="P48" s="78"/>
+      <c r="Q48" s="78"/>
+      <c r="R48" s="78"/>
+      <c r="S48" s="78"/>
+      <c r="T48" s="78"/>
+      <c r="U48" s="78"/>
+      <c r="V48" s="78"/>
+      <c r="W48" s="78"/>
+      <c r="X48" s="78"/>
+      <c r="Y48" s="78"/>
     </row>
     <row r="49" spans="2:25" ht="15" customHeight="1">
       <c r="B49" s="10"/>
@@ -4770,16 +4907,16 @@
       <c r="Y49" s="10"/>
     </row>
     <row r="50" spans="2:25" ht="15.75" customHeight="1">
-      <c r="B50" s="87" t="s">
+      <c r="B50" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="87"/>
-      <c r="D50" s="87"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="87"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="87"/>
-      <c r="I50" s="87"/>
+      <c r="C50" s="77"/>
+      <c r="D50" s="77"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="77"/>
+      <c r="H50" s="77"/>
+      <c r="I50" s="77"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -4790,11 +4927,11 @@
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
-      <c r="T50" s="86"/>
-      <c r="U50" s="87"/>
-      <c r="V50" s="87"/>
-      <c r="W50" s="87"/>
-      <c r="X50" s="87"/>
+      <c r="T50" s="76"/>
+      <c r="U50" s="77"/>
+      <c r="V50" s="77"/>
+      <c r="W50" s="77"/>
+      <c r="X50" s="77"/>
       <c r="Y50" s="10"/>
     </row>
     <row r="51" spans="2:25" ht="23.25" customHeight="1">
@@ -4824,35 +4961,35 @@
       <c r="Y51" s="8"/>
     </row>
     <row r="52" spans="2:25" ht="18" customHeight="1">
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
       <c r="J52" s="11"/>
-      <c r="K52" s="47" t="s">
+      <c r="K52" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L52" s="47"/>
-      <c r="M52" s="47"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="47"/>
-      <c r="Q52" s="47"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
       <c r="R52" s="13"/>
       <c r="S52" s="11"/>
-      <c r="T52" s="32" t="s">
+      <c r="T52" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="U52" s="32"/>
-      <c r="V52" s="32"/>
-      <c r="W52" s="32"/>
-      <c r="X52" s="32"/>
+      <c r="U52" s="17"/>
+      <c r="V52" s="17"/>
+      <c r="W52" s="17"/>
+      <c r="X52" s="17"/>
       <c r="Y52" s="11"/>
     </row>
     <row r="53" spans="2:25">
@@ -4882,16 +5019,16 @@
       <c r="Y53" s="11"/>
     </row>
     <row r="54" spans="2:25">
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
     </row>
     <row r="55" spans="2:25">
       <c r="B55" s="14"/>
@@ -4920,100 +5057,199 @@
       <c r="Y55" s="12"/>
     </row>
     <row r="56" spans="2:25">
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
       <c r="J56" s="11"/>
-      <c r="K56" s="47" t="s">
+      <c r="K56" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="L56" s="47"/>
-      <c r="M56" s="47"/>
-      <c r="N56" s="47"/>
-      <c r="O56" s="47"/>
-      <c r="P56" s="47"/>
-      <c r="Q56" s="47"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
       <c r="R56" s="13"/>
-      <c r="S56" s="104" t="s">
+      <c r="S56" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="T56" s="105"/>
-      <c r="U56" s="105"/>
-      <c r="V56" s="105"/>
-      <c r="W56" s="105"/>
-      <c r="X56" s="105"/>
-      <c r="Y56" s="105"/>
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="20"/>
+      <c r="X56" s="20"/>
+      <c r="Y56" s="20"/>
     </row>
     <row r="57" spans="2:25">
-      <c r="Q57" s="55"/>
-      <c r="R57" s="55"/>
-      <c r="S57" s="55"/>
-      <c r="T57" s="55"/>
-      <c r="U57" s="55"/>
+      <c r="Q57" s="104"/>
+      <c r="R57" s="104"/>
+      <c r="S57" s="104"/>
+      <c r="T57" s="104"/>
+      <c r="U57" s="104"/>
     </row>
     <row r="58" spans="2:25">
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-      <c r="J58" s="31"/>
-      <c r="K58" s="31"/>
-      <c r="L58" s="31"/>
-      <c r="M58" s="31"/>
-      <c r="N58" s="31"/>
-      <c r="O58" s="31"/>
-      <c r="P58" s="31"/>
-      <c r="Q58" s="31"/>
-      <c r="R58" s="31"/>
-      <c r="S58" s="31"/>
-      <c r="T58" s="31"/>
-      <c r="U58" s="31"/>
-      <c r="V58" s="31"/>
-      <c r="W58" s="31"/>
-      <c r="X58" s="31"/>
-      <c r="Y58" s="31"/>
+      <c r="C58" s="83"/>
+      <c r="D58" s="83"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="83"/>
+      <c r="H58" s="83"/>
+      <c r="I58" s="83"/>
+      <c r="J58" s="83"/>
+      <c r="K58" s="83"/>
+      <c r="L58" s="83"/>
+      <c r="M58" s="83"/>
+      <c r="N58" s="83"/>
+      <c r="O58" s="83"/>
+      <c r="P58" s="83"/>
+      <c r="Q58" s="83"/>
+      <c r="R58" s="83"/>
+      <c r="S58" s="83"/>
+      <c r="T58" s="83"/>
+      <c r="U58" s="83"/>
+      <c r="V58" s="83"/>
+      <c r="W58" s="83"/>
+      <c r="X58" s="83"/>
+      <c r="Y58" s="83"/>
     </row>
     <row r="59" spans="2:25">
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="31"/>
-      <c r="L59" s="31"/>
-      <c r="M59" s="31"/>
-      <c r="N59" s="31"/>
-      <c r="O59" s="31"/>
-      <c r="P59" s="31"/>
-      <c r="Q59" s="31"/>
-      <c r="R59" s="31"/>
-      <c r="S59" s="31"/>
-      <c r="T59" s="31"/>
-      <c r="U59" s="31"/>
-      <c r="V59" s="31"/>
-      <c r="W59" s="31"/>
-      <c r="X59" s="31"/>
-      <c r="Y59" s="31"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="83"/>
+      <c r="E59" s="83"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="83"/>
+      <c r="I59" s="83"/>
+      <c r="J59" s="83"/>
+      <c r="K59" s="83"/>
+      <c r="L59" s="83"/>
+      <c r="M59" s="83"/>
+      <c r="N59" s="83"/>
+      <c r="O59" s="83"/>
+      <c r="P59" s="83"/>
+      <c r="Q59" s="83"/>
+      <c r="R59" s="83"/>
+      <c r="S59" s="83"/>
+      <c r="T59" s="83"/>
+      <c r="U59" s="83"/>
+      <c r="V59" s="83"/>
+      <c r="W59" s="83"/>
+      <c r="X59" s="83"/>
+      <c r="Y59" s="83"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="123">
+    <mergeCell ref="K44:L45"/>
+    <mergeCell ref="M44:N45"/>
+    <mergeCell ref="O44:T45"/>
+    <mergeCell ref="U44:Y45"/>
+    <mergeCell ref="B58:Y59"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="K22:Y22"/>
+    <mergeCell ref="O16:Q17"/>
+    <mergeCell ref="S16:T17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="K16:M17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="B32:J33"/>
+    <mergeCell ref="B28:J29"/>
+    <mergeCell ref="K52:Q52"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="Q57:U57"/>
+    <mergeCell ref="O38:T39"/>
+    <mergeCell ref="U38:Y39"/>
+    <mergeCell ref="T52:X52"/>
+    <mergeCell ref="U32:Y33"/>
+    <mergeCell ref="B44:J45"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="O36:T37"/>
+    <mergeCell ref="K30:L31"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="K34:L35"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="B8:Y8"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O28:T29"/>
+    <mergeCell ref="U28:Y29"/>
+    <mergeCell ref="O30:T31"/>
+    <mergeCell ref="U30:Y31"/>
+    <mergeCell ref="M46:N47"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B30:J31"/>
+    <mergeCell ref="U26:Y27"/>
+    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="O25:T25"/>
+    <mergeCell ref="T50:X50"/>
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O26:T26"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B40:J41"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="O40:T41"/>
+    <mergeCell ref="U40:Y41"/>
+    <mergeCell ref="B42:J43"/>
+    <mergeCell ref="K42:L43"/>
+    <mergeCell ref="M42:N43"/>
+    <mergeCell ref="B48:Y48"/>
+    <mergeCell ref="O42:T43"/>
+    <mergeCell ref="K23:Y23"/>
+    <mergeCell ref="U25:Y25"/>
+    <mergeCell ref="B26:J27"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="U42:Y43"/>
     <mergeCell ref="B56:I56"/>
     <mergeCell ref="K56:Q56"/>
     <mergeCell ref="S56:Y56"/>
@@ -5038,100 +5274,6 @@
     <mergeCell ref="U36:Y37"/>
     <mergeCell ref="B36:J37"/>
     <mergeCell ref="B34:J35"/>
-    <mergeCell ref="O42:T43"/>
-    <mergeCell ref="K23:Y23"/>
-    <mergeCell ref="U25:Y25"/>
-    <mergeCell ref="B26:J27"/>
-    <mergeCell ref="B6:Y6"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="M46:N47"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B30:J31"/>
-    <mergeCell ref="U26:Y27"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="O25:T25"/>
-    <mergeCell ref="T50:X50"/>
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O26:T26"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B40:J41"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="O40:T41"/>
-    <mergeCell ref="U40:Y41"/>
-    <mergeCell ref="B42:J43"/>
-    <mergeCell ref="K42:L43"/>
-    <mergeCell ref="M42:N43"/>
-    <mergeCell ref="B48:Y48"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="O36:T37"/>
-    <mergeCell ref="K30:L31"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="M26:N27"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="K34:L35"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O28:T29"/>
-    <mergeCell ref="U28:Y29"/>
-    <mergeCell ref="O30:T31"/>
-    <mergeCell ref="U30:Y31"/>
-    <mergeCell ref="U42:Y43"/>
-    <mergeCell ref="B58:Y59"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="K22:Y22"/>
-    <mergeCell ref="O16:Q17"/>
-    <mergeCell ref="S16:T17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="K16:M17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="B32:J33"/>
-    <mergeCell ref="B28:J29"/>
-    <mergeCell ref="K52:Q52"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="Q57:U57"/>
-    <mergeCell ref="O38:T39"/>
-    <mergeCell ref="U38:Y39"/>
-    <mergeCell ref="T52:X52"/>
-    <mergeCell ref="U32:Y33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T20" r:id="rId1" xr:uid="{BE351EEA-9877-430E-96A9-ADC6513FEEA9}"/>
@@ -5159,124 +5301,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113" t="s">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1">
-      <c r="A2" s="113"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="121" t="s">
+      <c r="A2" s="127"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1">
-      <c r="U3" s="122"/>
-      <c r="V3" s="122"/>
-      <c r="W3" s="122"/>
-      <c r="X3" s="122"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="134"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="118" t="s">
+      <c r="B4" s="132"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="132"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="119"/>
-      <c r="P4" s="119"/>
-      <c r="Q4" s="119"/>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
-      <c r="T4" s="119"/>
-      <c r="U4" s="119"/>
-      <c r="V4" s="119"/>
-      <c r="W4" s="119"/>
-      <c r="X4" s="120"/>
+      <c r="O4" s="132"/>
+      <c r="P4" s="132"/>
+      <c r="Q4" s="132"/>
+      <c r="R4" s="132"/>
+      <c r="S4" s="132"/>
+      <c r="T4" s="132"/>
+      <c r="U4" s="132"/>
+      <c r="V4" s="132"/>
+      <c r="W4" s="132"/>
+      <c r="X4" s="133"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="115"/>
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="117"/>
+      <c r="A5" s="128"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="129"/>
+      <c r="Q5" s="129"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="129"/>
+      <c r="T5" s="129"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="129"/>
+      <c r="W5" s="129"/>
+      <c r="X5" s="130"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A6" s="3"/>
@@ -5305,66 +5447,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="114" t="s">
+      <c r="A7" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="114" t="s">
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="114"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="114"/>
-      <c r="N7" s="114"/>
-      <c r="O7" s="114"/>
-      <c r="P7" s="114" t="s">
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="114"/>
-      <c r="R7" s="114"/>
-      <c r="S7" s="114"/>
-      <c r="T7" s="114"/>
-      <c r="U7" s="114"/>
-      <c r="V7" s="114"/>
-      <c r="W7" s="114"/>
-      <c r="X7" s="114"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="109"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="109"/>
+      <c r="X7" s="109"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1">
-      <c r="A8" s="54"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="123" t="s">
+      <c r="A8" s="103"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="125"/>
-      <c r="P8" s="123" t="s">
+      <c r="K8" s="117"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="117"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="124"/>
-      <c r="R8" s="124"/>
-      <c r="S8" s="124"/>
-      <c r="T8" s="124"/>
-      <c r="U8" s="124"/>
-      <c r="V8" s="124"/>
-      <c r="W8" s="124"/>
-      <c r="X8" s="125"/>
+      <c r="Q8" s="117"/>
+      <c r="R8" s="117"/>
+      <c r="S8" s="117"/>
+      <c r="T8" s="117"/>
+      <c r="U8" s="117"/>
+      <c r="V8" s="117"/>
+      <c r="W8" s="117"/>
+      <c r="X8" s="118"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A9" s="3"/>
@@ -5393,66 +5535,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="76"/>
-      <c r="V10" s="76"/>
-      <c r="W10" s="76"/>
-      <c r="X10" s="76"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="97"/>
-      <c r="F11" s="97"/>
-      <c r="G11" s="97" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="97"/>
-      <c r="I11" s="97"/>
-      <c r="J11" s="97"/>
-      <c r="K11" s="97"/>
-      <c r="L11" s="97"/>
-      <c r="M11" s="97" t="s">
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="97"/>
-      <c r="O11" s="97"/>
-      <c r="P11" s="97"/>
-      <c r="Q11" s="97"/>
-      <c r="R11" s="97"/>
-      <c r="S11" s="97" t="s">
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="T11" s="97"/>
-      <c r="U11" s="97"/>
-      <c r="V11" s="97"/>
-      <c r="W11" s="97"/>
-      <c r="X11" s="97"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="3"/>
@@ -5481,66 +5623,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="114" t="s">
+      <c r="A13" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="114"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="114"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="114" t="s">
+      <c r="B13" s="109"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="114"/>
-      <c r="L13" s="114"/>
-      <c r="M13" s="114"/>
-      <c r="N13" s="114"/>
-      <c r="O13" s="114"/>
-      <c r="P13" s="114" t="s">
+      <c r="K13" s="109"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="114"/>
-      <c r="R13" s="114"/>
-      <c r="S13" s="114"/>
-      <c r="T13" s="114"/>
-      <c r="U13" s="114"/>
-      <c r="V13" s="114"/>
-      <c r="W13" s="114"/>
-      <c r="X13" s="114"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="123" t="s">
+      <c r="A14" s="103"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="124"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="124"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="125"/>
-      <c r="P14" s="123" t="s">
+      <c r="K14" s="117"/>
+      <c r="L14" s="117"/>
+      <c r="M14" s="117"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="124"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="124"/>
-      <c r="T14" s="124"/>
-      <c r="U14" s="124"/>
-      <c r="V14" s="124"/>
-      <c r="W14" s="124"/>
-      <c r="X14" s="125"/>
+      <c r="Q14" s="117"/>
+      <c r="R14" s="117"/>
+      <c r="S14" s="117"/>
+      <c r="T14" s="117"/>
+      <c r="U14" s="117"/>
+      <c r="V14" s="117"/>
+      <c r="W14" s="117"/>
+      <c r="X14" s="118"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A15" s="3"/>
@@ -5569,172 +5711,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="131" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="32" t="s">
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="132" t="s">
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="132"/>
-      <c r="V16" s="132"/>
-      <c r="W16" s="132"/>
-      <c r="X16" s="132"/>
+      <c r="U16" s="120"/>
+      <c r="V16" s="120"/>
+      <c r="W16" s="120"/>
+      <c r="X16" s="120"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="121"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="133" t="s">
+      <c r="B17" s="111"/>
+      <c r="C17" s="111"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="134"/>
-      <c r="L17" s="134"/>
-      <c r="M17" s="135"/>
-      <c r="N17" s="126" t="s">
+      <c r="K17" s="122"/>
+      <c r="L17" s="122"/>
+      <c r="M17" s="123"/>
+      <c r="N17" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="121"/>
-      <c r="P17" s="121"/>
-      <c r="Q17" s="121"/>
-      <c r="R17" s="121"/>
-      <c r="S17" s="127"/>
-      <c r="T17" s="126" t="s">
+      <c r="O17" s="111"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="112"/>
+      <c r="T17" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="121"/>
-      <c r="V17" s="121"/>
-      <c r="W17" s="121"/>
-      <c r="X17" s="127"/>
+      <c r="U17" s="111"/>
+      <c r="V17" s="111"/>
+      <c r="W17" s="111"/>
+      <c r="X17" s="112"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A18" s="128"/>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
-      <c r="G18" s="129"/>
-      <c r="H18" s="129"/>
-      <c r="I18" s="130"/>
-      <c r="J18" s="136"/>
-      <c r="K18" s="137"/>
-      <c r="L18" s="137"/>
-      <c r="M18" s="138"/>
-      <c r="N18" s="128"/>
-      <c r="O18" s="129"/>
-      <c r="P18" s="129"/>
-      <c r="Q18" s="129"/>
-      <c r="R18" s="129"/>
-      <c r="S18" s="130"/>
-      <c r="T18" s="128"/>
-      <c r="U18" s="129"/>
-      <c r="V18" s="129"/>
-      <c r="W18" s="129"/>
-      <c r="X18" s="130"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="115"/>
+      <c r="J18" s="124"/>
+      <c r="K18" s="125"/>
+      <c r="L18" s="125"/>
+      <c r="M18" s="126"/>
+      <c r="N18" s="113"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="114"/>
+      <c r="Q18" s="114"/>
+      <c r="R18" s="114"/>
+      <c r="S18" s="115"/>
+      <c r="T18" s="113"/>
+      <c r="U18" s="114"/>
+      <c r="V18" s="114"/>
+      <c r="W18" s="114"/>
+      <c r="X18" s="115"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1"/>
     <row r="20" spans="1:24" ht="39" customHeight="1"/>
     <row r="21" spans="1:24">
-      <c r="A21" s="142" t="s">
+      <c r="A21" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="142"/>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="142"/>
-      <c r="H21" s="142"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="142" t="s">
+      <c r="J21" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="142"/>
-      <c r="L21" s="142"/>
-      <c r="M21" s="142"/>
-      <c r="N21" s="142"/>
-      <c r="O21" s="142"/>
-      <c r="P21" s="142"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="108"/>
+      <c r="O21" s="108"/>
+      <c r="P21" s="108"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="142" t="s">
+      <c r="R21" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="142"/>
-      <c r="T21" s="142"/>
-      <c r="U21" s="142"/>
-      <c r="V21" s="142"/>
-      <c r="W21" s="142"/>
-      <c r="X21" s="142"/>
+      <c r="S21" s="108"/>
+      <c r="T21" s="108"/>
+      <c r="U21" s="108"/>
+      <c r="V21" s="108"/>
+      <c r="W21" s="108"/>
+      <c r="X21" s="108"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P23" s="139" t="s">
+      <c r="P23" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
-      <c r="S23" s="139"/>
-      <c r="T23" s="139"/>
-      <c r="U23" s="140" t="s">
+      <c r="Q23" s="105"/>
+      <c r="R23" s="105"/>
+      <c r="S23" s="105"/>
+      <c r="T23" s="105"/>
+      <c r="U23" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="140"/>
-      <c r="W23" s="140"/>
-      <c r="X23" s="140"/>
+      <c r="V23" s="106"/>
+      <c r="W23" s="106"/>
+      <c r="X23" s="106"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P24" s="139" t="s">
+      <c r="P24" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="139"/>
-      <c r="R24" s="139"/>
-      <c r="S24" s="139"/>
-      <c r="T24" s="139"/>
-      <c r="U24" s="141" t="s">
+      <c r="Q24" s="105"/>
+      <c r="R24" s="105"/>
+      <c r="S24" s="105"/>
+      <c r="T24" s="105"/>
+      <c r="U24" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="141"/>
-      <c r="W24" s="141"/>
-      <c r="X24" s="141"/>
+      <c r="V24" s="107"/>
+      <c r="W24" s="107"/>
+      <c r="X24" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -5749,25 +5903,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
carusel de imagenes pt 2, cosas pulidas
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
+++ b/Bitacioras/GFPI-F-147 Formato bitacora etapa productiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\pruebas\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82399CFC-707D-4D43-91DF-C9C8E5502F19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65607A-3148-4DA5-AFE8-D494B1681BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
   <si>
     <t>BITÁCORA DE SEGUIMIENTO ETAPA PRODUCTIVA</t>
   </si>
@@ -181,12 +181,202 @@
     <t>Programa de formación</t>
   </si>
   <si>
+    <t>Nota:  LOS DATOS PROPORCIONADOS SERÁN TRATADOS DE ACUERDO CON LA POLÍTICA DE TRATAMIENTO DE DATOS PERSONALES DEL SENA Y A LA LEY 1581 DE 2012.</t>
+  </si>
+  <si>
+    <t>Código: 
+GFPI-F-147</t>
+  </si>
+  <si>
+    <t>NIT</t>
+  </si>
+  <si>
+    <t>Documento Id.</t>
+  </si>
+  <si>
+    <t>Nombre del Instructor de Seguimiento</t>
+  </si>
+  <si>
+    <t>Nombre del Aprendiz</t>
+  </si>
+  <si>
+    <t>Firma de instructor de seguimiento</t>
+  </si>
+  <si>
+    <t>Firma del jefe inmediato (Si es del caso)</t>
+  </si>
+  <si>
+    <t>VÍNCULO LABORAL O CONTRACTUAL</t>
+  </si>
+  <si>
+    <t>APOYO A UNA UNIDAD PRODUCTIVA FAMILIAR</t>
+  </si>
+  <si>
+    <t>APOYO A INSTITUCIÓN ESTATAL NACIONAL,TERRITORIAL, O A UNA ONG, O A ENTIDAD SIN ANIMO DE LUCRO</t>
+  </si>
+  <si>
+    <t>MONITORIA</t>
+  </si>
+  <si>
+    <t>PASANTIA</t>
+  </si>
+  <si>
+    <t>Proceso Gestión de Formación Profesional Integral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Formato Bitácora seguimiento Etapa productiva</t>
+  </si>
+  <si>
+    <t>Versión: 03</t>
+  </si>
+  <si>
+    <t>REGIONAL Santander</t>
+  </si>
+  <si>
+    <t>Centro Agroturistico</t>
+  </si>
+  <si>
+    <t>Edgar Mauricio Campos Ribero</t>
+  </si>
+  <si>
+    <t>17/02/2025 al 03/03/2025</t>
+  </si>
+  <si>
+    <t>Analisi y Desarrollo de software</t>
+  </si>
+  <si>
+    <t>johan sebastian blanco cataño</t>
+  </si>
+  <si>
+    <t>jsblanco61@misena.edu.co</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>frchacon@sena.edu.co</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA NUEVA DEL ORIENTE SAS</t>
+  </si>
+  <si>
+    <t>900.446.865-3</t>
+  </si>
+  <si>
+    <t>Este día me centré exclusivamente en el menú para móviles. En la mañana intenté agregar más cosas, como hacer que su movimiento siguiera al dedo del usuario, pero al ver que esto podría traer problemas de rendimiento, opté por dejarlo lo más simple posible (me refiero a la lógica de gestos, no a su apariencia).
+El resto del día lo dediqué a optimizarlo al máximo, renombrando variables y reorganizando el código para que sea lo más legible e intuitivo posible para futuros desarrolladores. Me gustó cómo quedó, definitivamente lo guardaré para futuros proyectos.
+Después de esto, hice algunos cambios para que funcionara en cualquier tamaño. La animación de salida ahora funcionará para cualquier diseño de menú.</t>
+  </si>
+  <si>
+    <t>Perdí la mitad del día al descartar la idea de la mañana, pero es por el bien del proyecto. Es importante saber cuándo menos es más, aunque eso signifique eliminar progreso.
+Para que fuera compatible con cualquier ancho, tuve que invertir la lógica de abrir/cerrar, pero al final creo que no quedó confuso, que es lo importante.</t>
+  </si>
+  <si>
+    <t>Johan sebastian blanco Cataño</t>
+  </si>
+  <si>
+    <t>Cambié la forma de implementar el código JS en la página. Originalmente, en la imagen #1 se ve que el código se escribía directamente, lo que provocaba errores al usar caracteres como &amp;, &gt; y otros símbolos extraños.
+Busqué una solución a esto con &lt;![CDATA[ que hace que el XML deje de reconocer estos símbolos. En la imagen #2 no me gustaba cómo se veía, así que agregué una extensión a la documentación para facilitar la lectura en la imagen #3.
+Esto dio mejor lectura al código y redujo los errores.
+También hice lo mismo con el CSS del documento.
+Ya para el final del día, por fin implementé el menú desplegable, aunque aún hay que pulirlo más. Además, debo cambiar la forma en la que la página se organiza en dispositivos móviles.</t>
+  </si>
+  <si>
+    <t>lo que mas me tomo tiempo implementar fue la nueva forma de incrustar scrips y css eso me tomo todo el dia, aun que mientras lo asi me tome tiempo para optimizar mas cosas</t>
+  </si>
+  <si>
+    <t>Hoy quería centrarme en terminar de acomodar las cosas que quedaron mal ayer. Básicamente, ya no queda el espacio en blanco que dejaba el menú en móviles. Reorganicé la forma en que se acomoda el main para eso de nuevo, pero aún no me convence, ya que el código quedó muy raro y confuso.
+Le agregué scroll al menú en móviles, hice que la flecha se fijara al bajar y que al presionarla te llevara hacia arriba, como en WhatsApp. También terminé el botón de compartir que tenía pendiente.</t>
+  </si>
+  <si>
+    <t>Hoy fue un día muy estresante, ya que hubo muchos errores. Además de eso, opté por eliminar algunas funciones que ya había programado para volver a hacerlas.
+Siento que cada vez hago más esto último, y me da miedo llegar a un punto en el que no pueda avanzar.
+Me esforzaré por crear un código mejor y más escalable.</t>
+  </si>
+  <si>
+    <t>hise una animacion de maquina de escribir en la  superior del block, los mensajes son atravez de divs y puedes agregar cuantos quieras y los recorrera en orden, esto intentare que sea personalizable atravez de la interfaz de blogger, pero como le dedique mucho tiempo a eso decidi empezar con la implementacion de las redes sociales
+despaso arregle el problema de scroll que tenia el menu ya que cuando era muy pequeño sus componentes se atrabezaban entre si, el codigo de la redes sociales parece igual al los links de arriba pero enrealidad la pude llegar a resumir a la mitad de codigo que la primera, esto por que ya entendi como se llaman entre si los bloques y simplemente tube que ir subiendo poco a poco viendo que llamaba aque cosa hasta que logre hacer que todo el bloque sea uno solo y no varios
+no me alcanzo el tiempo para ponerle los iconos</t>
+  </si>
+  <si>
+    <t>supongo que fue el texto animado, me tomo demaciado, desde la idea que tenia, implementarlo en una sola palabra, acomodarlo en el blog y luego intentar hacerlo con un numero ilimitado de mensajes
+pero me gusto como quedo el codigo, bien comentado y fasil de entender
+pero si esto es lo que mas me costo hoy</t>
+  </si>
+  <si>
+    <t>Los íconos de las redes sociales no son imágenes; están en formato SVG directamente insertados en el código. De esta forma, aparecen instantáneamente al cargar la página y ayudan a la optimización al no ser imágenes.
+Me costó demasiado encontrar estos íconos, además de modificar su padding para que todos quedaran iguales, pero estoy bastante contento con el resultado.</t>
+  </si>
+  <si>
+    <t>Di compatibilidad para agregar inserciones de YouTube y TikTok, pero este último consume demasiados recursos en los celulares. En una PC funciona muy bien, pero tendré que anotar que, preferiblemente, no inserten videos de TikTok.
+Agregué redes sociales, además de que estas pueden modificarse desde la interfaz de Blogger. Siguiendo esa misma lógica, apliqué lo mismo a los textos animados: se pueden agregar cuantos se quieran, además de tener un orden totalmente reorganizable.</t>
+  </si>
+  <si>
+    <t>acomode los botones de descarga para que tuviera una mejor presentacion 
+estuve revisando un buen rato el codigo de descarga de los botones pero no fui capas de encontrar una forma para que fueran mas rapidos, aun que tienen un velocidad aceptable
+cree un sistema de notificaciones globales y asi poderlas usar en cualquier parate del proyecto, ademas para probarlas las integre al sistema de descarga de imagenes
+como extra organise los marcadores de una mejor forma, ahora se llaman marker, y son mas pequeños</t>
+  </si>
+  <si>
+    <t>sin mayores complicaciones, como dije antes lo unico fue lo de la forma de descargar imágenes que no lo pude mejorar</t>
+  </si>
+  <si>
+    <t>falle al intentar optimizar la imagenn</t>
+  </si>
+  <si>
+    <t>Completé los botones del carrusel de imágenes y organicé su código con funciones, lo cual le da más simplicidad.
+También cambié un poco el diseño de las flechas y las tarjetas, aunque en estas últimas solo modifiqué el sombreado y el contorno.
+Ahora el menú superior ya no ocupa todo el alto de la pantalla (esto fue una petición de mi jefe inmediato).
+Estuve un buen rato aprendiendo el funcionamiento del embed de X, aunque no pude conseguir que se mostraran menos posts. Sin embargo, logré encontrar un diseño sin bordes y con menos márgenes, que para mí le da un mejor aspecto.
+Se me ocurrió que cuando un post tenga muchas imágenes, podría tener una presentación igual a la del carrusel de arriba. Aunque, como se puede ver en la última imagen, hacerlo solo con CSS es demasiado imposible. Por ende, optaré por crear mañana un JS que extraiga las imágenes de los posts y las transforme en la antepenúltima imagen (aunque esta solo es una representación de cómo quiero que quede).
+Sinceramente, creo que esto saldrá mal y que probablemente disminuya la eficiencia de la página, pero aun así quiero intentarlo. Creo que sería una implementación muy buena</t>
+  </si>
+  <si>
+    <t>No pude hacer todo lo que quería con la inserción del embed, así que tendré que crear un código JS para poder lograr la idea de las imágenes.</t>
+  </si>
+  <si>
+    <t>Creé un carrusel de imágenes compatible con deslizamiento en móviles. Además, lo incorporé a la versión móvil de la página, pero no tuve tiempo para agregar los botones de adelantar y retroceder.</t>
+  </si>
+  <si>
+    <t>Fue un infierno. Tenía dos caminos: el carrusel con desvanecimiento pero sin ser scrolleable, o este. La verdad, mordí más de lo que podía masticar, pero quedó más o menos.
+Sinceramente, no me convencen las dimensiones de las imágenes de muestra.</t>
+  </si>
+  <si>
+    <t>Mejoré las funciones para notificaciones. Ahora el título es personalizable, además de contar con tres tipos distintos: info, positive y negative, cada una con su respectivo color.
+Pasé un buen rato buscando de nuevo alguna forma de descargar las imágenes más rápido, pero no pude.
+Agregué las vistas que ha tenido el blog.
+También implementé una visualización de las últimas publicaciones de X del CENA.
+Cambié los tamaños del menú lateral y el contenedor principal; ahora son un poco más grandes y tienen mejores márgenes.</t>
+  </si>
+  <si>
+    <t>Empezando el día, me dispuse a revisar la forma en la que se muestran las imágenes, ya que la manera en la que se amplían es muy poco eficiente. Estaba viendo la posibilidad de abrirlas en una nueva pestaña con su archivo original, pero esto hacía que la página se recargara al volver.
+Leyendo información sobre Blogger, encontré la forma de deshabilitar los scripts y CSS por defecto, lo que me permitiría no tener que descargar elementos innecesarios y tener total libertad para crear un sistema de ampliación de imágenes completamente desde cero.
+Sin embargo, esto iba a tomar demasiado tiempo, así que solo agregué un poco más de compatibilidad al sistema de presentación de imágenes existente.
+Luego, la tarea principal de hoy fue crear un sistema de descarga</t>
+  </si>
+  <si>
+    <t>Las imágenes, al provenir de un servidor diferente al que reside la página, hacían que el navegador me prohibiera hacerlo directamente (esto me complicó mucho).
+Pero lo peor fue intentar hallar la forma de agregar el botón para cada imagen del post. Quería hacerlo a través del HTML para que fuera más optimizado, pero desafortunadamente se me hizo imposible debido a cómo funciona Blogger.
+Así que me rendí y tuve que agregar los botones artificialmente a través de JS.</t>
+  </si>
+  <si>
+    <t>Agregué animaciones a las redes sociales cuando pasas el cursor por encima, además de un efecto de ola para hacerlas más llamativas.
+La animación del texto superior ahora no comienza hasta que el documento carga por completo. De esta manera, no se ve lageada, ya que al principio, con tantas cosas cargando, la animación se trababa.
+Volví a crear el sistema que determina si un post debe ocupar toda la fila. Si la pantalla mide menos de 900px, no se ejecutará, por lo que los dispositivos móviles no tendrán que procesarlo. Ahora, además de eso, detecta si la pantalla se vuelve más grande y, cuando alcanza cierto punto, se ejecuta y la función se borra, ya que no es necesaria más.
+También reorganicé el código del post, ya que noté que se ejecutaba una vez por cada post que se renderizaba (15 veces).</t>
+  </si>
+  <si>
+    <t>Tuve que cambiar la forma en que se ocultaba el texto animado para que se viera el puntero, incluso si la animación aún no había comenzado.
+Todo lo relacionado con acomodar los posts según el tamaño llevó un arduo trabajo, intentando encontrar la forma menos exigente para el sistema.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Aprendiz: </t>
     </r>
     <r>
       <rPr>
         <i/>
+        <u/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -196,190 +386,12 @@
       <t>recuerde diligenciar completamente el informe y entregarlo o subirlo  al espacio asignado para este.</t>
     </r>
   </si>
-  <si>
-    <t>Nota:  LOS DATOS PROPORCIONADOS SERÁN TRATADOS DE ACUERDO CON LA POLÍTICA DE TRATAMIENTO DE DATOS PERSONALES DEL SENA Y A LA LEY 1581 DE 2012.</t>
-  </si>
-  <si>
-    <t>Código: 
-GFPI-F-147</t>
-  </si>
-  <si>
-    <t>NIT</t>
-  </si>
-  <si>
-    <t>Documento Id.</t>
-  </si>
-  <si>
-    <t>Nombre del Instructor de Seguimiento</t>
-  </si>
-  <si>
-    <t>Nombre del Aprendiz</t>
-  </si>
-  <si>
-    <t>Firma de instructor de seguimiento</t>
-  </si>
-  <si>
-    <t>Firma del jefe inmediato (Si es del caso)</t>
-  </si>
-  <si>
-    <t>VÍNCULO LABORAL O CONTRACTUAL</t>
-  </si>
-  <si>
-    <t>APOYO A UNA UNIDAD PRODUCTIVA FAMILIAR</t>
-  </si>
-  <si>
-    <t>APOYO A INSTITUCIÓN ESTATAL NACIONAL,TERRITORIAL, O A UNA ONG, O A ENTIDAD SIN ANIMO DE LUCRO</t>
-  </si>
-  <si>
-    <t>MONITORIA</t>
-  </si>
-  <si>
-    <t>PASANTIA</t>
-  </si>
-  <si>
-    <t>Proceso Gestión de Formación Profesional Integral</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Formato Bitácora seguimiento Etapa productiva</t>
-  </si>
-  <si>
-    <t>Versión: 03</t>
-  </si>
-  <si>
-    <t>REGIONAL Santander</t>
-  </si>
-  <si>
-    <t>Centro Agroturistico</t>
-  </si>
-  <si>
-    <t>Edgar Mauricio Campos Ribero</t>
-  </si>
-  <si>
-    <t>17/02/2025 al 03/03/2025</t>
-  </si>
-  <si>
-    <t>Analisi y Desarrollo de software</t>
-  </si>
-  <si>
-    <t>johan sebastian blanco cataño</t>
-  </si>
-  <si>
-    <t>jsblanco61@misena.edu.co</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>frchacon@sena.edu.co</t>
-  </si>
-  <si>
-    <t>AGROPECUARIA NUEVA DEL ORIENTE SAS</t>
-  </si>
-  <si>
-    <t>900.446.865-3</t>
-  </si>
-  <si>
-    <t>Este día me centré exclusivamente en el menú para móviles. En la mañana intenté agregar más cosas, como hacer que su movimiento siguiera al dedo del usuario, pero al ver que esto podría traer problemas de rendimiento, opté por dejarlo lo más simple posible (me refiero a la lógica de gestos, no a su apariencia).
-El resto del día lo dediqué a optimizarlo al máximo, renombrando variables y reorganizando el código para que sea lo más legible e intuitivo posible para futuros desarrolladores. Me gustó cómo quedó, definitivamente lo guardaré para futuros proyectos.
-Después de esto, hice algunos cambios para que funcionara en cualquier tamaño. La animación de salida ahora funcionará para cualquier diseño de menú.</t>
-  </si>
-  <si>
-    <t>Perdí la mitad del día al descartar la idea de la mañana, pero es por el bien del proyecto. Es importante saber cuándo menos es más, aunque eso signifique eliminar progreso.
-Para que fuera compatible con cualquier ancho, tuve que invertir la lógica de abrir/cerrar, pero al final creo que no quedó confuso, que es lo importante.</t>
-  </si>
-  <si>
-    <t>Johan sebastian blanco Cataño</t>
-  </si>
-  <si>
-    <t>Cambié la forma de implementar el código JS en la página. Originalmente, en la imagen #1 se ve que el código se escribía directamente, lo que provocaba errores al usar caracteres como &amp;, &gt; y otros símbolos extraños.
-Busqué una solución a esto con &lt;![CDATA[ que hace que el XML deje de reconocer estos símbolos. En la imagen #2 no me gustaba cómo se veía, así que agregué una extensión a la documentación para facilitar la lectura en la imagen #3.
-Esto dio mejor lectura al código y redujo los errores.
-También hice lo mismo con el CSS del documento.
-Ya para el final del día, por fin implementé el menú desplegable, aunque aún hay que pulirlo más. Además, debo cambiar la forma en la que la página se organiza en dispositivos móviles.</t>
-  </si>
-  <si>
-    <t>lo que mas me tomo tiempo implementar fue la nueva forma de incrustar scrips y css eso me tomo todo el dia, aun que mientras lo asi me tome tiempo para optimizar mas cosas</t>
-  </si>
-  <si>
-    <t>Hoy quería centrarme en terminar de acomodar las cosas que quedaron mal ayer. Básicamente, ya no queda el espacio en blanco que dejaba el menú en móviles. Reorganicé la forma en que se acomoda el main para eso de nuevo, pero aún no me convence, ya que el código quedó muy raro y confuso.
-Le agregué scroll al menú en móviles, hice que la flecha se fijara al bajar y que al presionarla te llevara hacia arriba, como en WhatsApp. También terminé el botón de compartir que tenía pendiente.</t>
-  </si>
-  <si>
-    <t>Hoy fue un día muy estresante, ya que hubo muchos errores. Además de eso, opté por eliminar algunas funciones que ya había programado para volver a hacerlas.
-Siento que cada vez hago más esto último, y me da miedo llegar a un punto en el que no pueda avanzar.
-Me esforzaré por crear un código mejor y más escalable.</t>
-  </si>
-  <si>
-    <t>hise una animacion de maquina de escribir en la  superior del block, los mensajes son atravez de divs y puedes agregar cuantos quieras y los recorrera en orden, esto intentare que sea personalizable atravez de la interfaz de blogger, pero como le dedique mucho tiempo a eso decidi empezar con la implementacion de las redes sociales
-despaso arregle el problema de scroll que tenia el menu ya que cuando era muy pequeño sus componentes se atrabezaban entre si, el codigo de la redes sociales parece igual al los links de arriba pero enrealidad la pude llegar a resumir a la mitad de codigo que la primera, esto por que ya entendi como se llaman entre si los bloques y simplemente tube que ir subiendo poco a poco viendo que llamaba aque cosa hasta que logre hacer que todo el bloque sea uno solo y no varios
-no me alcanzo el tiempo para ponerle los iconos</t>
-  </si>
-  <si>
-    <t>supongo que fue el texto animado, me tomo demaciado, desde la idea que tenia, implementarlo en una sola palabra, acomodarlo en el blog y luego intentar hacerlo con un numero ilimitado de mensajes
-pero me gusto como quedo el codigo, bien comentado y fasil de entender
-pero si esto es lo que mas me costo hoy</t>
-  </si>
-  <si>
-    <t>Los íconos de las redes sociales no son imágenes; están en formato SVG directamente insertados en el código. De esta forma, aparecen instantáneamente al cargar la página y ayudan a la optimización al no ser imágenes.
-Me costó demasiado encontrar estos íconos, además de modificar su padding para que todos quedaran iguales, pero estoy bastante contento con el resultado.</t>
-  </si>
-  <si>
-    <t>Di compatibilidad para agregar inserciones de YouTube y TikTok, pero este último consume demasiados recursos en los celulares. En una PC funciona muy bien, pero tendré que anotar que, preferiblemente, no inserten videos de TikTok.
-Agregué redes sociales, además de que estas pueden modificarse desde la interfaz de Blogger. Siguiendo esa misma lógica, apliqué lo mismo a los textos animados: se pueden agregar cuantos se quieran, además de tener un orden totalmente reorganizable.</t>
-  </si>
-  <si>
-    <t>tuve cambiar la forma como se ocultaba el texto animado para hacer que se viera el puntero aun que la animacion no haya empezado, TODO lo que tuve que ver con acomodar los post según el tamaño llevo un arduo trabajo para intentar encontrar las forma menos exigente para el sistema de hacerlo</t>
-  </si>
-  <si>
-    <t>le agrege animaciones a las redes sociales cuando pasas el cursor por encima, tambien un efecto de ola que hacen para ser mas llamativas
-la animacion del texto superior no comienza hasta que el documento carga por completo, asi esta no seve lageada ya que al principio de tantas cosas las animacion se trababa
-volve a crear el sistema que determina si  un post debe ocupar toda la fila, si la pantallamide menos de 900px  no se ejecutara por ende los dispositivos moviles no tendran que prosesarlo, ahora  no solo eso si no que detecta si la pantalla de vuelve mas grande, y si llega ah un punto se ejecuta y la funcion se borra ya que no es nesesaria mas
-acomodo en otra parte el codigo del post ya que vi que se ejecutava una vez por cada post que se pintaba ( 15 veces)</t>
-  </si>
-  <si>
-    <t>empezando el dia me dispuse a ver la forma en la que las imágenes se muestran ya que las forma en la que se amplian es muy poco eficiente, estaba biendo la posibilibilidad de abrirlas abriendo su archivo original en una nueva pestaña pero esta forma hacia que la pagina se recargara al volver
-leyendo informacion sobre blogger vi la forma de desabilitar los scripts y css por defecto lo que me permitiria no tener que descargar cosas inesesaria y tener total libertad de crear una forma de amplear las imagenes totalmente desde 0
-pero esto ya iva a tomar mucho tiempo asi que solo le agrege un poco mas de compatibilidad al sistema de presentacion de imagenes existente
-luego la tarea principal de hoy fue crear un sistema de descarga</t>
-  </si>
-  <si>
-    <t>las imágenes al provenir de un servidor diferente al que reside la pagina  hacia que el naveganor me prohiviera hacerlo directamente (esto me complico mucho) 
-pero lo peor fue intentar hayar la forma de agregar el boton por cada imagen del post. Queria hacerlos atravez del html para que sea mas optimizdo pero desafortunadamente seme hiso imposible por como funciona blogger asi que me rendi y tuve que agregar los botones artificialmente atravez de js</t>
-  </si>
-  <si>
-    <t>acomode los botones de descarga para que tuviera una mejor presentacion 
-estuve revisando un buen rato el codigo de descarga de los botones pero no fui capas de encontrar una forma para que fueran mas rapidos, aun que tienen un velocidad aceptable
-cree un sistema de notificaciones globales y asi poderlas usar en cualquier parate del proyecto, ademas para probarlas las integre al sistema de descarga de imagenes
-como extra organise los marcadores de una mejor forma, ahora se llaman marker, y son mas pequeños</t>
-  </si>
-  <si>
-    <t>sin mayores complicaciones, como dije antes lo unico fue lo de la forma de descargar imágenes que no lo pude mejorar</t>
-  </si>
-  <si>
-    <t>mejore las funciones para notificaciones, ahora el titulo el personalizable ademas de tener 3 tipos distintos info, positibe y negative cada una con su respectivo color
-me puse un buen rato a buscar denuevo alguna forma para descargar las imágenes mas rapido pero no puede
-agrege las vistas que ah tenido el blog
-agrege una visualizacion de las ultimas publicaciones de x del cena 
-cambie los tamaños de el menu lateral y contenedor principal, son un poco mas grandes y con mejores margenes</t>
-  </si>
-  <si>
-    <t>falle al intentar optimizar la imagenn</t>
-  </si>
-  <si>
-    <t>29/02/2025</t>
-  </si>
-  <si>
-    <t>cree un carusel de imágenes, es compatible para deslizrlo en moviles, ademas de que lo incorpore a la pagina ala vercion de movil, pero no tuve tiempo para agregar lo botodes de adelantar y retroceder</t>
-  </si>
-  <si>
-    <t>fue un infierno, tenia 2 caminos el caruse con desbanecimiento pero sin se scroleable o este, y la verdad mordi mas de lo que podia masticar pero quedo mas oh menos sinseramente no me comvense las dimenciones de las imágenes de muestra</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,6 +543,25 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -763,7 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -906,13 +937,13 @@
     <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -921,15 +952,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -996,8 +1018,23 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,6 +1067,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1165,40 +1220,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3009,6 +3031,256 @@
         <a:xfrm>
           <a:off x="6278216" y="56466805"/>
           <a:ext cx="1383195" cy="3097661"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>32251</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>1217543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>34483</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>2718790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Imagen 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81051253-02D4-4B3E-806F-A38554F466E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5821794" y="63991434"/>
+          <a:ext cx="2395906" cy="1501247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>281487</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>2147225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>284881</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>911087</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Imagen 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A79F8CE6-8B87-49A3-8FF4-188EDB0E1739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6833030" y="61914529"/>
+          <a:ext cx="1254068" cy="1770449"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>224992</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>33972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>165654</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>692289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Imagen 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E03A275-AAD3-428A-B2EA-419DAF14C0B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6014535" y="59801276"/>
+          <a:ext cx="1953336" cy="658317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>84221</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>2149363</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>141411</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>977348</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Imagen 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25DB2D89-DCB4-4704-8917-3B9F43D96122}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5873764" y="61916667"/>
+          <a:ext cx="819190" cy="1834572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>222287</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>819979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>137999</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>2029240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Imagen 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3DA489B-D9E9-495C-9938-B1E33E44624B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6011830" y="60587283"/>
+          <a:ext cx="1928386" cy="1209261"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3429,8 +3701,8 @@
   </sheetPr>
   <dimension ref="B1:AA59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44:Y45"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:Y48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
@@ -3455,172 +3727,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B1" s="81"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="79" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+    </row>
+    <row r="2" spans="2:25" ht="35.25" customHeight="1">
+      <c r="B2" s="83"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+    </row>
+    <row r="3" spans="2:25" ht="18" customHeight="1">
+      <c r="B3" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="89"/>
+      <c r="T3" s="89"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="89"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+    </row>
+    <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B4" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+    </row>
+    <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
+      <c r="B5" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-    </row>
-    <row r="2" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B2" s="81"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="80"/>
-    </row>
-    <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-    </row>
-    <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-    </row>
-    <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B5" s="61" t="s">
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="60"/>
+    </row>
+    <row r="6" spans="2:25" ht="32.25" customHeight="1">
+      <c r="B6" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
-      <c r="U5" s="62"/>
-      <c r="V5" s="62"/>
-      <c r="W5" s="62"/>
-      <c r="X5" s="62"/>
-      <c r="Y5" s="63"/>
-    </row>
-    <row r="6" spans="2:25" ht="32.25" customHeight="1">
-      <c r="B6" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
-      <c r="V6" s="62"/>
-      <c r="W6" s="62"/>
-      <c r="X6" s="62"/>
-      <c r="Y6" s="63"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="60"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1">
       <c r="B7" s="21" t="s">
@@ -3652,29 +3924,29 @@
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1">
       <c r="B8" s="18"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="88"/>
-      <c r="W8" s="88"/>
-      <c r="X8" s="88"/>
-      <c r="Y8" s="88"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="90"/>
+      <c r="X8" s="90"/>
+      <c r="Y8" s="90"/>
     </row>
     <row r="9" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
       <c r="B9" s="33" t="s">
@@ -3691,7 +3963,7 @@
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N9" s="34"/>
       <c r="O9" s="34"/>
@@ -3711,21 +3983,21 @@
       <c r="Y9" s="33"/>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="N10" s="34"/>
       <c r="O10" s="34"/>
@@ -3735,14 +4007,14 @@
       <c r="Q10" s="31"/>
       <c r="R10" s="31"/>
       <c r="S10" s="32"/>
-      <c r="T10" s="66" t="s">
-        <v>68</v>
-      </c>
-      <c r="U10" s="66"/>
-      <c r="V10" s="66"/>
-      <c r="W10" s="66"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
+      <c r="T10" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B11" s="3"/>
@@ -3771,49 +4043,49 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="67" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="67" t="s">
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="67"/>
-      <c r="S12" s="67"/>
-      <c r="T12" s="67"/>
-      <c r="U12" s="67"/>
-      <c r="V12" s="67"/>
-      <c r="W12" s="67"/>
-      <c r="X12" s="67"/>
-      <c r="Y12" s="67"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="64"/>
+      <c r="U12" s="64"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="64"/>
+      <c r="X12" s="64"/>
+      <c r="Y12" s="64"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1">
-      <c r="B13" s="72">
+      <c r="B13" s="69">
         <v>3177294629</v>
       </c>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="74"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="71"/>
       <c r="K13" s="51">
         <v>3177294629</v>
       </c>
@@ -3822,17 +4094,17 @@
       <c r="N13" s="51"/>
       <c r="O13" s="51"/>
       <c r="P13" s="51"/>
-      <c r="Q13" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="66"/>
-      <c r="W13" s="66"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="66"/>
+      <c r="Q13" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="63"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="63"/>
     </row>
     <row r="14" spans="2:25" ht="9.9499999999999993" customHeight="1">
       <c r="B14" s="3"/>
@@ -3861,100 +4133,100 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1">
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="89"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="89"/>
-      <c r="W15" s="89"/>
-      <c r="X15" s="89"/>
-      <c r="Y15" s="89"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="91"/>
+      <c r="X15" s="91"/>
+      <c r="Y15" s="91"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1">
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="64" t="s">
+      <c r="C16" s="61"/>
+      <c r="D16" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="61"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="64"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="94" t="s">
+      <c r="L16" s="103"/>
+      <c r="M16" s="104"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="95"/>
-      <c r="M16" s="96"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="64" t="s">
+      <c r="P16" s="101"/>
+      <c r="Q16" s="101"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="65"/>
-      <c r="S16" s="64" t="s">
+      <c r="T16" s="61"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="64"/>
-      <c r="U16" s="65"/>
-      <c r="V16" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="W16" s="64"/>
-      <c r="X16" s="64"/>
-      <c r="Y16" s="65"/>
+      <c r="W16" s="61"/>
+      <c r="X16" s="61"/>
+      <c r="Y16" s="62"/>
     </row>
     <row r="17" spans="2:27" ht="45.75" customHeight="1">
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="97"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="99"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="93"/>
-      <c r="P17" s="93"/>
-      <c r="Q17" s="93"/>
-      <c r="R17" s="65"/>
-      <c r="S17" s="64"/>
-      <c r="T17" s="64"/>
-      <c r="U17" s="65"/>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
-      <c r="X17" s="64"/>
-      <c r="Y17" s="65"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="107"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="101"/>
+      <c r="P17" s="101"/>
+      <c r="Q17" s="101"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="61"/>
+      <c r="W17" s="61"/>
+      <c r="X17" s="61"/>
+      <c r="Y17" s="62"/>
     </row>
     <row r="18" spans="2:27" ht="9.9499999999999993" customHeight="1">
       <c r="B18" s="3"/>
@@ -3994,7 +4266,7 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
       <c r="J19" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
@@ -4017,23 +4289,23 @@
       <c r="Y19" s="27"/>
     </row>
     <row r="20" spans="2:27" ht="18" customHeight="1">
-      <c r="B20" s="100" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="102">
+      <c r="B20" s="108" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="110">
         <v>1096800316</v>
       </c>
-      <c r="K20" s="103"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="103"/>
-      <c r="N20" s="103"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="111"/>
+      <c r="M20" s="111"/>
+      <c r="N20" s="111"/>
       <c r="O20" s="23">
         <v>3219713759</v>
       </c>
@@ -4042,7 +4314,7 @@
       <c r="R20" s="24"/>
       <c r="S20" s="24"/>
       <c r="T20" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U20" s="29"/>
       <c r="V20" s="29"/>
@@ -4080,14 +4352,14 @@
       <c r="B22" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="91"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+      <c r="J22" s="99"/>
       <c r="K22" s="33" t="s">
         <v>47</v>
       </c>
@@ -4096,45 +4368,45 @@
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
       <c r="P22" s="33"/>
-      <c r="Q22" s="92"/>
-      <c r="R22" s="92"/>
-      <c r="S22" s="92"/>
-      <c r="T22" s="92"/>
-      <c r="U22" s="92"/>
-      <c r="V22" s="92"/>
-      <c r="W22" s="92"/>
-      <c r="X22" s="92"/>
-      <c r="Y22" s="92"/>
+      <c r="Q22" s="100"/>
+      <c r="R22" s="100"/>
+      <c r="S22" s="100"/>
+      <c r="T22" s="100"/>
+      <c r="U22" s="100"/>
+      <c r="V22" s="100"/>
+      <c r="W22" s="100"/>
+      <c r="X22" s="100"/>
+      <c r="Y22" s="100"/>
     </row>
     <row r="23" spans="2:27" ht="18" customHeight="1">
-      <c r="B23" s="69">
+      <c r="B23" s="66">
         <v>2557356</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="70"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57"/>
-      <c r="Q23" s="57"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="57"/>
-      <c r="U23" s="57"/>
-      <c r="V23" s="57"/>
-      <c r="W23" s="57"/>
-      <c r="X23" s="57"/>
-      <c r="Y23" s="58"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="54"/>
+      <c r="X23" s="54"/>
+      <c r="Y23" s="55"/>
     </row>
     <row r="24" spans="2:27" ht="9.75" customHeight="1">
       <c r="B24" s="3"/>
@@ -4166,41 +4438,41 @@
       <c r="B25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="60"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="57"/>
       <c r="K25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="59"/>
+      <c r="L25" s="56"/>
       <c r="M25" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="59"/>
+      <c r="N25" s="56"/>
       <c r="O25" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="59"/>
-      <c r="T25" s="60"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="56"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="57"/>
       <c r="U25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="59"/>
-      <c r="W25" s="59"/>
-      <c r="X25" s="59"/>
-      <c r="Y25" s="60"/>
+      <c r="V25" s="56"/>
+      <c r="W25" s="56"/>
+      <c r="X25" s="56"/>
+      <c r="Y25" s="57"/>
     </row>
     <row r="26" spans="2:27" ht="216" customHeight="1">
       <c r="B26" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
@@ -4213,19 +4485,19 @@
       <c r="K26" s="47">
         <v>45705</v>
       </c>
-      <c r="L26" s="53"/>
+      <c r="L26" s="48"/>
       <c r="M26" s="47">
         <v>45706</v>
       </c>
-      <c r="N26" s="53"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="70"/>
-      <c r="R26" s="70"/>
-      <c r="S26" s="70"/>
-      <c r="T26" s="71"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="66"/>
+      <c r="P26" s="67"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="67"/>
+      <c r="S26" s="67"/>
+      <c r="T26" s="68"/>
       <c r="U26" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V26" s="52"/>
       <c r="W26" s="52"/>
@@ -4242,16 +4514,16 @@
       <c r="H27" s="39"/>
       <c r="I27" s="39"/>
       <c r="J27" s="40"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="70"/>
-      <c r="Q27" s="70"/>
-      <c r="R27" s="70"/>
-      <c r="S27" s="70"/>
-      <c r="T27" s="71"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="66"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="68"/>
       <c r="U27" s="52"/>
       <c r="V27" s="52"/>
       <c r="W27" s="52"/>
@@ -4260,7 +4532,7 @@
     </row>
     <row r="28" spans="2:27" ht="126.75" customHeight="1">
       <c r="B28" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
@@ -4273,11 +4545,11 @@
       <c r="K28" s="47">
         <v>45706</v>
       </c>
-      <c r="L28" s="53"/>
+      <c r="L28" s="48"/>
       <c r="M28" s="47">
         <v>45707</v>
       </c>
-      <c r="N28" s="53"/>
+      <c r="N28" s="48"/>
       <c r="O28" s="51"/>
       <c r="P28" s="51"/>
       <c r="Q28" s="51"/>
@@ -4285,7 +4557,7 @@
       <c r="S28" s="51"/>
       <c r="T28" s="51"/>
       <c r="U28" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V28" s="52"/>
       <c r="W28" s="52"/>
@@ -4302,10 +4574,10 @@
       <c r="H29" s="39"/>
       <c r="I29" s="39"/>
       <c r="J29" s="40"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="55"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
       <c r="O29" s="51"/>
       <c r="P29" s="51"/>
       <c r="Q29" s="51"/>
@@ -4321,7 +4593,7 @@
     </row>
     <row r="30" spans="2:27" ht="105" customHeight="1">
       <c r="B30" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
@@ -4334,11 +4606,11 @@
       <c r="K30" s="47">
         <v>45707</v>
       </c>
-      <c r="L30" s="53"/>
+      <c r="L30" s="48"/>
       <c r="M30" s="47">
         <v>45708</v>
       </c>
-      <c r="N30" s="53"/>
+      <c r="N30" s="48"/>
       <c r="O30" s="51"/>
       <c r="P30" s="51"/>
       <c r="Q30" s="51"/>
@@ -4346,7 +4618,7 @@
       <c r="S30" s="51"/>
       <c r="T30" s="51"/>
       <c r="U30" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V30" s="52"/>
       <c r="W30" s="52"/>
@@ -4363,10 +4635,10 @@
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
       <c r="J31" s="40"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="55"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="50"/>
       <c r="O31" s="51"/>
       <c r="P31" s="51"/>
       <c r="Q31" s="51"/>
@@ -4382,7 +4654,7 @@
     </row>
     <row r="32" spans="2:27" ht="280.5" customHeight="1">
       <c r="B32" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
@@ -4395,11 +4667,11 @@
       <c r="K32" s="47">
         <v>45708</v>
       </c>
-      <c r="L32" s="53"/>
+      <c r="L32" s="48"/>
       <c r="M32" s="47">
         <v>45709</v>
       </c>
-      <c r="N32" s="53"/>
+      <c r="N32" s="48"/>
       <c r="O32" s="51"/>
       <c r="P32" s="51"/>
       <c r="Q32" s="51"/>
@@ -4407,7 +4679,7 @@
       <c r="S32" s="51"/>
       <c r="T32" s="51"/>
       <c r="U32" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V32" s="52"/>
       <c r="W32" s="52"/>
@@ -4424,10 +4696,10 @@
       <c r="H33" s="39"/>
       <c r="I33" s="39"/>
       <c r="J33" s="40"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="55"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="50"/>
       <c r="O33" s="51"/>
       <c r="P33" s="51"/>
       <c r="Q33" s="51"/>
@@ -4442,7 +4714,7 @@
     </row>
     <row r="34" spans="2:25" ht="295.5" customHeight="1">
       <c r="B34" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" s="36"/>
       <c r="D34" s="36"/>
@@ -4455,11 +4727,11 @@
       <c r="K34" s="47">
         <v>45709</v>
       </c>
-      <c r="L34" s="53"/>
+      <c r="L34" s="48"/>
       <c r="M34" s="47">
         <v>45710</v>
       </c>
-      <c r="N34" s="53"/>
+      <c r="N34" s="48"/>
       <c r="O34" s="51"/>
       <c r="P34" s="51"/>
       <c r="Q34" s="51"/>
@@ -4467,7 +4739,7 @@
       <c r="S34" s="51"/>
       <c r="T34" s="51"/>
       <c r="U34" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V34" s="52"/>
       <c r="W34" s="52"/>
@@ -4484,10 +4756,10 @@
       <c r="H35" s="39"/>
       <c r="I35" s="39"/>
       <c r="J35" s="40"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="55"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
       <c r="O35" s="51"/>
       <c r="P35" s="51"/>
       <c r="Q35" s="51"/>
@@ -4502,7 +4774,7 @@
     </row>
     <row r="36" spans="2:25" ht="249.75" customHeight="1">
       <c r="B36" s="35" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="36"/>
@@ -4515,11 +4787,11 @@
       <c r="K36" s="47">
         <v>45712</v>
       </c>
-      <c r="L36" s="53"/>
+      <c r="L36" s="48"/>
       <c r="M36" s="47">
         <v>45713</v>
       </c>
-      <c r="N36" s="53"/>
+      <c r="N36" s="48"/>
       <c r="O36" s="51"/>
       <c r="P36" s="51"/>
       <c r="Q36" s="51"/>
@@ -4527,7 +4799,7 @@
       <c r="S36" s="51"/>
       <c r="T36" s="51"/>
       <c r="U36" s="52" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="V36" s="52"/>
       <c r="W36" s="52"/>
@@ -4544,10 +4816,10 @@
       <c r="H37" s="39"/>
       <c r="I37" s="39"/>
       <c r="J37" s="40"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="54"/>
-      <c r="N37" s="55"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="50"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
       <c r="Q37" s="51"/>
@@ -4562,7 +4834,7 @@
     </row>
     <row r="38" spans="2:25" ht="182.25" customHeight="1">
       <c r="B38" s="35" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C38" s="36"/>
       <c r="D38" s="36"/>
@@ -4575,11 +4847,11 @@
       <c r="K38" s="47">
         <v>45713</v>
       </c>
-      <c r="L38" s="53"/>
+      <c r="L38" s="48"/>
       <c r="M38" s="47">
         <v>45714</v>
       </c>
-      <c r="N38" s="53"/>
+      <c r="N38" s="48"/>
       <c r="O38" s="51"/>
       <c r="P38" s="51"/>
       <c r="Q38" s="51"/>
@@ -4587,7 +4859,7 @@
       <c r="S38" s="51"/>
       <c r="T38" s="51"/>
       <c r="U38" s="52" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="V38" s="52"/>
       <c r="W38" s="52"/>
@@ -4604,10 +4876,10 @@
       <c r="H39" s="39"/>
       <c r="I39" s="39"/>
       <c r="J39" s="40"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="55"/>
-      <c r="M39" s="54"/>
-      <c r="N39" s="55"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="50"/>
       <c r="O39" s="51"/>
       <c r="P39" s="51"/>
       <c r="Q39" s="51"/>
@@ -4622,7 +4894,7 @@
     </row>
     <row r="40" spans="2:25" ht="219.75" customHeight="1">
       <c r="B40" s="35" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C40" s="36"/>
       <c r="D40" s="36"/>
@@ -4635,11 +4907,11 @@
       <c r="K40" s="47">
         <v>45714</v>
       </c>
-      <c r="L40" s="53"/>
+      <c r="L40" s="48"/>
       <c r="M40" s="47">
         <v>45715</v>
       </c>
-      <c r="N40" s="53"/>
+      <c r="N40" s="48"/>
       <c r="O40" s="41"/>
       <c r="P40" s="42"/>
       <c r="Q40" s="42"/>
@@ -4647,7 +4919,7 @@
       <c r="S40" s="42"/>
       <c r="T40" s="43"/>
       <c r="U40" s="35" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="V40" s="36"/>
       <c r="W40" s="36"/>
@@ -4664,10 +4936,10 @@
       <c r="H41" s="39"/>
       <c r="I41" s="39"/>
       <c r="J41" s="40"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="54"/>
-      <c r="N41" s="55"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="50"/>
       <c r="O41" s="44"/>
       <c r="P41" s="45"/>
       <c r="Q41" s="45"/>
@@ -4695,11 +4967,11 @@
       <c r="K42" s="47">
         <v>45715</v>
       </c>
-      <c r="L42" s="53"/>
+      <c r="L42" s="48"/>
       <c r="M42" s="47">
         <v>45716</v>
       </c>
-      <c r="N42" s="53"/>
+      <c r="N42" s="48"/>
       <c r="O42" s="41"/>
       <c r="P42" s="42"/>
       <c r="Q42" s="42"/>
@@ -4707,7 +4979,7 @@
       <c r="S42" s="42"/>
       <c r="T42" s="43"/>
       <c r="U42" s="35" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="V42" s="36"/>
       <c r="W42" s="36"/>
@@ -4724,10 +4996,10 @@
       <c r="H43" s="39"/>
       <c r="I43" s="39"/>
       <c r="J43" s="40"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="55"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="50"/>
       <c r="O43" s="44"/>
       <c r="P43" s="45"/>
       <c r="Q43" s="45"/>
@@ -4741,67 +5013,69 @@
       <c r="Y43" s="40"/>
     </row>
     <row r="44" spans="2:25" ht="153.75" customHeight="1">
-      <c r="B44" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="136"/>
-      <c r="D44" s="136"/>
-      <c r="E44" s="136"/>
-      <c r="F44" s="136"/>
-      <c r="G44" s="136"/>
-      <c r="H44" s="136"/>
-      <c r="I44" s="136"/>
-      <c r="J44" s="137"/>
+      <c r="B44" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="77"/>
       <c r="K44" s="47">
         <v>45716</v>
       </c>
-      <c r="L44" s="53"/>
-      <c r="M44" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="N44" s="53"/>
-      <c r="O44" s="141"/>
-      <c r="P44" s="142"/>
-      <c r="Q44" s="142"/>
-      <c r="R44" s="142"/>
-      <c r="S44" s="142"/>
-      <c r="T44" s="143"/>
-      <c r="U44" s="135" t="s">
-        <v>97</v>
-      </c>
-      <c r="V44" s="136"/>
-      <c r="W44" s="136"/>
-      <c r="X44" s="136"/>
-      <c r="Y44" s="137"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="47">
+        <v>45717</v>
+      </c>
+      <c r="N44" s="48"/>
+      <c r="O44" s="92"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="94"/>
+      <c r="U44" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="V44" s="76"/>
+      <c r="W44" s="76"/>
+      <c r="X44" s="76"/>
+      <c r="Y44" s="77"/>
     </row>
     <row r="45" spans="2:25" ht="195.75" customHeight="1">
-      <c r="B45" s="138"/>
-      <c r="C45" s="139"/>
-      <c r="D45" s="139"/>
-      <c r="E45" s="139"/>
-      <c r="F45" s="139"/>
-      <c r="G45" s="139"/>
-      <c r="H45" s="139"/>
-      <c r="I45" s="139"/>
-      <c r="J45" s="140"/>
-      <c r="K45" s="54"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="54"/>
-      <c r="N45" s="55"/>
-      <c r="O45" s="144"/>
-      <c r="P45" s="145"/>
-      <c r="Q45" s="145"/>
-      <c r="R45" s="145"/>
-      <c r="S45" s="145"/>
-      <c r="T45" s="146"/>
-      <c r="U45" s="138"/>
-      <c r="V45" s="139"/>
-      <c r="W45" s="139"/>
-      <c r="X45" s="139"/>
-      <c r="Y45" s="140"/>
-    </row>
-    <row r="46" spans="2:25">
-      <c r="B46" s="35"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="80"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="95"/>
+      <c r="P45" s="96"/>
+      <c r="Q45" s="96"/>
+      <c r="R45" s="96"/>
+      <c r="S45" s="96"/>
+      <c r="T45" s="97"/>
+      <c r="U45" s="78"/>
+      <c r="V45" s="79"/>
+      <c r="W45" s="79"/>
+      <c r="X45" s="79"/>
+      <c r="Y45" s="80"/>
+    </row>
+    <row r="46" spans="2:25" ht="237" customHeight="1">
+      <c r="B46" s="35" t="s">
+        <v>89</v>
+      </c>
       <c r="C46" s="36"/>
       <c r="D46" s="36"/>
       <c r="E46" s="36"/>
@@ -4810,9 +5084,13 @@
       <c r="H46" s="36"/>
       <c r="I46" s="36"/>
       <c r="J46" s="37"/>
-      <c r="K46" s="47"/>
+      <c r="K46" s="47">
+        <v>45719</v>
+      </c>
       <c r="L46" s="48"/>
-      <c r="M46" s="47"/>
+      <c r="M46" s="47">
+        <v>45720</v>
+      </c>
       <c r="N46" s="48"/>
       <c r="O46" s="41"/>
       <c r="P46" s="42"/>
@@ -4820,13 +5098,15 @@
       <c r="R46" s="42"/>
       <c r="S46" s="42"/>
       <c r="T46" s="43"/>
-      <c r="U46" s="35"/>
+      <c r="U46" s="35" t="s">
+        <v>90</v>
+      </c>
       <c r="V46" s="36"/>
       <c r="W46" s="36"/>
       <c r="X46" s="36"/>
       <c r="Y46" s="37"/>
     </row>
-    <row r="47" spans="2:25">
+    <row r="47" spans="2:25" ht="225" customHeight="1">
       <c r="B47" s="38"/>
       <c r="C47" s="39"/>
       <c r="D47" s="39"/>
@@ -4853,32 +5133,32 @@
       <c r="Y47" s="40"/>
     </row>
     <row r="48" spans="2:25" ht="15" customHeight="1">
-      <c r="B48" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="78"/>
-      <c r="L48" s="78"/>
-      <c r="M48" s="78"/>
-      <c r="N48" s="78"/>
-      <c r="O48" s="78"/>
-      <c r="P48" s="78"/>
-      <c r="Q48" s="78"/>
-      <c r="R48" s="78"/>
-      <c r="S48" s="78"/>
-      <c r="T48" s="78"/>
-      <c r="U48" s="78"/>
-      <c r="V48" s="78"/>
-      <c r="W48" s="78"/>
-      <c r="X48" s="78"/>
-      <c r="Y48" s="78"/>
+      <c r="B48" s="143" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="143"/>
+      <c r="D48" s="143"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="143"/>
+      <c r="G48" s="143"/>
+      <c r="H48" s="143"/>
+      <c r="I48" s="143"/>
+      <c r="J48" s="143"/>
+      <c r="K48" s="143"/>
+      <c r="L48" s="143"/>
+      <c r="M48" s="143"/>
+      <c r="N48" s="143"/>
+      <c r="O48" s="143"/>
+      <c r="P48" s="143"/>
+      <c r="Q48" s="143"/>
+      <c r="R48" s="143"/>
+      <c r="S48" s="143"/>
+      <c r="T48" s="143"/>
+      <c r="U48" s="143"/>
+      <c r="V48" s="143"/>
+      <c r="W48" s="143"/>
+      <c r="X48" s="143"/>
+      <c r="Y48" s="143"/>
     </row>
     <row r="49" spans="2:25" ht="15" customHeight="1">
       <c r="B49" s="10"/>
@@ -4907,16 +5187,16 @@
       <c r="Y49" s="10"/>
     </row>
     <row r="50" spans="2:25" ht="15.75" customHeight="1">
-      <c r="B50" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="77"/>
+      <c r="B50" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -4927,11 +5207,11 @@
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
-      <c r="T50" s="76"/>
-      <c r="U50" s="77"/>
-      <c r="V50" s="77"/>
-      <c r="W50" s="77"/>
-      <c r="X50" s="77"/>
+      <c r="T50" s="73"/>
+      <c r="U50" s="74"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="74"/>
+      <c r="X50" s="74"/>
       <c r="Y50" s="10"/>
     </row>
     <row r="51" spans="2:25" ht="23.25" customHeight="1">
@@ -4962,7 +5242,7 @@
     </row>
     <row r="52" spans="2:25" ht="18" customHeight="1">
       <c r="B52" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -5020,7 +5300,7 @@
     </row>
     <row r="54" spans="2:25">
       <c r="B54" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
@@ -5058,7 +5338,7 @@
     </row>
     <row r="56" spans="2:25">
       <c r="B56" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
@@ -5069,7 +5349,7 @@
       <c r="I56" s="17"/>
       <c r="J56" s="11"/>
       <c r="K56" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L56" s="18"/>
       <c r="M56" s="18"/>
@@ -5079,7 +5359,7 @@
       <c r="Q56" s="18"/>
       <c r="R56" s="13"/>
       <c r="S56" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T56" s="20"/>
       <c r="U56" s="20"/>
@@ -5089,68 +5369,76 @@
       <c r="Y56" s="20"/>
     </row>
     <row r="57" spans="2:25">
-      <c r="Q57" s="104"/>
-      <c r="R57" s="104"/>
-      <c r="S57" s="104"/>
-      <c r="T57" s="104"/>
-      <c r="U57" s="104"/>
+      <c r="Q57" s="112"/>
+      <c r="R57" s="112"/>
+      <c r="S57" s="112"/>
+      <c r="T57" s="112"/>
+      <c r="U57" s="112"/>
     </row>
     <row r="58" spans="2:25">
-      <c r="B58" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="83"/>
-      <c r="D58" s="83"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="83"/>
-      <c r="G58" s="83"/>
-      <c r="H58" s="83"/>
-      <c r="I58" s="83"/>
-      <c r="J58" s="83"/>
-      <c r="K58" s="83"/>
-      <c r="L58" s="83"/>
-      <c r="M58" s="83"/>
-      <c r="N58" s="83"/>
-      <c r="O58" s="83"/>
-      <c r="P58" s="83"/>
-      <c r="Q58" s="83"/>
-      <c r="R58" s="83"/>
-      <c r="S58" s="83"/>
-      <c r="T58" s="83"/>
-      <c r="U58" s="83"/>
-      <c r="V58" s="83"/>
-      <c r="W58" s="83"/>
-      <c r="X58" s="83"/>
-      <c r="Y58" s="83"/>
+      <c r="B58" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="85"/>
+      <c r="N58" s="85"/>
+      <c r="O58" s="85"/>
+      <c r="P58" s="85"/>
+      <c r="Q58" s="85"/>
+      <c r="R58" s="85"/>
+      <c r="S58" s="85"/>
+      <c r="T58" s="85"/>
+      <c r="U58" s="85"/>
+      <c r="V58" s="85"/>
+      <c r="W58" s="85"/>
+      <c r="X58" s="85"/>
+      <c r="Y58" s="85"/>
     </row>
     <row r="59" spans="2:25">
-      <c r="B59" s="83"/>
-      <c r="C59" s="83"/>
-      <c r="D59" s="83"/>
-      <c r="E59" s="83"/>
-      <c r="F59" s="83"/>
-      <c r="G59" s="83"/>
-      <c r="H59" s="83"/>
-      <c r="I59" s="83"/>
-      <c r="J59" s="83"/>
-      <c r="K59" s="83"/>
-      <c r="L59" s="83"/>
-      <c r="M59" s="83"/>
-      <c r="N59" s="83"/>
-      <c r="O59" s="83"/>
-      <c r="P59" s="83"/>
-      <c r="Q59" s="83"/>
-      <c r="R59" s="83"/>
-      <c r="S59" s="83"/>
-      <c r="T59" s="83"/>
-      <c r="U59" s="83"/>
-      <c r="V59" s="83"/>
-      <c r="W59" s="83"/>
-      <c r="X59" s="83"/>
-      <c r="Y59" s="83"/>
+      <c r="B59" s="85"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
+      <c r="L59" s="85"/>
+      <c r="M59" s="85"/>
+      <c r="N59" s="85"/>
+      <c r="O59" s="85"/>
+      <c r="P59" s="85"/>
+      <c r="Q59" s="85"/>
+      <c r="R59" s="85"/>
+      <c r="S59" s="85"/>
+      <c r="T59" s="85"/>
+      <c r="U59" s="85"/>
+      <c r="V59" s="85"/>
+      <c r="W59" s="85"/>
+      <c r="X59" s="85"/>
+      <c r="Y59" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="Q57:U57"/>
+    <mergeCell ref="O38:T39"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O28:T29"/>
     <mergeCell ref="K44:L45"/>
     <mergeCell ref="M44:N45"/>
     <mergeCell ref="O44:T45"/>
@@ -5171,10 +5459,10 @@
     <mergeCell ref="K52:Q52"/>
     <mergeCell ref="B19:I19"/>
     <mergeCell ref="B20:I20"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="Q57:U57"/>
-    <mergeCell ref="O38:T39"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B30:J31"/>
+    <mergeCell ref="U26:Y27"/>
+    <mergeCell ref="K26:L27"/>
     <mergeCell ref="U38:Y39"/>
     <mergeCell ref="T52:X52"/>
     <mergeCell ref="U32:Y33"/>
@@ -5195,22 +5483,6 @@
     <mergeCell ref="B5:Y5"/>
     <mergeCell ref="B7:Y7"/>
     <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O28:T29"/>
-    <mergeCell ref="U28:Y29"/>
-    <mergeCell ref="O30:T31"/>
-    <mergeCell ref="U30:Y31"/>
-    <mergeCell ref="M46:N47"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B30:J31"/>
-    <mergeCell ref="U26:Y27"/>
-    <mergeCell ref="K26:L27"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
     <mergeCell ref="B25:J25"/>
     <mergeCell ref="O25:T25"/>
     <mergeCell ref="T50:X50"/>
@@ -5227,6 +5499,13 @@
     <mergeCell ref="M42:N43"/>
     <mergeCell ref="B48:Y48"/>
     <mergeCell ref="O42:T43"/>
+    <mergeCell ref="U42:Y43"/>
+    <mergeCell ref="U28:Y29"/>
+    <mergeCell ref="O30:T31"/>
+    <mergeCell ref="U30:Y31"/>
+    <mergeCell ref="M46:N47"/>
+    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="K36:L37"/>
     <mergeCell ref="K23:Y23"/>
     <mergeCell ref="U25:Y25"/>
     <mergeCell ref="B26:J27"/>
@@ -5249,7 +5528,8 @@
     <mergeCell ref="B16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="B23:J23"/>
-    <mergeCell ref="U42:Y43"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="B56:I56"/>
     <mergeCell ref="K56:Q56"/>
     <mergeCell ref="S56:Y56"/>
@@ -5301,124 +5581,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="127"/>
-      <c r="P1" s="127"/>
-      <c r="Q1" s="127"/>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
+      <c r="V1" s="135"/>
+      <c r="W1" s="135"/>
+      <c r="X1" s="135"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1">
-      <c r="A2" s="127"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="127"/>
-      <c r="N2" s="127"/>
-      <c r="O2" s="127"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="127"/>
-      <c r="U2" s="111" t="s">
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="135"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="135"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="135"/>
+      <c r="U2" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1">
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="134"/>
-      <c r="X3" s="134"/>
+      <c r="U3" s="142"/>
+      <c r="V3" s="142"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="142"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="132"/>
-      <c r="M4" s="133"/>
-      <c r="N4" s="131" t="s">
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="141"/>
+      <c r="N4" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="132"/>
-      <c r="P4" s="132"/>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="132"/>
-      <c r="S4" s="132"/>
-      <c r="T4" s="132"/>
-      <c r="U4" s="132"/>
-      <c r="V4" s="132"/>
-      <c r="W4" s="132"/>
-      <c r="X4" s="133"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="140"/>
+      <c r="S4" s="140"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
+      <c r="W4" s="140"/>
+      <c r="X4" s="141"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="128"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="129"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="129"/>
-      <c r="M5" s="130"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="129"/>
-      <c r="P5" s="129"/>
-      <c r="Q5" s="129"/>
-      <c r="R5" s="129"/>
-      <c r="S5" s="129"/>
-      <c r="T5" s="129"/>
-      <c r="U5" s="129"/>
-      <c r="V5" s="129"/>
-      <c r="W5" s="129"/>
-      <c r="X5" s="130"/>
+      <c r="A5" s="136"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="137"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="138"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="137"/>
+      <c r="P5" s="137"/>
+      <c r="Q5" s="137"/>
+      <c r="R5" s="137"/>
+      <c r="S5" s="137"/>
+      <c r="T5" s="137"/>
+      <c r="U5" s="137"/>
+      <c r="V5" s="137"/>
+      <c r="W5" s="137"/>
+      <c r="X5" s="138"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A6" s="3"/>
@@ -5447,66 +5727,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="109"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109" t="s">
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="109"/>
-      <c r="P7" s="109" t="s">
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="117"/>
+      <c r="O7" s="117"/>
+      <c r="P7" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="109"/>
-      <c r="S7" s="109"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="109"/>
-      <c r="V7" s="109"/>
-      <c r="W7" s="109"/>
-      <c r="X7" s="109"/>
+      <c r="Q7" s="117"/>
+      <c r="R7" s="117"/>
+      <c r="S7" s="117"/>
+      <c r="T7" s="117"/>
+      <c r="U7" s="117"/>
+      <c r="V7" s="117"/>
+      <c r="W7" s="117"/>
+      <c r="X7" s="117"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1">
-      <c r="A8" s="103"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="116" t="s">
+      <c r="A8" s="111"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="117"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="116" t="s">
+      <c r="K8" s="125"/>
+      <c r="L8" s="125"/>
+      <c r="M8" s="125"/>
+      <c r="N8" s="125"/>
+      <c r="O8" s="126"/>
+      <c r="P8" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="117"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="117"/>
-      <c r="W8" s="117"/>
-      <c r="X8" s="118"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
+      <c r="X8" s="126"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A9" s="3"/>
@@ -5535,66 +5815,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="89"/>
-      <c r="S10" s="89"/>
-      <c r="T10" s="89"/>
-      <c r="U10" s="89"/>
-      <c r="V10" s="89"/>
-      <c r="W10" s="89"/>
-      <c r="X10" s="89"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="91"/>
+      <c r="X10" s="91"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66" t="s">
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66" t="s">
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66" t="s">
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="66"/>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="63"/>
+      <c r="X11" s="63"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="3"/>
@@ -5623,66 +5903,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109" t="s">
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="109"/>
-      <c r="L13" s="109"/>
-      <c r="M13" s="109"/>
-      <c r="N13" s="109"/>
-      <c r="O13" s="109"/>
-      <c r="P13" s="109" t="s">
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="117"/>
+      <c r="P13" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="109"/>
-      <c r="R13" s="109"/>
-      <c r="S13" s="109"/>
-      <c r="T13" s="109"/>
-      <c r="U13" s="109"/>
-      <c r="V13" s="109"/>
-      <c r="W13" s="109"/>
-      <c r="X13" s="109"/>
+      <c r="Q13" s="117"/>
+      <c r="R13" s="117"/>
+      <c r="S13" s="117"/>
+      <c r="T13" s="117"/>
+      <c r="U13" s="117"/>
+      <c r="V13" s="117"/>
+      <c r="W13" s="117"/>
+      <c r="X13" s="117"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1">
-      <c r="A14" s="103"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="116" t="s">
+      <c r="A14" s="111"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="117"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="118"/>
-      <c r="P14" s="116" t="s">
+      <c r="K14" s="125"/>
+      <c r="L14" s="125"/>
+      <c r="M14" s="125"/>
+      <c r="N14" s="125"/>
+      <c r="O14" s="126"/>
+      <c r="P14" s="124" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="117"/>
-      <c r="R14" s="117"/>
-      <c r="S14" s="117"/>
-      <c r="T14" s="117"/>
-      <c r="U14" s="117"/>
-      <c r="V14" s="117"/>
-      <c r="W14" s="117"/>
-      <c r="X14" s="118"/>
+      <c r="Q14" s="125"/>
+      <c r="R14" s="125"/>
+      <c r="S14" s="125"/>
+      <c r="T14" s="125"/>
+      <c r="U14" s="125"/>
+      <c r="V14" s="125"/>
+      <c r="W14" s="125"/>
+      <c r="X14" s="126"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1">
       <c r="A15" s="3"/>
@@ -5722,12 +6002,12 @@
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="119" t="s">
+      <c r="J16" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119"/>
-      <c r="M16" s="119"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
       <c r="N16" s="17" t="s">
         <v>13</v>
       </c>
@@ -5736,137 +6016,137 @@
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="120" t="s">
+      <c r="T16" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="120"/>
-      <c r="V16" s="120"/>
-      <c r="W16" s="120"/>
-      <c r="X16" s="120"/>
+      <c r="U16" s="128"/>
+      <c r="V16" s="128"/>
+      <c r="W16" s="128"/>
+      <c r="X16" s="128"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="111"/>
-      <c r="C17" s="111"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="121" t="s">
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="122"/>
-      <c r="L17" s="122"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="110" t="s">
+      <c r="K17" s="130"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="131"/>
+      <c r="N17" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="111"/>
-      <c r="P17" s="111"/>
-      <c r="Q17" s="111"/>
-      <c r="R17" s="111"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="110" t="s">
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="120"/>
+      <c r="T17" s="118" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="111"/>
-      <c r="V17" s="111"/>
-      <c r="W17" s="111"/>
-      <c r="X17" s="112"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="120"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A18" s="113"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="115"/>
-      <c r="J18" s="124"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="125"/>
-      <c r="M18" s="126"/>
-      <c r="N18" s="113"/>
-      <c r="O18" s="114"/>
-      <c r="P18" s="114"/>
-      <c r="Q18" s="114"/>
-      <c r="R18" s="114"/>
-      <c r="S18" s="115"/>
-      <c r="T18" s="113"/>
-      <c r="U18" s="114"/>
-      <c r="V18" s="114"/>
-      <c r="W18" s="114"/>
-      <c r="X18" s="115"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
+      <c r="H18" s="122"/>
+      <c r="I18" s="123"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="133"/>
+      <c r="L18" s="133"/>
+      <c r="M18" s="134"/>
+      <c r="N18" s="121"/>
+      <c r="O18" s="122"/>
+      <c r="P18" s="122"/>
+      <c r="Q18" s="122"/>
+      <c r="R18" s="122"/>
+      <c r="S18" s="123"/>
+      <c r="T18" s="121"/>
+      <c r="U18" s="122"/>
+      <c r="V18" s="122"/>
+      <c r="W18" s="122"/>
+      <c r="X18" s="123"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1"/>
     <row r="20" spans="1:24" ht="39" customHeight="1"/>
     <row r="21" spans="1:24">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="108"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="116"/>
+      <c r="G21" s="116"/>
+      <c r="H21" s="116"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="108" t="s">
+      <c r="J21" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="108"/>
-      <c r="L21" s="108"/>
-      <c r="M21" s="108"/>
-      <c r="N21" s="108"/>
-      <c r="O21" s="108"/>
-      <c r="P21" s="108"/>
+      <c r="K21" s="116"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="116"/>
+      <c r="N21" s="116"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="116"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="108" t="s">
+      <c r="R21" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="108"/>
-      <c r="T21" s="108"/>
-      <c r="U21" s="108"/>
-      <c r="V21" s="108"/>
-      <c r="W21" s="108"/>
-      <c r="X21" s="108"/>
+      <c r="S21" s="116"/>
+      <c r="T21" s="116"/>
+      <c r="U21" s="116"/>
+      <c r="V21" s="116"/>
+      <c r="W21" s="116"/>
+      <c r="X21" s="116"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P23" s="105" t="s">
+      <c r="P23" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="105"/>
-      <c r="R23" s="105"/>
-      <c r="S23" s="105"/>
-      <c r="T23" s="105"/>
-      <c r="U23" s="106" t="s">
+      <c r="Q23" s="113"/>
+      <c r="R23" s="113"/>
+      <c r="S23" s="113"/>
+      <c r="T23" s="113"/>
+      <c r="U23" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="106"/>
-      <c r="W23" s="106"/>
-      <c r="X23" s="106"/>
+      <c r="V23" s="114"/>
+      <c r="W23" s="114"/>
+      <c r="X23" s="114"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1">
-      <c r="P24" s="105" t="s">
+      <c r="P24" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="105"/>
-      <c r="R24" s="105"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="105"/>
-      <c r="U24" s="107" t="s">
+      <c r="Q24" s="113"/>
+      <c r="R24" s="113"/>
+      <c r="S24" s="113"/>
+      <c r="T24" s="113"/>
+      <c r="U24" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="107"/>
-      <c r="W24" s="107"/>
-      <c r="X24" s="107"/>
+      <c r="V24" s="115"/>
+      <c r="W24" s="115"/>
+      <c r="X24" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="40">

</xml_diff>